<commit_message>
constrained spline plus some best fit
</commit_message>
<xml_diff>
--- a/InterpolationExamples.xlsx
+++ b/InterpolationExamples.xlsx
@@ -4,18 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="15135" windowHeight="6345" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="15135" windowHeight="6345" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Example 1" sheetId="2" r:id="rId1"/>
     <sheet name="Example 2" sheetId="4" r:id="rId2"/>
+    <sheet name="Constrained Example" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="4">
   <si>
     <t>Length (Years)</t>
   </si>
@@ -280,6 +282,91 @@
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
             <a:t> as previous example, except this time surfact generating function takes an extra pair of axes - in case you want a more finely grained view of the surface. </a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Yellow cells are input</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>771525</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1181100" y="3190875"/>
+          <a:ext cx="5000625" cy="819149"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Uses a constrained cubic spline to prevent overshooting</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
         </a:p>
         <a:p>
           <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
@@ -995,8 +1082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B4:T44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1053,7 +1140,7 @@
         <v>0</v>
       </c>
       <c r="M5" s="9">
-        <f t="shared" ref="M5:P5" si="0">E5</f>
+        <f t="shared" ref="M5" si="0">E5</f>
         <v>0.25</v>
       </c>
       <c r="N5" s="9">
@@ -1093,7 +1180,7 @@
         <v>0.5</v>
       </c>
       <c r="D6" s="8">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
@@ -1110,28 +1197,28 @@
       </c>
       <c r="L6" s="3">
         <f t="array" ref="L6:T44">FS("Kalahari.splineSurfaceWithNewAxes", D5:H5,C6:C14,D6:H14,L5:T5,K6:K44)</f>
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="M6" s="3">
-        <v>14.53125</v>
+        <v>12</v>
       </c>
       <c r="N6" s="3">
-        <v>13.5</v>
+        <v>12</v>
       </c>
       <c r="O6" s="3">
-        <v>12.612903225806452</v>
+        <v>12.026209677419354</v>
       </c>
       <c r="P6" s="3">
         <v>12</v>
       </c>
       <c r="Q6" s="3">
-        <v>11.621387768817204</v>
+        <v>11.845934139784946</v>
       </c>
       <c r="R6" s="3">
-        <v>11.422715053763442</v>
+        <v>11.62231182795699</v>
       </c>
       <c r="S6" s="3">
-        <v>11.34601814516129</v>
+        <v>11.420866935483872</v>
       </c>
       <c r="T6" s="3">
         <v>11.333333333333334</v>
@@ -1159,31 +1246,31 @@
         <v>0.75</v>
       </c>
       <c r="L7" s="3">
-        <v>15.209228603894779</v>
+        <v>12.5211988454575</v>
       </c>
       <c r="M7" s="3">
-        <v>14.316089479731387</v>
+        <v>12.795819737671231</v>
       </c>
       <c r="N7" s="3">
-        <v>12.963563516322782</v>
+        <v>12.061491764065659</v>
       </c>
       <c r="O7" s="3">
-        <v>12.021574977178608</v>
+        <v>11.582688935751513</v>
       </c>
       <c r="P7" s="3">
-        <v>11.48929732926762</v>
+        <v>11.489624096233991</v>
       </c>
       <c r="Q7" s="3">
-        <v>11.228639152220234</v>
+        <v>11.412045883975368</v>
       </c>
       <c r="R7" s="3">
-        <v>11.145438687938254</v>
+        <v>11.307591985912465</v>
       </c>
       <c r="S7" s="3">
-        <v>11.156516593891325</v>
+        <v>11.215872351100725</v>
       </c>
       <c r="T7" s="3">
-        <v>11.178693527549093</v>
+        <v>11.176496928595601</v>
       </c>
     </row>
     <row r="8" spans="2:20">
@@ -1204,7 +1291,7 @@
         <v>1</v>
       </c>
       <c r="L8" s="3">
-        <v>15.724619932432432</v>
+        <v>13.806545608108108</v>
       </c>
       <c r="M8" s="3">
         <v>14</v>
@@ -1213,19 +1300,19 @@
         <v>12.25</v>
       </c>
       <c r="O8" s="3">
-        <v>11.301168629747259</v>
+        <v>11.115548533844905</v>
       </c>
       <c r="P8" s="3">
         <v>10.878306878306878</v>
       </c>
       <c r="Q8" s="3">
-        <v>10.762326276719547</v>
+        <v>10.866737580664621</v>
       </c>
       <c r="R8" s="3">
-        <v>10.819157748618435</v>
+        <v>10.911967796569613</v>
       </c>
       <c r="S8" s="3">
-        <v>10.935987065784824</v>
+        <v>10.970790833766515</v>
       </c>
       <c r="T8" s="3">
         <v>11</v>
@@ -1251,31 +1338,31 @@
         <v>1.25</v>
       </c>
       <c r="L9" s="3">
-        <v>16.377716777823402</v>
+        <v>15.438642597036834</v>
       </c>
       <c r="M9" s="3">
-        <v>13.958098097666593</v>
+        <v>14.28210305796738</v>
       </c>
       <c r="N9" s="3">
-        <v>12.391752730886086</v>
+        <v>12.591801048092762</v>
       </c>
       <c r="O9" s="3">
-        <v>11.628916408813827</v>
+        <v>11.581363929956453</v>
       </c>
       <c r="P9" s="3">
-        <v>11.15602658117513</v>
+        <v>11.154392746343277</v>
       </c>
       <c r="Q9" s="3">
-        <v>10.972266938934613</v>
+        <v>11.014562703503817</v>
       </c>
       <c r="R9" s="3">
-        <v>10.984656509220333</v>
+        <v>11.028843990997279</v>
       </c>
       <c r="S9" s="3">
-        <v>11.077173153201223</v>
+        <v>11.105030544210024</v>
       </c>
       <c r="T9" s="3">
-        <v>11.133794732046203</v>
+        <v>11.150916298528415</v>
       </c>
     </row>
     <row r="10" spans="2:20">
@@ -1304,25 +1391,25 @@
         <v>14.089613970588236</v>
       </c>
       <c r="N10" s="3">
-        <v>13.176562499999999</v>
+        <v>13.194078947368421</v>
       </c>
       <c r="O10" s="3">
-        <v>12.569509050172348</v>
+        <v>12.58248147678923</v>
       </c>
       <c r="P10" s="3">
         <v>11.74074074074074</v>
       </c>
       <c r="Q10" s="3">
-        <v>11.335952276221413</v>
+        <v>11.340149836040595</v>
       </c>
       <c r="R10" s="3">
-        <v>11.312567387891255</v>
+        <v>11.334032203795346</v>
       </c>
       <c r="S10" s="3">
-        <v>11.455942063717323</v>
+        <v>11.496218871183761</v>
       </c>
       <c r="T10" s="3">
-        <v>11.551432291666666</v>
+        <v>11.600540865384616</v>
       </c>
     </row>
     <row r="11" spans="2:20">
@@ -1334,7 +1421,9 @@
         <v>17.25</v>
       </c>
       <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
+      <c r="F11" s="8">
+        <v>18</v>
+      </c>
       <c r="G11" s="8"/>
       <c r="H11" s="8">
         <v>16</v>
@@ -1345,31 +1434,31 @@
         <v>1.75</v>
       </c>
       <c r="L11" s="3">
-        <v>17.455771050014313</v>
+        <v>18.153539254570848</v>
       </c>
       <c r="M11" s="3">
-        <v>14.221060868572831</v>
+        <v>14.12890451942984</v>
       </c>
       <c r="N11" s="3">
-        <v>14.133292747632868</v>
+        <v>14.098031017247505</v>
       </c>
       <c r="O11" s="3">
-        <v>13.437526038989335</v>
+        <v>13.51010924852579</v>
       </c>
       <c r="P11" s="3">
-        <v>11.91635825079377</v>
+        <v>11.922566823154813</v>
       </c>
       <c r="Q11" s="3">
-        <v>11.264121340795384</v>
+        <v>11.24785418289251</v>
       </c>
       <c r="R11" s="3">
-        <v>11.418741117278651</v>
+        <v>11.435686808593426</v>
       </c>
       <c r="S11" s="3">
-        <v>11.879041851161865</v>
+        <v>11.945096440886262</v>
       </c>
       <c r="T11" s="3">
-        <v>12.143847813363315</v>
+        <v>12.235114820399717</v>
       </c>
     </row>
     <row r="12" spans="2:20">
@@ -1385,14 +1474,16 @@
       <c r="G12" s="8">
         <v>19</v>
       </c>
-      <c r="H12" s="8"/>
+      <c r="H12" s="8">
+        <v>19</v>
+      </c>
       <c r="J12" s="4"/>
       <c r="K12" s="10">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="L12" s="3">
-        <v>17.740675675675675</v>
+        <v>18.883918918918919</v>
       </c>
       <c r="M12" s="3">
         <v>14.363970588235293</v>
@@ -1401,22 +1492,22 @@
         <v>15</v>
       </c>
       <c r="O12" s="3">
-        <v>14.159643347428608</v>
+        <v>14.265131310820427</v>
       </c>
       <c r="P12" s="3">
         <v>12</v>
       </c>
       <c r="Q12" s="3">
-        <v>11.172831503573144</v>
+        <v>11.140862323060144</v>
       </c>
       <c r="R12" s="3">
-        <v>11.570053543299585</v>
+        <v>11.588926231609019</v>
       </c>
       <c r="S12" s="3">
-        <v>12.39362033915401</v>
+        <v>12.486637601276458</v>
       </c>
       <c r="T12" s="3">
-        <v>12.845486111111111</v>
+        <v>12.976442307692308</v>
       </c>
     </row>
     <row r="13" spans="2:20">
@@ -1439,31 +1530,31 @@
         <v>2.25</v>
       </c>
       <c r="L13" s="3">
-        <v>17.883088285187853</v>
+        <v>19.256072058433425</v>
       </c>
       <c r="M13" s="3">
-        <v>14.565098838673588</v>
+        <v>14.614932394903581</v>
       </c>
       <c r="N13" s="3">
-        <v>15.616731320254962</v>
+        <v>15.597627811561848</v>
       </c>
       <c r="O13" s="3">
-        <v>14.802288349737585</v>
+        <v>14.878656953645773</v>
       </c>
       <c r="P13" s="3">
-        <v>12.44198643091001</v>
+        <v>12.410861877363207</v>
       </c>
       <c r="Q13" s="3">
-        <v>11.579404344784749</v>
+        <v>11.527343850457033</v>
       </c>
       <c r="R13" s="3">
-        <v>12.09317084101758</v>
+        <v>12.110279477877933</v>
       </c>
       <c r="S13" s="3">
-        <v>13.070677161425106</v>
+        <v>13.179114198878546</v>
       </c>
       <c r="T13" s="3">
-        <v>13.599314547823928</v>
+        <v>13.753293452711496</v>
       </c>
     </row>
     <row r="14" spans="2:20">
@@ -1486,31 +1577,31 @@
         <v>2.5</v>
       </c>
       <c r="L14" s="3">
-        <v>17.910953631575062</v>
+        <v>19.334292646785872</v>
       </c>
       <c r="M14" s="3">
-        <v>14.827078432110849</v>
+        <v>14.868783391781387</v>
       </c>
       <c r="N14" s="3">
-        <v>16.022302833380181</v>
+        <v>15.938607639683363</v>
       </c>
       <c r="O14" s="3">
-        <v>15.378797541500765</v>
+        <v>15.393020372776082</v>
       </c>
       <c r="P14" s="3">
-        <v>13.192224206737846</v>
+        <v>13.128831415261942</v>
       </c>
       <c r="Q14" s="3">
-        <v>12.400899963212781</v>
+        <v>12.336569044265367</v>
       </c>
       <c r="R14" s="3">
-        <v>12.902895388812381</v>
+        <v>12.914953815121301</v>
       </c>
       <c r="S14" s="3">
-        <v>13.836219422364815</v>
+        <v>13.939754352717308</v>
       </c>
       <c r="T14" s="3">
-        <v>14.338881002698255</v>
+        <v>14.486739281940963</v>
       </c>
     </row>
     <row r="15" spans="2:20">
@@ -1519,31 +1610,31 @@
         <v>2.75</v>
       </c>
       <c r="L15" s="3">
-        <v>17.852109054066631</v>
+        <v>19.182714884718358</v>
       </c>
       <c r="M15" s="3">
-        <v>15.141511456551509</v>
+        <v>15.154235339827322</v>
       </c>
       <c r="N15" s="3">
-        <v>16.305222929815312</v>
+        <v>16.15814549006846</v>
       </c>
       <c r="O15" s="3">
-        <v>15.889234698636916</v>
+        <v>15.853361990436019</v>
       </c>
       <c r="P15" s="3">
-        <v>14.075516545863426</v>
+        <v>14.011551912196374</v>
       </c>
       <c r="Q15" s="3">
-        <v>13.404313087277975</v>
+        <v>13.353083354984516</v>
       </c>
       <c r="R15" s="3">
-        <v>13.811063615892788</v>
+        <v>13.817826076731567</v>
       </c>
       <c r="S15" s="3">
-        <v>14.58000609402737</v>
+        <v>14.650525249942685</v>
       </c>
       <c r="T15" s="3">
-        <v>14.995378484001233</v>
+        <v>15.095926047123022</v>
       </c>
     </row>
     <row r="16" spans="2:20">
@@ -1552,28 +1643,28 @@
         <v>3</v>
       </c>
       <c r="L16" s="3">
-        <v>17.734391891891889</v>
+        <v>18.865472972972974</v>
       </c>
       <c r="M16" s="3">
         <v>15.5</v>
       </c>
       <c r="N16" s="3">
-        <v>16.553999999999998</v>
+        <v>16.391447368421051</v>
       </c>
       <c r="O16" s="3">
-        <v>16.333663597064803</v>
+        <v>16.304822228850242</v>
       </c>
       <c r="P16" s="3">
         <v>14.916666666666664</v>
       </c>
       <c r="Q16" s="3">
-        <v>14.356638445401044</v>
+        <v>14.361432233113842</v>
       </c>
       <c r="R16" s="3">
-        <v>14.629511951467595</v>
+        <v>14.633773096101194</v>
       </c>
       <c r="S16" s="3">
-        <v>15.191796148467015</v>
+        <v>15.193394077704614</v>
       </c>
       <c r="T16" s="3">
         <v>15.5</v>
@@ -1585,31 +1676,31 @@
         <v>3.25</v>
       </c>
       <c r="L17" s="3">
-        <v>17.585927856450223</v>
+        <v>18.447130052228452</v>
       </c>
       <c r="M17" s="3">
-        <v>15.894836258846704</v>
+        <v>15.924906995340551</v>
       </c>
       <c r="N17" s="3">
-        <v>16.839470526920337</v>
+        <v>16.739869041764035</v>
       </c>
       <c r="O17" s="3">
-        <v>16.71607004364084</v>
+        <v>16.778617338925322</v>
       </c>
       <c r="P17" s="3">
-        <v>15.582334238901971</v>
+        <v>15.728084183071379</v>
       </c>
       <c r="Q17" s="3">
-        <v>15.079626910860984</v>
+        <v>15.193649924075697</v>
       </c>
       <c r="R17" s="3">
-        <v>15.216051062239604</v>
+        <v>15.227716449678992</v>
       </c>
       <c r="S17" s="3">
-        <v>15.591394496900687</v>
+        <v>15.494441032088783</v>
       </c>
       <c r="T17" s="3">
-        <v>15.805445018707079</v>
+        <v>15.657980943512598</v>
       </c>
     </row>
     <row r="18" spans="11:20">
@@ -1618,31 +1709,31 @@
         <v>3.5</v>
       </c>
       <c r="L18" s="3">
-        <v>17.435996147821243</v>
+        <v>17.993965022910135</v>
       </c>
       <c r="M18" s="3">
-        <v>16.321072863025805</v>
+        <v>16.408257397220201</v>
       </c>
       <c r="N18" s="3">
-        <v>17.161783363748228</v>
+        <v>17.169365322396288</v>
       </c>
       <c r="O18" s="3">
-        <v>17.056127968971992</v>
+        <v>17.25026688629552</v>
       </c>
       <c r="P18" s="3">
-        <v>16.106604737821741</v>
+        <v>16.434773789402694</v>
       </c>
       <c r="Q18" s="3">
-        <v>15.614053936369826</v>
+        <v>15.871725852984371</v>
       </c>
       <c r="R18" s="3">
-        <v>15.612388564887592</v>
+        <v>15.664756686139203</v>
       </c>
       <c r="S18" s="3">
-        <v>15.818789807196119</v>
+        <v>15.656198344923871</v>
       </c>
       <c r="T18" s="3">
-        <v>15.950438847116498</v>
+        <v>15.688382885395054</v>
       </c>
     </row>
     <row r="19" spans="11:20">
@@ -1651,31 +1742,31 @@
         <v>3.75</v>
       </c>
       <c r="L19" s="3">
-        <v>17.314164338254614</v>
+        <v>17.572685725379994</v>
       </c>
       <c r="M19" s="3">
-        <v>16.774452550857443</v>
+        <v>16.919470139092688</v>
       </c>
       <c r="N19" s="3">
-        <v>17.503415456201999</v>
+        <v>17.612040783935655</v>
       </c>
       <c r="O19" s="3">
-        <v>17.377433334602866</v>
+        <v>17.681366265276985</v>
       </c>
       <c r="P19" s="3">
-        <v>16.565420090052861</v>
+        <v>17.051970019551177</v>
       </c>
       <c r="Q19" s="3">
-        <v>16.055451119497882</v>
+        <v>16.465138239877135</v>
       </c>
       <c r="R19" s="3">
-        <v>15.906206313584342</v>
+        <v>16.060039097212432</v>
       </c>
       <c r="S19" s="3">
-        <v>15.944016686383762</v>
+        <v>15.825311256974299</v>
       </c>
       <c r="T19" s="3">
-        <v>15.99521325196767</v>
+        <v>15.749593384579981</v>
       </c>
     </row>
     <row r="20" spans="11:20">
@@ -1687,25 +1778,25 @@
         <v>17.25</v>
       </c>
       <c r="M20" s="3">
-        <v>17.250718060661764</v>
+        <v>17.427964154411764</v>
       </c>
       <c r="N20" s="3">
-        <v>17.846843749999998</v>
+        <v>18</v>
       </c>
       <c r="O20" s="3">
-        <v>17.703582102078059</v>
+        <v>18.033510870185886</v>
       </c>
       <c r="P20" s="3">
-        <v>17.034722222222221</v>
+        <v>17.594907407407405</v>
       </c>
       <c r="Q20" s="3">
-        <v>16.499350057815462</v>
+        <v>17.043365304791269</v>
       </c>
       <c r="R20" s="3">
-        <v>16.185186162502635</v>
+        <v>16.528708974629275</v>
       </c>
       <c r="S20" s="3">
-        <v>16.037109741494046</v>
+        <v>16.148425009004498</v>
       </c>
       <c r="T20" s="3">
         <v>16</v>
@@ -1717,31 +1808,31 @@
         <v>4.25</v>
       </c>
       <c r="L21" s="3">
-        <v>17.265077439599327</v>
+        <v>17.076444511619222</v>
       </c>
       <c r="M21" s="3">
-        <v>17.740932551290015</v>
+        <v>17.905921945080724</v>
       </c>
       <c r="N21" s="3">
-        <v>18.173684911907415</v>
+        <v>18.279775818531125</v>
       </c>
       <c r="O21" s="3">
-        <v>18.047393213488871</v>
+        <v>18.277357903744729</v>
       </c>
       <c r="P21" s="3">
-        <v>17.566458731537651</v>
+        <v>18.073683624147556</v>
       </c>
       <c r="Q21" s="3">
-        <v>17.014334971711417</v>
+        <v>17.655214413155729</v>
       </c>
       <c r="R21" s="3">
-        <v>16.515324086928064</v>
+        <v>17.151548553805576</v>
       </c>
       <c r="S21" s="3">
-        <v>16.15394039192055</v>
+        <v>16.728068541538473</v>
       </c>
       <c r="T21" s="3">
-        <v>16.014698201421833</v>
+        <v>16.550156871795799</v>
       </c>
     </row>
     <row r="22" spans="11:20">
@@ -1750,31 +1841,31 @@
         <v>4.5</v>
       </c>
       <c r="L22" s="3">
-        <v>17.348997900763578</v>
+        <v>17.037871223035047</v>
       </c>
       <c r="M22" s="3">
-        <v>18.217440863717918</v>
+        <v>18.336580286801059</v>
       </c>
       <c r="N22" s="3">
-        <v>18.462114492876893</v>
+        <v>18.455614184766581</v>
       </c>
       <c r="O22" s="3">
-        <v>18.378577533113358</v>
+        <v>18.41981180230135</v>
       </c>
       <c r="P22" s="3">
-        <v>18.11659989753074</v>
+        <v>18.477848890090236</v>
       </c>
       <c r="Q22" s="3">
-        <v>17.561200572848755</v>
+        <v>18.266809511966233</v>
       </c>
       <c r="R22" s="3">
-        <v>16.875872546597432</v>
+        <v>17.871887844898112</v>
       </c>
       <c r="S22" s="3">
-        <v>16.293727306509389</v>
+        <v>17.490305594138583</v>
       </c>
       <c r="T22" s="3">
-        <v>16.047876340317234</v>
+        <v>17.319284464940363</v>
       </c>
     </row>
     <row r="23" spans="11:20">
@@ -1783,31 +1874,31 @@
         <v>4.75</v>
       </c>
       <c r="L23" s="3">
-        <v>17.483369361495988</v>
+        <v>17.10396092153195</v>
       </c>
       <c r="M23" s="3">
-        <v>18.647908259452304</v>
+        <v>18.705939523723803</v>
       </c>
       <c r="N23" s="3">
-        <v>18.689447764907925</v>
+        <v>18.546189318267874</v>
       </c>
       <c r="O23" s="3">
-        <v>18.656068905776259</v>
+        <v>18.476838810609948</v>
       </c>
       <c r="P23" s="3">
-        <v>18.617121670314017</v>
+        <v>18.791816562839646</v>
       </c>
       <c r="Q23" s="3">
-        <v>18.073794195709034</v>
+        <v>18.82360369361016</v>
       </c>
       <c r="R23" s="3">
-        <v>17.224398122360352</v>
+        <v>18.59869380174889</v>
       </c>
       <c r="S23" s="3">
-        <v>16.441525966469797</v>
+        <v>18.317083606126772</v>
       </c>
       <c r="T23" s="3">
-        <v>16.097770244239204</v>
+        <v>18.178769825614744</v>
       </c>
     </row>
     <row r="24" spans="11:20">
@@ -1816,31 +1907,31 @@
         <v>5</v>
       </c>
       <c r="L24" s="3">
-        <v>17.649799799799798</v>
+        <v>17.244394394394394</v>
       </c>
       <c r="M24" s="3">
         <v>19</v>
       </c>
       <c r="N24" s="3">
-        <v>18.832999999999998</v>
+        <v>18.570175438596493</v>
       </c>
       <c r="O24" s="3">
-        <v>18.838801176302308</v>
+        <v>18.464405173424701</v>
       </c>
       <c r="P24" s="3">
         <v>19</v>
       </c>
       <c r="Q24" s="3">
-        <v>18.485963174773818</v>
+        <v>19.271050050474923</v>
       </c>
       <c r="R24" s="3">
-        <v>17.518467395066441</v>
+        <v>19.24093337819993</v>
       </c>
       <c r="S24" s="3">
-        <v>16.582391853011028</v>
+        <v>19.090350016824974</v>
       </c>
       <c r="T24" s="3">
-        <v>16.162615740740744</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="11:20">
@@ -1849,31 +1940,31 @@
         <v>5.25</v>
       </c>
       <c r="L25" s="3">
-        <v>17.831990311140764</v>
+        <v>17.431965841936954</v>
       </c>
       <c r="M25" s="3">
-        <v>19.249411481379084</v>
+        <v>19.209185303654081</v>
       </c>
       <c r="N25" s="3">
-        <v>18.877424100639189</v>
+        <v>18.545063628059275</v>
       </c>
       <c r="O25" s="3">
-        <v>18.897026714318002</v>
+        <v>18.39813738133979</v>
       </c>
       <c r="P25" s="3">
-        <v>19.213880804085036</v>
+        <v>19.093088266346239</v>
       </c>
       <c r="Q25" s="3">
-        <v>18.747098194003332</v>
+        <v>19.567691373292643</v>
       </c>
       <c r="R25" s="3">
-        <v>17.725301187133141</v>
+        <v>19.726156473842067</v>
       </c>
       <c r="S25" s="3">
-        <v>16.704489706284022</v>
+        <v>19.714302010019821</v>
       </c>
       <c r="T25" s="3">
-        <v>16.240663674265523</v>
+        <v>19.677946423851225</v>
       </c>
     </row>
     <row r="26" spans="11:20">
@@ -1882,31 +1973,31 @@
         <v>5.5</v>
       </c>
       <c r="L26" s="3">
-        <v>18.022014460834736</v>
+        <v>17.651923116594585</v>
       </c>
       <c r="M26" s="3">
-        <v>19.403958637652583</v>
+        <v>19.341611998204044</v>
       </c>
       <c r="N26" s="3">
-        <v>18.836723491257864</v>
+        <v>18.483612419944386</v>
       </c>
       <c r="O26" s="3">
-        <v>18.846271988656795</v>
+        <v>18.292302908309427</v>
       </c>
       <c r="P26" s="3">
-        <v>19.274089869600711</v>
+        <v>19.086873255336272</v>
       </c>
       <c r="Q26" s="3">
-        <v>18.868763335272497</v>
+        <v>19.724429246174445</v>
       </c>
       <c r="R26" s="3">
-        <v>17.850737287249224</v>
+        <v>20.056244771261426</v>
       </c>
       <c r="S26" s="3">
-        <v>16.808421302206479</v>
+        <v>20.182135747356678</v>
       </c>
       <c r="T26" s="3">
-        <v>16.330224956819876</v>
+        <v>20.201918091219657</v>
       </c>
     </row>
     <row r="27" spans="11:20">
@@ -1915,31 +2006,31 @@
         <v>5.75</v>
       </c>
       <c r="L27" s="3">
-        <v>18.214038931660074</v>
+        <v>17.892627483832346</v>
       </c>
       <c r="M27" s="3">
-        <v>19.479487537394764</v>
+        <v>19.409819891041288</v>
       </c>
       <c r="N27" s="3">
-        <v>18.732239226774968</v>
+        <v>18.397397210285327</v>
       </c>
       <c r="O27" s="3">
-        <v>18.713381992953895</v>
+        <v>18.160829474127794</v>
       </c>
       <c r="P27" s="3">
-        <v>19.212622950962405</v>
+        <v>19.003422567598733</v>
       </c>
       <c r="Q27" s="3">
-        <v>18.878066029934896</v>
+        <v>19.765254951576186</v>
       </c>
       <c r="R27" s="3">
-        <v>17.910267725671272</v>
+        <v>20.251662898792972</v>
       </c>
       <c r="S27" s="3">
-        <v>16.897897675637825</v>
+        <v>20.509297134945605</v>
       </c>
       <c r="T27" s="3">
-        <v>16.429625517300831</v>
+        <v>20.584808385730589</v>
       </c>
     </row>
     <row r="28" spans="11:20">
@@ -1948,31 +2039,31 @@
         <v>6</v>
       </c>
       <c r="L28" s="3">
-        <v>18.402230406395137</v>
+        <v>18.142440209115286</v>
       </c>
       <c r="M28" s="3">
-        <v>19.491844249179898</v>
+        <v>19.426348789557192</v>
       </c>
       <c r="N28" s="3">
-        <v>18.585312362109448</v>
+        <v>18.297993395115597</v>
       </c>
       <c r="O28" s="3">
-        <v>18.525201720844493</v>
+        <v>18.0176447985891</v>
       </c>
       <c r="P28" s="3">
-        <v>19.06147580258552</v>
+        <v>18.864803803762275</v>
       </c>
       <c r="Q28" s="3">
-        <v>18.80211370934412</v>
+        <v>19.714159771953732</v>
       </c>
       <c r="R28" s="3">
-        <v>17.919384532655901</v>
+        <v>20.332875484771666</v>
       </c>
       <c r="S28" s="3">
-        <v>16.976629861437452</v>
+        <v>20.711232078896657</v>
       </c>
       <c r="T28" s="3">
-        <v>16.537191284605395</v>
+        <v>20.839510691009302</v>
       </c>
     </row>
     <row r="29" spans="11:20">
@@ -1981,31 +2072,31 @@
         <v>6.25</v>
       </c>
       <c r="L29" s="3">
-        <v>18.580755567818304</v>
+        <v>18.38972255790847</v>
       </c>
       <c r="M29" s="3">
-        <v>19.456874841582248</v>
+        <v>19.403738501143156</v>
       </c>
       <c r="N29" s="3">
-        <v>18.417283952180249</v>
+        <v>18.1969763704687</v>
       </c>
       <c r="O29" s="3">
-        <v>18.30857616596381</v>
+        <v>17.876676601487535</v>
       </c>
       <c r="P29" s="3">
-        <v>18.852644178885445</v>
+        <v>18.693084564455525</v>
       </c>
       <c r="Q29" s="3">
-        <v>18.668013804853754</v>
+        <v>19.595134989762929</v>
       </c>
       <c r="R29" s="3">
-        <v>17.893579738459682</v>
+        <v>20.320347157532446</v>
       </c>
       <c r="S29" s="3">
-        <v>17.048328894464774</v>
+        <v>20.803386485319894</v>
       </c>
       <c r="T29" s="3">
-        <v>16.651248187630575</v>
+        <v>20.978918390681088</v>
       </c>
     </row>
     <row r="30" spans="11:20">
@@ -2014,31 +2105,31 @@
         <v>6.5</v>
       </c>
       <c r="L30" s="3">
-        <v>18.743781098707924</v>
+        <v>18.622835795676945</v>
       </c>
       <c r="M30" s="3">
-        <v>19.390425383176087</v>
+        <v>19.354528833190567</v>
       </c>
       <c r="N30" s="3">
-        <v>18.249495051906308</v>
+        <v>18.105921532378133</v>
       </c>
       <c r="O30" s="3">
-        <v>18.090350321947025</v>
+        <v>17.751852602617301</v>
       </c>
       <c r="P30" s="3">
-        <v>18.618123834277569</v>
+        <v>18.510332450307136</v>
       </c>
       <c r="Q30" s="3">
-        <v>18.502873747817382</v>
+        <v>19.432171887459649</v>
       </c>
       <c r="R30" s="3">
-        <v>17.848345373339232</v>
+        <v>20.234542545410289</v>
       </c>
       <c r="S30" s="3">
-        <v>17.116705809579205</v>
+        <v>20.801206260325376</v>
       </c>
       <c r="T30" s="3">
-        <v>16.770122155273398</v>
+        <v>21.015924868371226</v>
       </c>
     </row>
     <row r="31" spans="11:20">
@@ -2047,31 +2138,31 @@
         <v>6.75</v>
       </c>
       <c r="L31" s="3">
-        <v>18.88547368184237</v>
+        <v>18.830141187885769</v>
       </c>
       <c r="M31" s="3">
-        <v>19.30834194253568</v>
+        <v>19.291259593090818</v>
       </c>
       <c r="N31" s="3">
-        <v>18.103286716206579</v>
+        <v>18.036404276877398</v>
       </c>
       <c r="O31" s="3">
-        <v>17.897369182429362</v>
+        <v>17.657100521772598</v>
       </c>
       <c r="P31" s="3">
-        <v>18.389910523177289</v>
+        <v>18.338615061945745</v>
       </c>
       <c r="Q31" s="3">
-        <v>18.333800969588598</v>
+        <v>19.249261747499737</v>
       </c>
       <c r="R31" s="3">
-        <v>17.799173467551132</v>
+        <v>20.095926276740137</v>
       </c>
       <c r="S31" s="3">
-        <v>17.185471641640138</v>
+        <v>20.720137310023151</v>
       </c>
       <c r="T31" s="3">
-        <v>16.892139116430865</v>
+        <v>20.963423507704995</v>
       </c>
     </row>
     <row r="32" spans="11:20">
@@ -2089,22 +2180,22 @@
         <v>18</v>
       </c>
       <c r="O32" s="3">
-        <v>17.756477741046016</v>
+        <v>17.606348078747629</v>
       </c>
       <c r="P32" s="3">
         <v>18.2</v>
       </c>
       <c r="Q32" s="3">
-        <v>18.187902901520989</v>
+        <v>19.070395852339072</v>
       </c>
       <c r="R32" s="3">
-        <v>17.761556051351995</v>
+        <v>19.924962979856954</v>
       </c>
       <c r="S32" s="3">
-        <v>17.258337425506998</v>
+        <v>20.575625540523284</v>
       </c>
       <c r="T32" s="3">
-        <v>17.015625</v>
+        <v>20.834307692307693</v>
       </c>
     </row>
     <row r="33" spans="11:20">
@@ -2113,31 +2204,31 @@
         <v>7.25</v>
       </c>
       <c r="L33" s="3">
-        <v>19.08318644679192</v>
+        <v>19.123735897295294</v>
       </c>
       <c r="M33" s="3">
-        <v>19.157747362210202</v>
+        <v>19.170447603579348</v>
       </c>
       <c r="N33" s="3">
-        <v>17.95580698638695</v>
+        <v>18.005150533686674</v>
       </c>
       <c r="O33" s="3">
-        <v>17.688099330363055</v>
+        <v>17.609648423740055</v>
       </c>
       <c r="P33" s="3">
-        <v>18.073473243817972</v>
+        <v>18.111609961538505</v>
       </c>
       <c r="Q33" s="3">
-        <v>18.086662331789665</v>
+        <v>18.915179021504628</v>
       </c>
       <c r="R33" s="3">
-        <v>17.74771360811112</v>
+        <v>19.739453974824006</v>
       </c>
       <c r="S33" s="3">
-        <v>17.338002438814058</v>
+        <v>20.382271816872983</v>
       </c>
       <c r="T33" s="3">
-        <v>17.138904189930209</v>
+        <v>20.641469543027902</v>
       </c>
     </row>
     <row r="34" spans="11:20">
@@ -2146,31 +2237,31 @@
         <v>7.5</v>
       </c>
       <c r="L34" s="3">
-        <v>19.137498259160203</v>
+        <v>19.204522144289747</v>
       </c>
       <c r="M34" s="3">
-        <v>19.103468199839696</v>
+        <v>19.124460334334152</v>
       </c>
       <c r="N34" s="3">
-        <v>17.966203871193521</v>
+        <v>18.047763453507113</v>
       </c>
       <c r="O34" s="3">
-        <v>17.686970638670033</v>
+        <v>17.66155642856145</v>
       </c>
       <c r="P34" s="3">
-        <v>18.007752132331046</v>
+        <v>18.070788029389778</v>
       </c>
       <c r="Q34" s="3">
-        <v>18.029063475855878</v>
+        <v>18.785670222807894</v>
       </c>
       <c r="R34" s="3">
-        <v>17.756780433648757</v>
+        <v>19.546547348617825</v>
       </c>
       <c r="S34" s="3">
-        <v>17.42311893029515</v>
+        <v>20.151296839868156</v>
       </c>
       <c r="T34" s="3">
-        <v>17.260294890380514</v>
+        <v>20.397796129607471</v>
       </c>
     </row>
     <row r="35" spans="11:20">
@@ -2179,31 +2270,31 @@
         <v>7.75</v>
       </c>
       <c r="L35" s="3">
-        <v>19.167060384879647</v>
+        <v>19.248494405312044</v>
       </c>
       <c r="M35" s="3">
-        <v>19.062019009864052</v>
+        <v>19.087524453274817</v>
       </c>
       <c r="N35" s="3">
-        <v>18.02151787842724</v>
+        <v>18.120612770938259</v>
       </c>
       <c r="O35" s="3">
-        <v>17.741406693187368</v>
+        <v>17.752752395426864</v>
       </c>
       <c r="P35" s="3">
-        <v>17.993343767895915</v>
+        <v>18.069932382822277</v>
       </c>
       <c r="Q35" s="3">
-        <v>18.00846590600235</v>
+        <v>18.679541961131466</v>
       </c>
       <c r="R35" s="3">
-        <v>17.784619276897839</v>
+        <v>19.350727879943236</v>
       </c>
       <c r="S35" s="3">
-        <v>17.511327391458966</v>
+        <v>19.893076269241842</v>
       </c>
       <c r="T35" s="3">
-        <v>17.378113760562325</v>
+        <v>20.116173259011539</v>
       </c>
     </row>
     <row r="36" spans="11:20">
@@ -2212,31 +2303,31 @@
         <v>8</v>
       </c>
       <c r="L36" s="3">
-        <v>19.175997771725061</v>
+        <v>19.261788344690878</v>
       </c>
       <c r="M36" s="3">
-        <v>19.031785701023562</v>
+        <v>19.058655633176468</v>
       </c>
       <c r="N36" s="3">
-        <v>18.112076232095635</v>
+        <v>18.216472497457033</v>
       </c>
       <c r="O36" s="3">
-        <v>17.839722521135489</v>
+        <v>17.873916626551335</v>
       </c>
       <c r="P36" s="3">
-        <v>18.020755252869318</v>
+        <v>18.101441201104496</v>
       </c>
       <c r="Q36" s="3">
-        <v>18.018229194511875</v>
+        <v>18.594466741357977</v>
       </c>
       <c r="R36" s="3">
-        <v>17.827092886791327</v>
+        <v>19.156480347505084</v>
       </c>
       <c r="S36" s="3">
-        <v>17.600268313814212</v>
+        <v>19.617985764727091</v>
       </c>
       <c r="T36" s="3">
-        <v>17.490677459687056</v>
+        <v>19.809486738205255</v>
       </c>
     </row>
     <row r="37" spans="11:20">
@@ -2245,31 +2336,31 @@
         <v>8.25</v>
       </c>
       <c r="L37" s="3">
-        <v>19.16843536747125</v>
+        <v>19.250539626754939</v>
       </c>
       <c r="M37" s="3">
-        <v>19.011154182058526</v>
+        <v>19.036869546814234</v>
       </c>
       <c r="N37" s="3">
-        <v>18.228206156206234</v>
+        <v>18.328116644540387</v>
       </c>
       <c r="O37" s="3">
-        <v>17.970233149734806</v>
+        <v>18.015729424149928</v>
       </c>
       <c r="P37" s="3">
-        <v>18.080493689607959</v>
+        <v>18.157712663504906</v>
       </c>
       <c r="Q37" s="3">
-        <v>18.051712913667199</v>
+        <v>18.528117068370022</v>
       </c>
       <c r="R37" s="3">
-        <v>17.880064012262174</v>
+        <v>18.96828953000821</v>
       </c>
       <c r="S37" s="3">
-        <v>17.687582188869591</v>
+        <v>19.336400986056962</v>
       </c>
       <c r="T37" s="3">
-        <v>17.59630264696613</v>
+        <v>19.490622374153769</v>
       </c>
     </row>
     <row r="38" spans="11:20">
@@ -2278,31 +2369,31 @@
         <v>8.5</v>
       </c>
       <c r="L38" s="3">
-        <v>19.14849811989302</v>
+        <v>19.220883915832928</v>
       </c>
       <c r="M38" s="3">
-        <v>18.998510361709222</v>
+        <v>19.021181866963236</v>
       </c>
       <c r="N38" s="3">
-        <v>18.360234874766551</v>
+        <v>18.448319223665234</v>
       </c>
       <c r="O38" s="3">
-        <v>18.121253606205734</v>
+        <v>18.168871090437658</v>
       </c>
       <c r="P38" s="3">
-        <v>18.163066180468544</v>
+        <v>18.231144949291977</v>
       </c>
       <c r="Q38" s="3">
-        <v>18.102276635751071</v>
+        <v>18.478165447050213</v>
       </c>
       <c r="R38" s="3">
-        <v>17.939395402243328</v>
+        <v>18.790640206157441</v>
       </c>
       <c r="S38" s="3">
-        <v>17.770909508133794</v>
+        <v>19.058697592964499</v>
       </c>
       <c r="T38" s="3">
-        <v>17.693305981610955</v>
+        <v>19.17246597382222</v>
       </c>
     </row>
     <row r="39" spans="11:20">
@@ -2311,31 +2402,31 @@
         <v>8.75</v>
       </c>
       <c r="L39" s="3">
-        <v>19.120310976765179</v>
+        <v>19.17895687625353</v>
       </c>
       <c r="M39" s="3">
-        <v>18.99224014871594</v>
+        <v>19.010608266398588</v>
       </c>
       <c r="N39" s="3">
-        <v>18.498489611784127</v>
+        <v>18.56985424630852</v>
       </c>
       <c r="O39" s="3">
-        <v>18.281098917768709</v>
+        <v>18.324021927629595</v>
       </c>
       <c r="P39" s="3">
-        <v>18.258979827807803</v>
+        <v>18.314136237734196</v>
       </c>
       <c r="Q39" s="3">
-        <v>18.163279933046272</v>
+        <v>18.442284382281166</v>
       </c>
       <c r="R39" s="3">
-        <v>18.000949805667748</v>
+        <v>18.628017154657623</v>
       </c>
       <c r="S39" s="3">
-        <v>17.847890763115533</v>
+        <v>18.795251245182762</v>
       </c>
       <c r="T39" s="3">
-        <v>17.780004122832949</v>
+        <v>18.867903344175769</v>
       </c>
     </row>
     <row r="40" spans="11:20">
@@ -2344,31 +2435,31 @@
         <v>9</v>
       </c>
       <c r="L40" s="3">
-        <v>19.087998885862529</v>
+        <v>19.130894172345439</v>
       </c>
       <c r="M40" s="3">
-        <v>18.990729451818972</v>
+        <v>19.004164417895424</v>
       </c>
       <c r="N40" s="3">
-        <v>18.633297591266473</v>
+        <v>18.685495723947174</v>
       </c>
       <c r="O40" s="3">
-        <v>18.438084111644134</v>
+        <v>18.471862237940773</v>
       </c>
       <c r="P40" s="3">
-        <v>18.358741733982441</v>
+        <v>18.39908470810003</v>
       </c>
       <c r="Q40" s="3">
-        <v>18.228082377835552</v>
+        <v>18.418146378945483</v>
       </c>
       <c r="R40" s="3">
-        <v>18.060589971468374</v>
+        <v>18.484905154213596</v>
       </c>
       <c r="S40" s="3">
-        <v>17.916166445323508</v>
+        <v>18.556437602444806</v>
       </c>
       <c r="T40" s="3">
-        <v>17.854713729843528</v>
+        <v>18.589820292179553</v>
       </c>
     </row>
     <row r="41" spans="11:20">
@@ -2377,31 +2468,31 @@
         <v>9.25</v>
       </c>
       <c r="L41" s="3">
-        <v>19.055686794959882</v>
+        <v>19.082831468437348</v>
       </c>
       <c r="M41" s="3">
-        <v>18.992364179758603</v>
+        <v>19.000865994228857</v>
       </c>
       <c r="N41" s="3">
-        <v>18.75498603722113</v>
+        <v>18.788017668058135</v>
       </c>
       <c r="O41" s="3">
-        <v>18.580524215052442</v>
+        <v>18.60307232358624</v>
       </c>
       <c r="P41" s="3">
-        <v>18.452859001349172</v>
+        <v>18.47838853965796</v>
       </c>
       <c r="Q41" s="3">
-        <v>18.290043542401662</v>
+        <v>18.403423941925777</v>
       </c>
       <c r="R41" s="3">
-        <v>18.114178648578172</v>
+        <v>18.36578898353018</v>
       </c>
       <c r="S41" s="3">
-        <v>17.97337704626641</v>
+        <v>18.352632324483665</v>
       </c>
       <c r="T41" s="3">
-        <v>17.915751461854107</v>
+        <v>18.351102624798717</v>
       </c>
     </row>
     <row r="42" spans="11:20">
@@ -2410,31 +2501,31 @@
         <v>9.5</v>
       </c>
       <c r="L42" s="3">
-        <v>19.027499651832041</v>
+        <v>19.040904428857949</v>
       </c>
       <c r="M42" s="3">
-        <v>18.99553024127513</v>
+        <v>18.999728668174022</v>
       </c>
       <c r="N42" s="3">
-        <v>18.853882173655613</v>
+        <v>18.870194090118332</v>
       </c>
       <c r="O42" s="3">
-        <v>18.69673425521405</v>
+        <v>18.708332486781039</v>
       </c>
       <c r="P42" s="3">
-        <v>18.53183873226472</v>
+        <v>18.544445911676465</v>
       </c>
       <c r="Q42" s="3">
-        <v>18.342522999027384</v>
+        <v>18.395789576104665</v>
       </c>
       <c r="R42" s="3">
-        <v>18.157578585930082</v>
+        <v>18.27515342131224</v>
       </c>
       <c r="S42" s="3">
-        <v>18.017163057452951</v>
+        <v>18.194211071032413</v>
       </c>
       <c r="T42" s="3">
-        <v>17.961433978076101</v>
+        <v>18.164636148998419</v>
       </c>
     </row>
     <row r="43" spans="11:20">
@@ -2443,31 +2534,31 @@
         <v>9.75</v>
       </c>
       <c r="L43" s="3">
-        <v>19.007562404253807</v>
+        <v>19.011248717935931</v>
       </c>
       <c r="M43" s="3">
-        <v>18.998613545108828</v>
+        <v>18.999768112506022</v>
       </c>
       <c r="N43" s="3">
-        <v>18.920313224577448</v>
+        <v>18.924799001604693</v>
       </c>
       <c r="O43" s="3">
-        <v>18.775029259349367</v>
+        <v>18.778323029740221</v>
       </c>
       <c r="P43" s="3">
-        <v>18.586188029085783</v>
+        <v>18.589655003424014</v>
       </c>
       <c r="Q43" s="3">
-        <v>18.378880319995449</v>
+        <v>18.392915786364743</v>
       </c>
       <c r="R43" s="3">
-        <v>18.186652532457067</v>
+        <v>18.217483246264582</v>
       </c>
       <c r="S43" s="3">
-        <v>18.045164970391827</v>
+        <v>18.091549501824083</v>
       </c>
       <c r="T43" s="3">
-        <v>17.99007793772093</v>
+        <v>18.043306671743792</v>
       </c>
     </row>
     <row r="44" spans="11:20">
@@ -2501,6 +2592,1529 @@
       </c>
       <c r="T44" s="3">
         <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B4:T44"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="6.140625" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:20">
+      <c r="B4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="J4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="1"/>
+      <c r="L4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+    </row>
+    <row r="5" spans="2:20" ht="15.75" thickBot="1">
+      <c r="C5" s="2"/>
+      <c r="D5" s="9">
+        <v>0</v>
+      </c>
+      <c r="E5" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="F5" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="G5" s="9">
+        <v>1</v>
+      </c>
+      <c r="H5" s="9">
+        <v>2</v>
+      </c>
+      <c r="K5" s="2"/>
+      <c r="L5" s="9">
+        <f>D5</f>
+        <v>0</v>
+      </c>
+      <c r="M5" s="9">
+        <f t="shared" ref="M5" si="0">E5</f>
+        <v>0.25</v>
+      </c>
+      <c r="N5" s="9">
+        <f>M5+0.25</f>
+        <v>0.5</v>
+      </c>
+      <c r="O5" s="9">
+        <f t="shared" ref="O5:T5" si="1">N5+0.25</f>
+        <v>0.75</v>
+      </c>
+      <c r="P5" s="9">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="Q5" s="9">
+        <f t="shared" si="1"/>
+        <v>1.25</v>
+      </c>
+      <c r="R5" s="9">
+        <f t="shared" si="1"/>
+        <v>1.5</v>
+      </c>
+      <c r="S5" s="9">
+        <f t="shared" si="1"/>
+        <v>1.75</v>
+      </c>
+      <c r="T5" s="9">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:20">
+      <c r="B6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="D6" s="8">
+        <v>12</v>
+      </c>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8">
+        <v>12</v>
+      </c>
+      <c r="H6" s="8"/>
+      <c r="J6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K6" s="10">
+        <f>C6</f>
+        <v>0.5</v>
+      </c>
+      <c r="L6" s="3">
+        <f t="array" ref="L6:T44">FS("Kalahari.constrainedSplineSurface", D5:H5,C6:C14,D6:H14,L5:T5,K6:K44)</f>
+        <v>12</v>
+      </c>
+      <c r="M6" s="3">
+        <v>14.75390625</v>
+      </c>
+      <c r="N6" s="3">
+        <v>18.875</v>
+      </c>
+      <c r="O6" s="3">
+        <v>20.671875</v>
+      </c>
+      <c r="P6" s="3">
+        <v>20.125</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>18.07421875</v>
+      </c>
+      <c r="R6" s="3">
+        <v>17</v>
+      </c>
+      <c r="S6" s="3">
+        <v>17</v>
+      </c>
+      <c r="T6" s="3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="2:20">
+      <c r="B7" s="4"/>
+      <c r="C7" s="10">
+        <v>1</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8">
+        <v>15</v>
+      </c>
+      <c r="F7" s="8">
+        <v>12.25</v>
+      </c>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8">
+        <v>11</v>
+      </c>
+      <c r="J7" s="4"/>
+      <c r="K7" s="10">
+        <f>K6+0.25</f>
+        <v>0.75</v>
+      </c>
+      <c r="L7" s="3">
+        <v>13.8359375</v>
+      </c>
+      <c r="M7" s="3">
+        <v>16.583333333333332</v>
+      </c>
+      <c r="N7" s="3">
+        <v>19.6171875</v>
+      </c>
+      <c r="O7" s="3">
+        <v>20.1640625</v>
+      </c>
+      <c r="P7" s="3">
+        <v>19.083333333333332</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>17.716145833333332</v>
+      </c>
+      <c r="R7" s="3">
+        <v>17</v>
+      </c>
+      <c r="S7" s="3">
+        <v>17</v>
+      </c>
+      <c r="T7" s="3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="2:20">
+      <c r="B8" s="4"/>
+      <c r="C8" s="10">
+        <v>1.5</v>
+      </c>
+      <c r="D8" s="8">
+        <v>17</v>
+      </c>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="10">
+        <f t="shared" ref="K8:K43" si="2">K7+0.25</f>
+        <v>1</v>
+      </c>
+      <c r="L8" s="3">
+        <v>15.4375</v>
+      </c>
+      <c r="M8" s="3">
+        <v>17.712890625</v>
+      </c>
+      <c r="N8" s="3">
+        <v>19.5</v>
+      </c>
+      <c r="O8" s="3">
+        <v>19.373046875</v>
+      </c>
+      <c r="P8" s="3">
+        <v>18.5625</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>17.537109375</v>
+      </c>
+      <c r="R8" s="3">
+        <v>17</v>
+      </c>
+      <c r="S8" s="3">
+        <v>17</v>
+      </c>
+      <c r="T8" s="3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="2:20">
+      <c r="B9" s="4"/>
+      <c r="C9" s="10">
+        <v>2</v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8">
+        <v>15</v>
+      </c>
+      <c r="G9" s="8">
+        <v>12</v>
+      </c>
+      <c r="H9" s="8"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="10">
+        <f t="shared" si="2"/>
+        <v>1.25</v>
+      </c>
+      <c r="L9" s="3">
+        <v>16.5703125</v>
+      </c>
+      <c r="M9" s="3">
+        <v>18</v>
+      </c>
+      <c r="N9" s="3">
+        <v>19</v>
+      </c>
+      <c r="O9" s="3">
+        <v>18.8984375</v>
+      </c>
+      <c r="P9" s="3">
+        <v>18.25</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>17.4296875</v>
+      </c>
+      <c r="R9" s="3">
+        <v>17</v>
+      </c>
+      <c r="S9" s="3">
+        <v>17</v>
+      </c>
+      <c r="T9" s="3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="2:20">
+      <c r="B10" s="4"/>
+      <c r="C10" s="10">
+        <v>3</v>
+      </c>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8">
+        <v>16</v>
+      </c>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8">
+        <v>15.5</v>
+      </c>
+      <c r="J10" s="4"/>
+      <c r="K10" s="10">
+        <f t="shared" si="2"/>
+        <v>1.5</v>
+      </c>
+      <c r="L10" s="3">
+        <v>17</v>
+      </c>
+      <c r="M10" s="3">
+        <v>17.833333333333332</v>
+      </c>
+      <c r="N10" s="3">
+        <v>18.666666666666668</v>
+      </c>
+      <c r="O10" s="3">
+        <v>18.58203125</v>
+      </c>
+      <c r="P10" s="3">
+        <v>18.041666666666668</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>17.358072916666668</v>
+      </c>
+      <c r="R10" s="3">
+        <v>17</v>
+      </c>
+      <c r="S10" s="3">
+        <v>17</v>
+      </c>
+      <c r="T10" s="3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="2:20">
+      <c r="B11" s="4"/>
+      <c r="C11" s="10">
+        <v>4</v>
+      </c>
+      <c r="D11" s="8">
+        <v>17</v>
+      </c>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8">
+        <v>18</v>
+      </c>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8">
+        <v>16</v>
+      </c>
+      <c r="J11" s="4"/>
+      <c r="K11" s="10">
+        <f t="shared" si="2"/>
+        <v>1.75</v>
+      </c>
+      <c r="L11" s="3">
+        <v>17</v>
+      </c>
+      <c r="M11" s="3">
+        <v>17.714285714285715</v>
+      </c>
+      <c r="N11" s="3">
+        <v>18.428571428571427</v>
+      </c>
+      <c r="O11" s="3">
+        <v>18.356026785714285</v>
+      </c>
+      <c r="P11" s="3">
+        <v>17.892857142857142</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>17.306919642857142</v>
+      </c>
+      <c r="R11" s="3">
+        <v>17</v>
+      </c>
+      <c r="S11" s="3">
+        <v>17</v>
+      </c>
+      <c r="T11" s="3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="2:20">
+      <c r="B12" s="4"/>
+      <c r="C12" s="10">
+        <v>5</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8">
+        <v>19</v>
+      </c>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8">
+        <v>19</v>
+      </c>
+      <c r="H12" s="8">
+        <v>19</v>
+      </c>
+      <c r="J12" s="4"/>
+      <c r="K12" s="10">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="L12" s="3">
+        <v>17</v>
+      </c>
+      <c r="M12" s="3">
+        <v>17.625</v>
+      </c>
+      <c r="N12" s="3">
+        <v>18.25</v>
+      </c>
+      <c r="O12" s="3">
+        <v>18.1865234375</v>
+      </c>
+      <c r="P12" s="3">
+        <v>17.78125</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>17.2685546875</v>
+      </c>
+      <c r="R12" s="3">
+        <v>17</v>
+      </c>
+      <c r="S12" s="3">
+        <v>17</v>
+      </c>
+      <c r="T12" s="3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="2:20">
+      <c r="B13" s="4"/>
+      <c r="C13" s="10">
+        <v>7</v>
+      </c>
+      <c r="D13" s="8">
+        <v>19</v>
+      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8">
+        <v>18</v>
+      </c>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="10">
+        <f t="shared" si="2"/>
+        <v>2.25</v>
+      </c>
+      <c r="L13" s="3">
+        <v>17</v>
+      </c>
+      <c r="M13" s="3">
+        <v>17.555555555555557</v>
+      </c>
+      <c r="N13" s="3">
+        <v>18.111111111111111</v>
+      </c>
+      <c r="O13" s="3">
+        <v>18.0546875</v>
+      </c>
+      <c r="P13" s="3">
+        <v>17.694444444444443</v>
+      </c>
+      <c r="Q13" s="3">
+        <v>17.238715277777779</v>
+      </c>
+      <c r="R13" s="3">
+        <v>17</v>
+      </c>
+      <c r="S13" s="3">
+        <v>17</v>
+      </c>
+      <c r="T13" s="3">
+        <v>17.038258744855959</v>
+      </c>
+    </row>
+    <row r="14" spans="2:20">
+      <c r="B14" s="4"/>
+      <c r="C14" s="10">
+        <v>10</v>
+      </c>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8">
+        <v>19</v>
+      </c>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8">
+        <v>18</v>
+      </c>
+      <c r="J14" s="4"/>
+      <c r="K14" s="10">
+        <f t="shared" si="2"/>
+        <v>2.5</v>
+      </c>
+      <c r="L14" s="3">
+        <v>17</v>
+      </c>
+      <c r="M14" s="3">
+        <v>17.5</v>
+      </c>
+      <c r="N14" s="3">
+        <v>18</v>
+      </c>
+      <c r="O14" s="3">
+        <v>17.94921875</v>
+      </c>
+      <c r="P14" s="3">
+        <v>17.625</v>
+      </c>
+      <c r="Q14" s="3">
+        <v>17.21484375</v>
+      </c>
+      <c r="R14" s="3">
+        <v>17</v>
+      </c>
+      <c r="S14" s="3">
+        <v>17.034432870370363</v>
+      </c>
+      <c r="T14" s="3">
+        <v>17.141666666666662</v>
+      </c>
+    </row>
+    <row r="15" spans="2:20">
+      <c r="K15" s="10">
+        <f t="shared" si="2"/>
+        <v>2.75</v>
+      </c>
+      <c r="L15" s="3">
+        <v>17</v>
+      </c>
+      <c r="M15" s="3">
+        <v>17.454545454545453</v>
+      </c>
+      <c r="N15" s="3">
+        <v>17.90909090909091</v>
+      </c>
+      <c r="O15" s="3">
+        <v>17.862926136363637</v>
+      </c>
+      <c r="P15" s="3">
+        <v>17.568181818181817</v>
+      </c>
+      <c r="Q15" s="3">
+        <v>17.1953125</v>
+      </c>
+      <c r="R15" s="3">
+        <v>17.031302609427602</v>
+      </c>
+      <c r="S15" s="3">
+        <v>17.128787878787875</v>
+      </c>
+      <c r="T15" s="3">
+        <v>17.296874999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="2:20">
+      <c r="K16" s="10">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="L16" s="3">
+        <v>17</v>
+      </c>
+      <c r="M16" s="3">
+        <v>17.416666666666668</v>
+      </c>
+      <c r="N16" s="3">
+        <v>17.833333333333332</v>
+      </c>
+      <c r="O16" s="3">
+        <v>17.791015625</v>
+      </c>
+      <c r="P16" s="3">
+        <v>17.520833333333332</v>
+      </c>
+      <c r="Q16" s="3">
+        <v>17.207730516975303</v>
+      </c>
+      <c r="R16" s="3">
+        <v>17.118055555555554</v>
+      </c>
+      <c r="S16" s="3">
+        <v>17.272135416666661</v>
+      </c>
+      <c r="T16" s="3">
+        <v>17.493827160493822</v>
+      </c>
+    </row>
+    <row r="17" spans="11:20">
+      <c r="K17" s="10">
+        <f t="shared" si="2"/>
+        <v>3.25</v>
+      </c>
+      <c r="L17" s="3">
+        <v>17</v>
+      </c>
+      <c r="M17" s="3">
+        <v>17.384615384615383</v>
+      </c>
+      <c r="N17" s="3">
+        <v>17.76923076923077</v>
+      </c>
+      <c r="O17" s="3">
+        <v>17.73016826923077</v>
+      </c>
+      <c r="P17" s="3">
+        <v>17.507256054131048</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>17.274238782051277</v>
+      </c>
+      <c r="R17" s="3">
+        <v>17.25120192307692</v>
+      </c>
+      <c r="S17" s="3">
+        <v>17.455840455840452</v>
+      </c>
+      <c r="T17" s="3">
+        <v>17.72449252136752</v>
+      </c>
+    </row>
+    <row r="18" spans="11:20">
+      <c r="K18" s="10">
+        <f t="shared" si="2"/>
+        <v>3.5</v>
+      </c>
+      <c r="L18" s="3">
+        <v>17</v>
+      </c>
+      <c r="M18" s="3">
+        <v>17.357142857142858</v>
+      </c>
+      <c r="N18" s="3">
+        <v>17.714285714285715</v>
+      </c>
+      <c r="O18" s="3">
+        <v>17.702608300264547</v>
+      </c>
+      <c r="P18" s="3">
+        <v>17.547619047619044</v>
+      </c>
+      <c r="Q18" s="3">
+        <v>17.386718749999996</v>
+      </c>
+      <c r="R18" s="3">
+        <v>17.423280423280421</v>
+      </c>
+      <c r="S18" s="3">
+        <v>17.672743055555554</v>
+      </c>
+      <c r="T18" s="3">
+        <v>17.982142857142843</v>
+      </c>
+    </row>
+    <row r="19" spans="11:20">
+      <c r="K19" s="10">
+        <f t="shared" si="2"/>
+        <v>3.75</v>
+      </c>
+      <c r="L19" s="3">
+        <v>17</v>
+      </c>
+      <c r="M19" s="3">
+        <v>17.333333333333332</v>
+      </c>
+      <c r="N19" s="3">
+        <v>17.689621913580243</v>
+      </c>
+      <c r="O19" s="3">
+        <v>17.727256944444441</v>
+      </c>
+      <c r="P19" s="3">
+        <v>17.634374999999995</v>
+      </c>
+      <c r="Q19" s="3">
+        <v>17.538290895061724</v>
+      </c>
+      <c r="R19" s="3">
+        <v>17.627893518518519</v>
+      </c>
+      <c r="S19" s="3">
+        <v>17.916666666666654</v>
+      </c>
+      <c r="T19" s="3">
+        <v>18.260918209876536</v>
+      </c>
+    </row>
+    <row r="20" spans="11:20">
+      <c r="K20" s="10">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="L20" s="3">
+        <v>17</v>
+      </c>
+      <c r="M20" s="3">
+        <v>17.334020543981477</v>
+      </c>
+      <c r="N20" s="3">
+        <v>17.713541666666664</v>
+      </c>
+      <c r="O20" s="3">
+        <v>17.797363281249996</v>
+      </c>
+      <c r="P20" s="3">
+        <v>17.760995370370367</v>
+      </c>
+      <c r="Q20" s="3">
+        <v>17.722927517361111</v>
+      </c>
+      <c r="R20" s="3">
+        <v>17.859374999999989</v>
+      </c>
+      <c r="S20" s="3">
+        <v>18.182110821759252</v>
+      </c>
+      <c r="T20" s="3">
+        <v>18.555555555555546</v>
+      </c>
+    </row>
+    <row r="21" spans="11:20">
+      <c r="K21" s="10">
+        <f t="shared" si="2"/>
+        <v>4.25</v>
+      </c>
+      <c r="L21" s="3">
+        <v>17.020254629629626</v>
+      </c>
+      <c r="M21" s="3">
+        <v>17.377450980392155</v>
+      </c>
+      <c r="N21" s="3">
+        <v>17.780330882352938</v>
+      </c>
+      <c r="O21" s="3">
+        <v>17.906947848583876</v>
+      </c>
+      <c r="P21" s="3">
+        <v>17.921670751633986</v>
+      </c>
+      <c r="Q21" s="3">
+        <v>17.935202205882344</v>
+      </c>
+      <c r="R21" s="3">
+        <v>18.112574891067531</v>
+      </c>
+      <c r="S21" s="3">
+        <v>18.464052287581691</v>
+      </c>
+      <c r="T21" s="3">
+        <v>18.861213235294116</v>
+      </c>
+    </row>
+    <row r="22" spans="11:20">
+      <c r="K22" s="10">
+        <f t="shared" si="2"/>
+        <v>4.5</v>
+      </c>
+      <c r="L22" s="3">
+        <v>17.078703703703702</v>
+      </c>
+      <c r="M22" s="3">
+        <v>17.459201388888886</v>
+      </c>
+      <c r="N22" s="3">
+        <v>17.884773662551439</v>
+      </c>
+      <c r="O22" s="3">
+        <v>18.05058834876543</v>
+      </c>
+      <c r="P22" s="3">
+        <v>18.1111111111111</v>
+      </c>
+      <c r="Q22" s="3">
+        <v>18.170122813786001</v>
+      </c>
+      <c r="R22" s="3">
+        <v>18.382716049382708</v>
+      </c>
+      <c r="S22" s="3">
+        <v>18.7578125</v>
+      </c>
+      <c r="T22" s="3">
+        <v>19.173353909465014</v>
+      </c>
+    </row>
+    <row r="23" spans="11:20">
+      <c r="K23" s="10">
+        <f t="shared" si="2"/>
+        <v>4.75</v>
+      </c>
+      <c r="L23" s="3">
+        <v>17.171874999999996</v>
+      </c>
+      <c r="M23" s="3">
+        <v>17.575048732943468</v>
+      </c>
+      <c r="N23" s="3">
+        <v>18.022021198830409</v>
+      </c>
+      <c r="O23" s="3">
+        <v>18.22327302631578</v>
+      </c>
+      <c r="P23" s="3">
+        <v>18.324409113060423</v>
+      </c>
+      <c r="Q23" s="3">
+        <v>18.423017178362567</v>
+      </c>
+      <c r="R23" s="3">
+        <v>18.665296052631579</v>
+      </c>
+      <c r="S23" s="3">
+        <v>19.058966861598435</v>
+      </c>
+      <c r="T23" s="3">
+        <v>19.487664473684198</v>
+      </c>
+    </row>
+    <row r="24" spans="11:20">
+      <c r="K24" s="10">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="L24" s="3">
+        <v>17.296296296296294</v>
+      </c>
+      <c r="M24" s="3">
+        <v>17.720920138888889</v>
+      </c>
+      <c r="N24" s="3">
+        <v>18.187499999999993</v>
+      </c>
+      <c r="O24" s="3">
+        <v>18.420298032407402</v>
+      </c>
+      <c r="P24" s="3">
+        <v>18.556944444444436</v>
+      </c>
+      <c r="Q24" s="3">
+        <v>18.689453125</v>
+      </c>
+      <c r="R24" s="3">
+        <v>18.956018518518512</v>
+      </c>
+      <c r="S24" s="3">
+        <v>19.363281249999989</v>
+      </c>
+      <c r="T24" s="3">
+        <v>19.8</v>
+      </c>
+    </row>
+    <row r="25" spans="11:20">
+      <c r="K25" s="10">
+        <f t="shared" si="2"/>
+        <v>5.25</v>
+      </c>
+      <c r="L25" s="3">
+        <v>17.44849537037037</v>
+      </c>
+      <c r="M25" s="3">
+        <v>17.892857142857135</v>
+      </c>
+      <c r="N25" s="3">
+        <v>18.376846340388003</v>
+      </c>
+      <c r="O25" s="3">
+        <v>18.637194113756607</v>
+      </c>
+      <c r="P25" s="3">
+        <v>18.804315476190474</v>
+      </c>
+      <c r="Q25" s="3">
+        <v>18.96518132716049</v>
+      </c>
+      <c r="R25" s="3">
+        <v>19.250744047619037</v>
+      </c>
+      <c r="S25" s="3">
+        <v>19.666666666666668</v>
+      </c>
+      <c r="T25" s="3">
+        <v>19.761904761904763</v>
+      </c>
+    </row>
+    <row r="26" spans="11:20">
+      <c r="K26" s="10">
+        <f t="shared" si="2"/>
+        <v>5.5</v>
+      </c>
+      <c r="L26" s="3">
+        <v>17.624999999999993</v>
+      </c>
+      <c r="M26" s="3">
+        <v>18.086989688552183</v>
+      </c>
+      <c r="N26" s="3">
+        <v>18.585858585858578</v>
+      </c>
+      <c r="O26" s="3">
+        <v>18.869673295454547</v>
+      </c>
+      <c r="P26" s="3">
+        <v>19.062289562289557</v>
+      </c>
+      <c r="Q26" s="3">
+        <v>19.246093749999989</v>
+      </c>
+      <c r="R26" s="3">
+        <v>19.545454545454547</v>
+      </c>
+      <c r="S26" s="3">
+        <v>19.636363636363637</v>
+      </c>
+      <c r="T26" s="3">
+        <v>19.727272727272727</v>
+      </c>
+    </row>
+    <row r="27" spans="11:20">
+      <c r="K27" s="10">
+        <f t="shared" si="2"/>
+        <v>5.75</v>
+      </c>
+      <c r="L27" s="3">
+        <v>17.822337962962958</v>
+      </c>
+      <c r="M27" s="3">
+        <v>18.299516908212553</v>
+      </c>
+      <c r="N27" s="3">
+        <v>18.810461956521738</v>
+      </c>
+      <c r="O27" s="3">
+        <v>19.113589472624795</v>
+      </c>
+      <c r="P27" s="3">
+        <v>19.326766304347817</v>
+      </c>
+      <c r="Q27" s="3">
+        <v>19.528192934782609</v>
+      </c>
+      <c r="R27" s="3">
+        <v>19.521739130434781</v>
+      </c>
+      <c r="S27" s="3">
+        <v>19.608695652173914</v>
+      </c>
+      <c r="T27" s="3">
+        <v>19.695652173913043</v>
+      </c>
+    </row>
+    <row r="28" spans="11:20">
+      <c r="K28" s="10">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="L28" s="3">
+        <v>18.037037037037031</v>
+      </c>
+      <c r="M28" s="3">
+        <v>18.526692708333332</v>
+      </c>
+      <c r="N28" s="3">
+        <v>19.046682098765427</v>
+      </c>
+      <c r="O28" s="3">
+        <v>19.364908854166657</v>
+      </c>
+      <c r="P28" s="3">
+        <v>19.59375</v>
+      </c>
+      <c r="Q28" s="3">
+        <v>19.506184895833332</v>
+      </c>
+      <c r="R28" s="3">
+        <v>19.5</v>
+      </c>
+      <c r="S28" s="3">
+        <v>19.583333333333332</v>
+      </c>
+      <c r="T28" s="3">
+        <v>19.666666666666668</v>
+      </c>
+    </row>
+    <row r="29" spans="11:20">
+      <c r="K29" s="10">
+        <f t="shared" si="2"/>
+        <v>6.25</v>
+      </c>
+      <c r="L29" s="3">
+        <v>18.265625</v>
+      </c>
+      <c r="M29" s="3">
+        <v>18.764814814814812</v>
+      </c>
+      <c r="N29" s="3">
+        <v>19.290624999999991</v>
+      </c>
+      <c r="O29" s="3">
+        <v>19.619687500000001</v>
+      </c>
+      <c r="P29" s="3">
+        <v>19.57</v>
+      </c>
+      <c r="Q29" s="3">
+        <v>19.485937499999999</v>
+      </c>
+      <c r="R29" s="3">
+        <v>19.48</v>
+      </c>
+      <c r="S29" s="3">
+        <v>19.559999999999999</v>
+      </c>
+      <c r="T29" s="3">
+        <v>19.64</v>
+      </c>
+    </row>
+    <row r="30" spans="11:20">
+      <c r="K30" s="10">
+        <f t="shared" si="2"/>
+        <v>6.5</v>
+      </c>
+      <c r="L30" s="3">
+        <v>18.504629629629626</v>
+      </c>
+      <c r="M30" s="3">
+        <v>19.010216346153836</v>
+      </c>
+      <c r="N30" s="3">
+        <v>19.53846153846154</v>
+      </c>
+      <c r="O30" s="3">
+        <v>19.595853365384617</v>
+      </c>
+      <c r="P30" s="3">
+        <v>19.548076923076923</v>
+      </c>
+      <c r="Q30" s="3">
+        <v>19.467247596153847</v>
+      </c>
+      <c r="R30" s="3">
+        <v>19.46153846153846</v>
+      </c>
+      <c r="S30" s="3">
+        <v>19.53846153846154</v>
+      </c>
+      <c r="T30" s="3">
+        <v>19.615384615384617</v>
+      </c>
+    </row>
+    <row r="31" spans="11:20">
+      <c r="K31" s="10">
+        <f t="shared" si="2"/>
+        <v>6.75</v>
+      </c>
+      <c r="L31" s="3">
+        <v>18.750578703703695</v>
+      </c>
+      <c r="M31" s="3">
+        <v>19.25925925925926</v>
+      </c>
+      <c r="N31" s="3">
+        <v>19.518518518518519</v>
+      </c>
+      <c r="O31" s="3">
+        <v>19.573784722222221</v>
+      </c>
+      <c r="P31" s="3">
+        <v>19.527777777777779</v>
+      </c>
+      <c r="Q31" s="3">
+        <v>19.44994212962963</v>
+      </c>
+      <c r="R31" s="3">
+        <v>19.444444444444443</v>
+      </c>
+      <c r="S31" s="3">
+        <v>19.518518518518519</v>
+      </c>
+      <c r="T31" s="3">
+        <v>19.592592592592592</v>
+      </c>
+    </row>
+    <row r="32" spans="11:20">
+      <c r="K32" s="10">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="L32" s="3">
+        <v>19</v>
+      </c>
+      <c r="M32" s="3">
+        <v>19.25</v>
+      </c>
+      <c r="N32" s="3">
+        <v>19.5</v>
+      </c>
+      <c r="O32" s="3">
+        <v>19.553292410714285</v>
+      </c>
+      <c r="P32" s="3">
+        <v>19.508928571428573</v>
+      </c>
+      <c r="Q32" s="3">
+        <v>19.433872767857142</v>
+      </c>
+      <c r="R32" s="3">
+        <v>19.428571428571427</v>
+      </c>
+      <c r="S32" s="3">
+        <v>19.5</v>
+      </c>
+      <c r="T32" s="3">
+        <v>19.571428571428573</v>
+      </c>
+    </row>
+    <row r="33" spans="11:20">
+      <c r="K33" s="10">
+        <f t="shared" si="2"/>
+        <v>7.25</v>
+      </c>
+      <c r="L33" s="3">
+        <v>19</v>
+      </c>
+      <c r="M33" s="3">
+        <v>19.241379310344829</v>
+      </c>
+      <c r="N33" s="3">
+        <v>19.482758620689655</v>
+      </c>
+      <c r="O33" s="3">
+        <v>19.534213362068964</v>
+      </c>
+      <c r="P33" s="3">
+        <v>19.491379310344829</v>
+      </c>
+      <c r="Q33" s="3">
+        <v>19.418911637931036</v>
+      </c>
+      <c r="R33" s="3">
+        <v>19.413793103448278</v>
+      </c>
+      <c r="S33" s="3">
+        <v>19.482758620689655</v>
+      </c>
+      <c r="T33" s="3">
+        <v>19.551724137931036</v>
+      </c>
+    </row>
+    <row r="34" spans="11:20">
+      <c r="K34" s="10">
+        <f t="shared" si="2"/>
+        <v>7.5</v>
+      </c>
+      <c r="L34" s="3">
+        <v>19</v>
+      </c>
+      <c r="M34" s="3">
+        <v>19.233333333333334</v>
+      </c>
+      <c r="N34" s="3">
+        <v>19.466666666666665</v>
+      </c>
+      <c r="O34" s="3">
+        <v>19.516406249999999</v>
+      </c>
+      <c r="P34" s="3">
+        <v>19.475000000000001</v>
+      </c>
+      <c r="Q34" s="3">
+        <v>19.404947916666668</v>
+      </c>
+      <c r="R34" s="3">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="S34" s="3">
+        <v>19.466666666666665</v>
+      </c>
+      <c r="T34" s="3">
+        <v>19.533333333333335</v>
+      </c>
+    </row>
+    <row r="35" spans="11:20">
+      <c r="K35" s="10">
+        <f t="shared" si="2"/>
+        <v>7.75</v>
+      </c>
+      <c r="L35" s="3">
+        <v>19</v>
+      </c>
+      <c r="M35" s="3">
+        <v>19.225806451612904</v>
+      </c>
+      <c r="N35" s="3">
+        <v>19.451612903225808</v>
+      </c>
+      <c r="O35" s="3">
+        <v>19.499747983870968</v>
+      </c>
+      <c r="P35" s="3">
+        <v>19.45967741935484</v>
+      </c>
+      <c r="Q35" s="3">
+        <v>19.39188508064516</v>
+      </c>
+      <c r="R35" s="3">
+        <v>19.387096774193548</v>
+      </c>
+      <c r="S35" s="3">
+        <v>19.451612903225808</v>
+      </c>
+      <c r="T35" s="3">
+        <v>19.516129032258064</v>
+      </c>
+    </row>
+    <row r="36" spans="11:20">
+      <c r="K36" s="10">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="L36" s="3">
+        <v>19</v>
+      </c>
+      <c r="M36" s="3">
+        <v>19.21875</v>
+      </c>
+      <c r="N36" s="3">
+        <v>19.4375</v>
+      </c>
+      <c r="O36" s="3">
+        <v>19.484130859375</v>
+      </c>
+      <c r="P36" s="3">
+        <v>19.4453125</v>
+      </c>
+      <c r="Q36" s="3">
+        <v>19.379638671875</v>
+      </c>
+      <c r="R36" s="3">
+        <v>19.375</v>
+      </c>
+      <c r="S36" s="3">
+        <v>19.4375</v>
+      </c>
+      <c r="T36" s="3">
+        <v>19.5</v>
+      </c>
+    </row>
+    <row r="37" spans="11:20">
+      <c r="K37" s="10">
+        <f t="shared" si="2"/>
+        <v>8.25</v>
+      </c>
+      <c r="L37" s="3">
+        <v>19</v>
+      </c>
+      <c r="M37" s="3">
+        <v>19.212121212121211</v>
+      </c>
+      <c r="N37" s="3">
+        <v>19.424242424242426</v>
+      </c>
+      <c r="O37" s="3">
+        <v>19.469460227272727</v>
+      </c>
+      <c r="P37" s="3">
+        <v>19.431818181818183</v>
+      </c>
+      <c r="Q37" s="3">
+        <v>19.368134469696969</v>
+      </c>
+      <c r="R37" s="3">
+        <v>19.363636363636363</v>
+      </c>
+      <c r="S37" s="3">
+        <v>19.424242424242426</v>
+      </c>
+      <c r="T37" s="3">
+        <v>19.484848484848484</v>
+      </c>
+    </row>
+    <row r="38" spans="11:20">
+      <c r="K38" s="10">
+        <f t="shared" si="2"/>
+        <v>8.5</v>
+      </c>
+      <c r="L38" s="3">
+        <v>19</v>
+      </c>
+      <c r="M38" s="3">
+        <v>19.205882352941178</v>
+      </c>
+      <c r="N38" s="3">
+        <v>19.411764705882351</v>
+      </c>
+      <c r="O38" s="3">
+        <v>19.455652573529413</v>
+      </c>
+      <c r="P38" s="3">
+        <v>19.419117647058822</v>
+      </c>
+      <c r="Q38" s="3">
+        <v>19.357306985294116</v>
+      </c>
+      <c r="R38" s="3">
+        <v>19.352941176470587</v>
+      </c>
+      <c r="S38" s="3">
+        <v>19.411764705882351</v>
+      </c>
+      <c r="T38" s="3">
+        <v>19.470588235294116</v>
+      </c>
+    </row>
+    <row r="39" spans="11:20">
+      <c r="K39" s="10">
+        <f t="shared" si="2"/>
+        <v>8.75</v>
+      </c>
+      <c r="L39" s="3">
+        <v>19</v>
+      </c>
+      <c r="M39" s="3">
+        <v>19.2</v>
+      </c>
+      <c r="N39" s="3">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="O39" s="3">
+        <v>19.442633928571428</v>
+      </c>
+      <c r="P39" s="3">
+        <v>19.407142857142858</v>
+      </c>
+      <c r="Q39" s="3">
+        <v>19.347098214285715</v>
+      </c>
+      <c r="R39" s="3">
+        <v>19.342857142857142</v>
+      </c>
+      <c r="S39" s="3">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="T39" s="3">
+        <v>19.457142857142856</v>
+      </c>
+    </row>
+    <row r="40" spans="11:20">
+      <c r="K40" s="10">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="L40" s="3">
+        <v>19</v>
+      </c>
+      <c r="M40" s="3">
+        <v>19.194444444444443</v>
+      </c>
+      <c r="N40" s="3">
+        <v>19.388888888888889</v>
+      </c>
+      <c r="O40" s="3">
+        <v>19.430338541666668</v>
+      </c>
+      <c r="P40" s="3">
+        <v>19.395833333333332</v>
+      </c>
+      <c r="Q40" s="3">
+        <v>19.337456597222221</v>
+      </c>
+      <c r="R40" s="3">
+        <v>19.333333333333332</v>
+      </c>
+      <c r="S40" s="3">
+        <v>19.388888888888889</v>
+      </c>
+      <c r="T40" s="3">
+        <v>19.444444444444443</v>
+      </c>
+    </row>
+    <row r="41" spans="11:20">
+      <c r="K41" s="10">
+        <f t="shared" si="2"/>
+        <v>9.25</v>
+      </c>
+      <c r="L41" s="3">
+        <v>19</v>
+      </c>
+      <c r="M41" s="3">
+        <v>19.189189189189189</v>
+      </c>
+      <c r="N41" s="3">
+        <v>19.378378378378379</v>
+      </c>
+      <c r="O41" s="3">
+        <v>19.41870777027027</v>
+      </c>
+      <c r="P41" s="3">
+        <v>19.385135135135137</v>
+      </c>
+      <c r="Q41" s="3">
+        <v>19.328336148648649</v>
+      </c>
+      <c r="R41" s="3">
+        <v>19.324324324324323</v>
+      </c>
+      <c r="S41" s="3">
+        <v>19.378378378378379</v>
+      </c>
+      <c r="T41" s="3">
+        <v>19.432432432432432</v>
+      </c>
+    </row>
+    <row r="42" spans="11:20">
+      <c r="K42" s="10">
+        <f t="shared" si="2"/>
+        <v>9.5</v>
+      </c>
+      <c r="L42" s="3">
+        <v>19</v>
+      </c>
+      <c r="M42" s="3">
+        <v>19.184210526315791</v>
+      </c>
+      <c r="N42" s="3">
+        <v>19.368421052631579</v>
+      </c>
+      <c r="O42" s="3">
+        <v>19.407689144736842</v>
+      </c>
+      <c r="P42" s="3">
+        <v>19.375</v>
+      </c>
+      <c r="Q42" s="3">
+        <v>19.319695723684209</v>
+      </c>
+      <c r="R42" s="3">
+        <v>19.315789473684209</v>
+      </c>
+      <c r="S42" s="3">
+        <v>19.368421052631579</v>
+      </c>
+      <c r="T42" s="3">
+        <v>19.421052631578949</v>
+      </c>
+    </row>
+    <row r="43" spans="11:20">
+      <c r="K43" s="10">
+        <f t="shared" si="2"/>
+        <v>9.75</v>
+      </c>
+      <c r="L43" s="3">
+        <v>19</v>
+      </c>
+      <c r="M43" s="3">
+        <v>19.179487179487179</v>
+      </c>
+      <c r="N43" s="3">
+        <v>19.358974358974358</v>
+      </c>
+      <c r="O43" s="3">
+        <v>19.397235576923077</v>
+      </c>
+      <c r="P43" s="3">
+        <v>19.365384615384617</v>
+      </c>
+      <c r="Q43" s="3">
+        <v>19.311498397435898</v>
+      </c>
+      <c r="R43" s="3">
+        <v>19.307692307692307</v>
+      </c>
+      <c r="S43" s="3">
+        <v>19.358974358974358</v>
+      </c>
+      <c r="T43" s="3">
+        <v>19.410256410256409</v>
+      </c>
+    </row>
+    <row r="44" spans="11:20">
+      <c r="K44" s="10">
+        <f>K43+0.25</f>
+        <v>10</v>
+      </c>
+      <c r="L44" s="3">
+        <v>19</v>
+      </c>
+      <c r="M44" s="3">
+        <v>19.175000000000001</v>
+      </c>
+      <c r="N44" s="3">
+        <v>19.350000000000001</v>
+      </c>
+      <c r="O44" s="3">
+        <v>19.387304687499999</v>
+      </c>
+      <c r="P44" s="3">
+        <v>19.356249999999999</v>
+      </c>
+      <c r="Q44" s="3">
+        <v>19.3037109375</v>
+      </c>
+      <c r="R44" s="3">
+        <v>19.3</v>
+      </c>
+      <c r="S44" s="3">
+        <v>19.350000000000001</v>
+      </c>
+      <c r="T44" s="3">
+        <v>19.399999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add sheet with best fit
</commit_message>
<xml_diff>
--- a/InterpolationExamples.xlsx
+++ b/InterpolationExamples.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="15135" windowHeight="6345"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="15135" windowHeight="6345" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Constrained Example" sheetId="6" r:id="rId1"/>
+    <sheet name="Best fit" sheetId="7" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t>Length (Years)</t>
   </si>
@@ -28,10 +29,25 @@
     <t>Rate</t>
   </si>
   <si>
-    <t>Zero Start Points</t>
+    <t>Length</t>
   </si>
   <si>
-    <t>Length</t>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Spot Rates</t>
+  </si>
+  <si>
+    <t>Forward Rates</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>End</t>
+  </si>
+  <si>
+    <t>Alpha</t>
   </si>
 </sst>
 </file>
@@ -69,7 +85,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -183,11 +199,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -204,13 +238,28 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -601,8 +650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B4:Q44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView showGridLines="0" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -617,10 +666,10 @@
   <sheetData>
     <row r="4" spans="2:17">
       <c r="B4" s="4"/>
-      <c r="C4" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="17"/>
+      <c r="C4" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="24"/>
       <c r="E4" s="5"/>
       <c r="G4" s="4" t="s">
         <v>2</v>
@@ -636,7 +685,7 @@
     </row>
     <row r="5" spans="2:17" ht="15.75" thickBot="1">
       <c r="C5" s="14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>3</v>
@@ -683,7 +732,7 @@
         <v>0.25</v>
       </c>
       <c r="D6" s="11">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E6" s="9"/>
       <c r="G6" s="4" t="s">
@@ -695,31 +744,31 @@
       </c>
       <c r="I6" s="3">
         <f t="array" ref="I6:Q44">FS("Kalahari.constrainedSplineSurface", C6:C14,D6:D14,I5:Q5,H6:H44)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J6" s="3">
-        <v>12.95811764705882</v>
+        <v>12.408000000000001</v>
       </c>
       <c r="K6" s="3">
-        <v>13.856941176470592</v>
+        <v>11.888000000000005</v>
       </c>
       <c r="L6" s="3">
-        <v>14.617411764705878</v>
+        <v>11.536000000000001</v>
       </c>
       <c r="M6" s="3">
-        <v>15.160470588235299</v>
+        <v>11.447999999999993</v>
       </c>
       <c r="N6" s="3">
-        <v>15.407058823529397</v>
+        <v>11.720000000000013</v>
       </c>
       <c r="O6" s="3">
-        <v>15.662309368191714</v>
+        <v>13.555555555555543</v>
       </c>
       <c r="P6" s="3">
-        <v>16.084967320261441</v>
+        <v>16.666666666666671</v>
       </c>
       <c r="Q6" s="3">
-        <v>16.340958605664511</v>
+        <v>19.277777777777771</v>
       </c>
     </row>
     <row r="7" spans="2:17">
@@ -735,31 +784,31 @@
         <v>0.5</v>
       </c>
       <c r="I7" s="3">
-        <v>12.47905882352941</v>
+        <v>12.704000000000001</v>
       </c>
       <c r="J7" s="3">
-        <v>13.407529411764706</v>
+        <v>12.148000000000003</v>
       </c>
       <c r="K7" s="3">
-        <v>14.237176470588235</v>
+        <v>11.712000000000003</v>
       </c>
       <c r="L7" s="3">
-        <v>14.888941176470588</v>
+        <v>11.491999999999997</v>
       </c>
       <c r="M7" s="3">
-        <v>15.283764705882348</v>
+        <v>11.584000000000003</v>
       </c>
       <c r="N7" s="3">
-        <v>15.534684095860555</v>
+        <v>12.637777777777778</v>
       </c>
       <c r="O7" s="3">
-        <v>15.873638344226578</v>
+        <v>15.111111111111107</v>
       </c>
       <c r="P7" s="3">
-        <v>16.212962962962976</v>
+        <v>17.972222222222221</v>
       </c>
       <c r="Q7" s="3">
-        <v>16.352941176470587</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="2:17">
@@ -768,7 +817,7 @@
         <v>1.5</v>
       </c>
       <c r="D8" s="11">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E8" s="9"/>
       <c r="G8" s="4"/>
@@ -777,31 +826,31 @@
         <v>0.75</v>
       </c>
       <c r="I8" s="3">
-        <v>12.93835294117647</v>
+        <v>12.432000000000002</v>
       </c>
       <c r="J8" s="3">
-        <v>13.810823529411763</v>
+        <v>11.944000000000003</v>
       </c>
       <c r="K8" s="3">
-        <v>14.544941176470589</v>
+        <v>11.624000000000001</v>
       </c>
       <c r="L8" s="3">
-        <v>15.061647058823525</v>
+        <v>11.568000000000003</v>
       </c>
       <c r="M8" s="3">
-        <v>15.409946259985469</v>
+        <v>12.241185185185183</v>
       </c>
       <c r="N8" s="3">
-        <v>15.718111837327518</v>
+        <v>13.980740740740742</v>
       </c>
       <c r="O8" s="3">
-        <v>16.029411764705888</v>
+        <v>16.499999999999996</v>
       </c>
       <c r="P8" s="3">
-        <v>16.263616557734206</v>
+        <v>18.888888888888889</v>
       </c>
       <c r="Q8" s="3">
-        <v>16.265795206971664</v>
+        <v>20.111111111111143</v>
       </c>
     </row>
     <row r="9" spans="2:17">
@@ -817,31 +866,31 @@
         <v>1</v>
       </c>
       <c r="I9" s="3">
-        <v>13.358117647058823</v>
+        <v>12.208000000000002</v>
       </c>
       <c r="J9" s="3">
-        <v>14.148235294117647</v>
+        <v>11.82</v>
       </c>
       <c r="K9" s="3">
-        <v>14.760470588235291</v>
+        <v>11.648000000000003</v>
       </c>
       <c r="L9" s="3">
-        <v>15.211812636165572</v>
+        <v>12.064888888888888</v>
       </c>
       <c r="M9" s="3">
-        <v>15.578701525054463</v>
+        <v>13.347555555555555</v>
       </c>
       <c r="N9" s="3">
-        <v>15.873823529411766</v>
+        <v>15.305</v>
       </c>
       <c r="O9" s="3">
-        <v>16.113289760348582</v>
+        <v>17.555555555555554</v>
       </c>
       <c r="P9" s="3">
-        <v>16.220588235294109</v>
+        <v>19.250000000000025</v>
       </c>
       <c r="Q9" s="3">
-        <v>16.063180827886708</v>
+        <v>19.444444444444443</v>
       </c>
     </row>
     <row r="10" spans="2:17">
@@ -849,7 +898,7 @@
       <c r="C10" s="10">
         <v>3</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="16">
         <v>15</v>
       </c>
       <c r="E10" s="9"/>
@@ -859,31 +908,31 @@
         <v>1.25</v>
       </c>
       <c r="I10" s="3">
-        <v>13.718588235294117</v>
+        <v>12.056000000000001</v>
       </c>
       <c r="J10" s="3">
-        <v>14.399999999999997</v>
+        <v>11.800000000000002</v>
       </c>
       <c r="K10" s="3">
-        <v>14.940838344226574</v>
+        <v>12.029511111111111</v>
       </c>
       <c r="L10" s="3">
-        <v>15.386443572984746</v>
+        <v>12.985244444444444</v>
       </c>
       <c r="M10" s="3">
-        <v>15.731152941176472</v>
+        <v>14.533599999999998</v>
       </c>
       <c r="N10" s="3">
-        <v>15.972043572984745</v>
+        <v>16.388444444444445</v>
       </c>
       <c r="O10" s="3">
-        <v>16.108932461873628</v>
+        <v>18.111111111111128</v>
       </c>
       <c r="P10" s="3">
-        <v>16.067538126361654</v>
+        <v>18.888888888888889</v>
       </c>
       <c r="Q10" s="3">
-        <v>15.444294662309371</v>
+        <v>18.149305555555554</v>
       </c>
     </row>
     <row r="11" spans="2:17">
@@ -901,31 +950,31 @@
         <v>1.5</v>
       </c>
       <c r="I11" s="3">
-        <v>13.999999999999998</v>
+        <v>12.000000000000002</v>
       </c>
       <c r="J11" s="3">
-        <v>14.610384894698617</v>
+        <v>12.092592592592593</v>
       </c>
       <c r="K11" s="3">
-        <v>15.131526506899055</v>
+        <v>12.802370370370371</v>
       </c>
       <c r="L11" s="3">
-        <v>15.545529411764706</v>
+        <v>14.033999999999999</v>
       </c>
       <c r="M11" s="3">
-        <v>15.836781408859837</v>
+        <v>15.565037037037037</v>
       </c>
       <c r="N11" s="3">
-        <v>15.991953522149592</v>
+        <v>17.045925925925943</v>
       </c>
       <c r="O11" s="3">
-        <v>15.999999999999998</v>
+        <v>17.999999999999996</v>
       </c>
       <c r="P11" s="3">
-        <v>15.551073438634717</v>
+        <v>17.902199074074073</v>
       </c>
       <c r="Q11" s="3">
-        <v>14.542120551924477</v>
+        <v>16.796296296296294</v>
       </c>
     </row>
     <row r="12" spans="2:17">
@@ -941,31 +990,31 @@
         <v>1.75</v>
       </c>
       <c r="I12" s="3">
-        <v>14.237472766884528</v>
+        <v>12.222222222222223</v>
       </c>
       <c r="J12" s="3">
-        <v>14.821039526921878</v>
+        <v>12.746031746031747</v>
       </c>
       <c r="K12" s="3">
-        <v>15.304302521008404</v>
+        <v>13.727428571428572</v>
       </c>
       <c r="L12" s="3">
-        <v>15.662585745409272</v>
+        <v>14.989460317460317</v>
       </c>
       <c r="M12" s="3">
-        <v>15.873170245876121</v>
+        <v>16.246222222222237</v>
       </c>
       <c r="N12" s="3">
-        <v>15.915294117647054</v>
+        <v>17.102857142857143</v>
       </c>
       <c r="O12" s="3">
-        <v>15.566964285714288</v>
+        <v>17.281249999999996</v>
       </c>
       <c r="P12" s="3">
-        <v>14.762527233115472</v>
+        <v>16.777777777777779</v>
       </c>
       <c r="Q12" s="3">
-        <v>13.799496187363838</v>
+        <v>15.731646825396824</v>
       </c>
     </row>
     <row r="13" spans="2:17">
@@ -983,31 +1032,31 @@
         <v>2</v>
       </c>
       <c r="I13" s="3">
-        <v>14.468409586056643</v>
+        <v>12.777777777777779</v>
       </c>
       <c r="J13" s="3">
-        <v>15.011029411764707</v>
+        <v>13.5625</v>
       </c>
       <c r="K13" s="3">
-        <v>15.436880174291936</v>
+        <v>14.601777777777778</v>
       </c>
       <c r="L13" s="3">
-        <v>15.71620043572984</v>
+        <v>15.657444444444456</v>
       </c>
       <c r="M13" s="3">
-        <v>15.820941176470585</v>
+        <v>16.396000000000001</v>
       </c>
       <c r="N13" s="3">
-        <v>15.546976102941176</v>
+        <v>16.58609375</v>
       </c>
       <c r="O13" s="3">
-        <v>14.875000000000002</v>
+        <v>16.375</v>
       </c>
       <c r="P13" s="3">
-        <v>14.085180078976038</v>
+        <v>15.848524305555555</v>
       </c>
       <c r="Q13" s="3">
-        <v>13.531590413943357</v>
+        <v>15.222222222222221</v>
       </c>
     </row>
     <row r="14" spans="2:17">
@@ -1023,31 +1072,31 @@
         <v>2.25</v>
       </c>
       <c r="I14" s="3">
-        <v>14.676470588235295</v>
+        <v>13.5</v>
       </c>
       <c r="J14" s="3">
-        <v>15.16146211571048</v>
+        <v>14.358024691358025</v>
       </c>
       <c r="K14" s="3">
-        <v>15.509616073589923</v>
+        <v>15.238617283950626</v>
       </c>
       <c r="L14" s="3">
-        <v>15.687215686274506</v>
+        <v>15.856000000000002</v>
       </c>
       <c r="M14" s="3">
-        <v>15.504031045751637</v>
+        <v>16.015194444444447</v>
       </c>
       <c r="N14" s="3">
-        <v>14.934117647058823</v>
+        <v>15.857777777777777</v>
       </c>
       <c r="O14" s="3">
-        <v>14.260416666666666</v>
+        <v>15.59375</v>
       </c>
       <c r="P14" s="3">
-        <v>13.815298959089811</v>
+        <v>15.382716049382717</v>
       </c>
       <c r="Q14" s="3">
-        <v>14.370672960542246</v>
+        <v>15.873456790123457</v>
       </c>
     </row>
     <row r="15" spans="2:17">
@@ -1056,31 +1105,31 @@
         <v>2.5</v>
       </c>
       <c r="I15" s="3">
-        <v>14.845315904139431</v>
+        <v>14.222222222222223</v>
       </c>
       <c r="J15" s="3">
-        <v>15.254466230936814</v>
+        <v>14.955555555555566</v>
       </c>
       <c r="K15" s="3">
-        <v>15.504188235294114</v>
+        <v>15.459199999999999</v>
       </c>
       <c r="L15" s="3">
-        <v>15.41536911764706</v>
+        <v>15.567275</v>
       </c>
       <c r="M15" s="3">
-        <v>14.956752941176472</v>
+        <v>15.4168</v>
       </c>
       <c r="N15" s="3">
-        <v>14.375080882352941</v>
+        <v>15.206375</v>
       </c>
       <c r="O15" s="3">
-        <v>14</v>
+        <v>15.2</v>
       </c>
       <c r="P15" s="3">
-        <v>14.542102396514164</v>
+        <v>15.952777777777778</v>
       </c>
       <c r="Q15" s="3">
-        <v>15.125272331154685</v>
+        <v>16.477777777777778</v>
       </c>
     </row>
     <row r="16" spans="2:17">
@@ -1089,31 +1138,31 @@
         <v>2.75</v>
       </c>
       <c r="I16" s="3">
-        <v>14.958605664488012</v>
+        <v>14.777777777777787</v>
       </c>
       <c r="J16" s="3">
-        <v>15.27272727272727</v>
+        <v>15.181818181818182</v>
       </c>
       <c r="K16" s="3">
-        <v>15.27369385026738</v>
+        <v>15.232795454545453</v>
       </c>
       <c r="L16" s="3">
-        <v>14.925903743315509</v>
+        <v>15.064</v>
       </c>
       <c r="M16" s="3">
-        <v>14.446479946524066</v>
+        <v>14.864704545454545</v>
       </c>
       <c r="N16" s="3">
-        <v>14.127914438502673</v>
+        <v>14.883636363636363</v>
       </c>
       <c r="O16" s="3">
-        <v>14.643939393939398</v>
+        <v>15.734848484848483</v>
       </c>
       <c r="P16" s="3">
-        <v>15.21251733016439</v>
+        <v>16.494949494949495</v>
       </c>
       <c r="Q16" s="3">
-        <v>15.818429391958803</v>
+        <v>17.047979797979796</v>
       </c>
     </row>
     <row r="17" spans="8:17">
@@ -1122,31 +1171,31 @@
         <v>3</v>
       </c>
       <c r="I17" s="3">
-        <v>14.999999999999998</v>
+        <v>15</v>
       </c>
       <c r="J17" s="3">
-        <v>15.080729166666666</v>
+        <v>14.997395833333334</v>
       </c>
       <c r="K17" s="3">
-        <v>14.836823529411765</v>
+        <v>14.799333333333331</v>
       </c>
       <c r="L17" s="3">
-        <v>14.460724264705883</v>
+        <v>14.587312500000001</v>
       </c>
       <c r="M17" s="3">
-        <v>14.213960784313727</v>
+        <v>14.597333333333333</v>
       </c>
       <c r="N17" s="3">
-        <v>14.707532679738563</v>
+        <v>15.400277777777779</v>
       </c>
       <c r="O17" s="3">
-        <v>15.25</v>
+        <v>16.25</v>
       </c>
       <c r="P17" s="3">
-        <v>15.840640885984024</v>
+        <v>17.016203703703706</v>
       </c>
       <c r="Q17" s="3">
-        <v>16.465504720406685</v>
+        <v>17.592592592592595</v>
       </c>
     </row>
     <row r="18" spans="8:17">
@@ -1158,28 +1207,28 @@
         <v>14.84375</v>
       </c>
       <c r="J18" s="3">
-        <v>14.692307692307692</v>
+        <v>14.615384615384615</v>
       </c>
       <c r="K18" s="3">
-        <v>14.414279411764706</v>
+        <v>14.379673076923076</v>
       </c>
       <c r="L18" s="3">
-        <v>14.244995475113123</v>
+        <v>14.361846153846155</v>
       </c>
       <c r="M18" s="3">
-        <v>14.742374057315233</v>
+        <v>15.096256410256409</v>
       </c>
       <c r="N18" s="3">
-        <v>15.262081447963801</v>
+        <v>15.901538461538461</v>
       </c>
       <c r="O18" s="3">
-        <v>15.826923076923077</v>
+        <v>16.75</v>
       </c>
       <c r="P18" s="3">
-        <v>16.436232612703204</v>
+        <v>17.521367521367527</v>
       </c>
       <c r="Q18" s="3">
-        <v>17.07713256242668</v>
+        <v>18.117521367521366</v>
       </c>
     </row>
     <row r="19" spans="8:17">
@@ -1191,28 +1240,28 @@
         <v>14.5</v>
       </c>
       <c r="J19" s="3">
-        <v>14.310267857142858</v>
+        <v>14.238839285714286</v>
       </c>
       <c r="K19" s="3">
-        <v>14.21727731092437</v>
+        <v>14.185142857142855</v>
       </c>
       <c r="L19" s="3">
-        <v>14.733448179271708</v>
+        <v>14.84195238095238</v>
       </c>
       <c r="M19" s="3">
-        <v>15.254823529411766</v>
+        <v>15.583428571428572</v>
       </c>
       <c r="N19" s="3">
-        <v>15.796932773109244</v>
+        <v>16.390714285714285</v>
       </c>
       <c r="O19" s="3">
-        <v>16.380952380952383</v>
+        <v>17.238095238095241</v>
       </c>
       <c r="P19" s="3">
-        <v>17.006263616557735</v>
+        <v>18.013888888888889</v>
       </c>
       <c r="Q19" s="3">
-        <v>17.660908807967633</v>
+        <v>18.626984126984127</v>
       </c>
     </row>
     <row r="20" spans="8:17">
@@ -1224,28 +1273,28 @@
         <v>14.15625</v>
       </c>
       <c r="J20" s="3">
-        <v>14.133333333333333</v>
+        <v>14.066666666666666</v>
       </c>
       <c r="K20" s="3">
-        <v>14.675014379084967</v>
+        <v>14.645022222222224</v>
       </c>
       <c r="L20" s="3">
-        <v>15.212329411764706</v>
+        <v>15.313600000000001</v>
       </c>
       <c r="M20" s="3">
-        <v>15.754501960784316</v>
+        <v>16.061199999999999</v>
       </c>
       <c r="N20" s="3">
-        <v>16.316026143790854</v>
+        <v>16.870222222222225</v>
       </c>
       <c r="O20" s="3">
-        <v>16.916666666666668</v>
+        <v>17.716666666666665</v>
       </c>
       <c r="P20" s="3">
-        <v>17.555846042120553</v>
+        <v>18.496296296296297</v>
       </c>
       <c r="Q20" s="3">
-        <v>18.222403776325347</v>
+        <v>19.124074074074077</v>
       </c>
     </row>
     <row r="21" spans="8:17">
@@ -1257,28 +1306,28 @@
         <v>14</v>
       </c>
       <c r="J21" s="3">
-        <v>14.567708333333334</v>
+        <v>14.505208333333334</v>
       </c>
       <c r="K21" s="3">
-        <v>15.127617647058823</v>
+        <v>15.099499999999999</v>
       </c>
       <c r="L21" s="3">
-        <v>15.683433823529413</v>
+        <v>15.778375</v>
       </c>
       <c r="M21" s="3">
-        <v>16.243803921568631</v>
+        <v>16.531333333333336</v>
       </c>
       <c r="N21" s="3">
-        <v>16.822316176470586</v>
+        <v>17.341875000000002</v>
       </c>
       <c r="O21" s="3">
-        <v>17.4375</v>
+        <v>18.1875</v>
       </c>
       <c r="P21" s="3">
-        <v>18.088813997821354</v>
+        <v>18.970486111111114</v>
       </c>
       <c r="Q21" s="3">
-        <v>18.765795206971678</v>
+        <v>19.611111111111111</v>
       </c>
     </row>
     <row r="22" spans="8:17">
@@ -1290,28 +1339,28 @@
         <v>14.416666666666668</v>
       </c>
       <c r="J22" s="3">
-        <v>15</v>
+        <v>14.941176470588236</v>
       </c>
       <c r="K22" s="3">
-        <v>15.575993079584775</v>
+        <v>15.549529411764706</v>
       </c>
       <c r="L22" s="3">
-        <v>16.148133794694353</v>
+        <v>16.237490196078433</v>
       </c>
       <c r="M22" s="3">
-        <v>16.724560553633218</v>
+        <v>16.995176470588234</v>
       </c>
       <c r="N22" s="3">
-        <v>17.318062283737021</v>
+        <v>17.807058823529413</v>
       </c>
       <c r="O22" s="3">
-        <v>17.946078431372552</v>
+        <v>18.651960784313729</v>
       </c>
       <c r="P22" s="3">
-        <v>18.608099448929899</v>
+        <v>19.437908496732028</v>
       </c>
       <c r="Q22" s="3">
-        <v>19.294277841855695</v>
+        <v>20.08986928104575</v>
       </c>
     </row>
     <row r="23" spans="8:17">
@@ -1323,28 +1372,28 @@
         <v>14.833333333333334</v>
       </c>
       <c r="J23" s="3">
-        <v>15.430555555555555</v>
+        <v>15.375</v>
       </c>
       <c r="K23" s="3">
-        <v>16.02084531590414</v>
+        <v>15.995851851851853</v>
       </c>
       <c r="L23" s="3">
-        <v>16.607496732026146</v>
+        <v>16.69188888888889</v>
       </c>
       <c r="M23" s="3">
-        <v>17.198196078431373</v>
+        <v>17.453777777777777</v>
       </c>
       <c r="N23" s="3">
-        <v>17.805021786492375</v>
+        <v>18.266851851851854</v>
       </c>
       <c r="O23" s="3">
-        <v>18.444444444444443</v>
+        <v>19.111111111111111</v>
       </c>
       <c r="P23" s="3">
-        <v>19.11598281287824</v>
+        <v>19.899691358024693</v>
       </c>
       <c r="Q23" s="3">
-        <v>19.810336480271122</v>
+        <v>20.561728395061731</v>
       </c>
     </row>
     <row r="24" spans="8:17">
@@ -1356,28 +1405,28 @@
         <v>15.25</v>
       </c>
       <c r="J24" s="3">
-        <v>15.859649122807019</v>
+        <v>15.807017543859651</v>
       </c>
       <c r="K24" s="3">
-        <v>16.4627306501548</v>
+        <v>16.439052631578946</v>
       </c>
       <c r="L24" s="3">
-        <v>17.062365325077401</v>
+        <v>17.142315789473685</v>
       </c>
       <c r="M24" s="3">
-        <v>17.665834881320951</v>
+        <v>17.907964912280704</v>
       </c>
       <c r="N24" s="3">
-        <v>18.284582043343651</v>
+        <v>18.722105263157896</v>
       </c>
       <c r="O24" s="3">
-        <v>18.934210526315791</v>
+        <v>19.565789473684209</v>
       </c>
       <c r="P24" s="3">
-        <v>19.614264419217982</v>
+        <v>20.356725146198833</v>
       </c>
       <c r="Q24" s="3">
-        <v>20.315932805870883</v>
+        <v>21.027777777777775</v>
       </c>
     </row>
     <row r="25" spans="8:17">
@@ -1389,28 +1438,28 @@
         <v>15.666666666666668</v>
       </c>
       <c r="J25" s="3">
-        <v>16.287500000000001</v>
+        <v>16.237500000000001</v>
       </c>
       <c r="K25" s="3">
-        <v>16.90209411764706</v>
+        <v>16.8796</v>
       </c>
       <c r="L25" s="3">
-        <v>17.513413725490199</v>
+        <v>17.58936666666667</v>
       </c>
       <c r="M25" s="3">
-        <v>18.128376470588236</v>
+        <v>18.3584</v>
       </c>
       <c r="N25" s="3">
-        <v>18.75785294117647</v>
+        <v>19.173500000000001</v>
       </c>
       <c r="O25" s="3">
-        <v>19.416666666666668</v>
+        <v>20.016666666666669</v>
       </c>
       <c r="P25" s="3">
-        <v>20.104384531590412</v>
+        <v>20.80972222222222</v>
       </c>
       <c r="Q25" s="3">
-        <v>20.812636165577342</v>
+        <v>21.488888888888887</v>
       </c>
     </row>
     <row r="26" spans="8:17">
@@ -1422,28 +1471,28 @@
         <v>16.083333333333332</v>
       </c>
       <c r="J26" s="3">
-        <v>16.714285714285715</v>
+        <v>16.666666666666668</v>
       </c>
       <c r="K26" s="3">
-        <v>17.339295985060694</v>
+        <v>17.317873015873015</v>
       </c>
       <c r="L26" s="3">
-        <v>17.961187675070029</v>
+        <v>18.03352380952381</v>
       </c>
       <c r="M26" s="3">
-        <v>18.586549019607844</v>
+        <v>18.805619047619047</v>
       </c>
       <c r="N26" s="3">
-        <v>19.225732959850607</v>
+        <v>19.621587301587304</v>
       </c>
       <c r="O26" s="3">
-        <v>19.892857142857139</v>
+        <v>20.464285714285712</v>
       </c>
       <c r="P26" s="3">
-        <v>20.587509077705157</v>
+        <v>21.25925925925926</v>
       </c>
       <c r="Q26" s="3">
-        <v>20.726320157692708</v>
+        <v>21.37037037037037</v>
       </c>
     </row>
     <row r="27" spans="8:17">
@@ -1455,28 +1504,28 @@
         <v>16.5</v>
       </c>
       <c r="J27" s="3">
-        <v>17.140151515151516</v>
+        <v>17.094696969696972</v>
       </c>
       <c r="K27" s="3">
-        <v>17.774631016042779</v>
+        <v>17.754181818181817</v>
       </c>
       <c r="L27" s="3">
-        <v>18.406133689839574</v>
+        <v>18.47518181818182</v>
       </c>
       <c r="M27" s="3">
-        <v>19.040948306595368</v>
+        <v>19.250060606060607</v>
       </c>
       <c r="N27" s="3">
-        <v>19.688957219251336</v>
+        <v>20.066818181818178</v>
       </c>
       <c r="O27" s="3">
-        <v>20.363636363636363</v>
+        <v>20.90909090909091</v>
       </c>
       <c r="P27" s="3">
-        <v>20.515349574173104</v>
+        <v>21.156565656565657</v>
       </c>
       <c r="Q27" s="3">
-        <v>20.647851059615764</v>
+        <v>21.262626262626263</v>
       </c>
     </row>
     <row r="28" spans="8:17">
@@ -1488,28 +1537,28 @@
         <v>16.916666666666668</v>
       </c>
       <c r="J28" s="3">
-        <v>17.565217391304348</v>
+        <v>17.521739130434781</v>
       </c>
       <c r="K28" s="3">
-        <v>18.208342710997442</v>
+        <v>18.18878260869565</v>
       </c>
       <c r="L28" s="3">
-        <v>18.848620630861042</v>
+        <v>18.914666666666669</v>
       </c>
       <c r="M28" s="3">
-        <v>19.49206649616368</v>
+        <v>19.692086956521738</v>
       </c>
       <c r="N28" s="3">
-        <v>20.148132992327366</v>
+        <v>20.509565217391305</v>
       </c>
       <c r="O28" s="3">
-        <v>20.304347826086957</v>
+        <v>20.826086956521738</v>
       </c>
       <c r="P28" s="3">
-        <v>20.44946481007862</v>
+        <v>21.062801932367151</v>
       </c>
       <c r="Q28" s="3">
-        <v>20.576205361371603</v>
+        <v>21.164251207729468</v>
       </c>
     </row>
     <row r="29" spans="8:17">
@@ -1521,28 +1570,28 @@
         <v>17.333333333333332</v>
       </c>
       <c r="J29" s="3">
-        <v>17.989583333333332</v>
+        <v>17.947916666666668</v>
       </c>
       <c r="K29" s="3">
-        <v>18.640633986928105</v>
+        <v>18.62188888888889</v>
       </c>
       <c r="L29" s="3">
-        <v>19.288955882352941</v>
+        <v>19.352249999999998</v>
       </c>
       <c r="M29" s="3">
-        <v>19.940313725490196</v>
+        <v>20.132000000000001</v>
       </c>
       <c r="N29" s="3">
-        <v>20.100294117647056</v>
+        <v>20.446666666666669</v>
       </c>
       <c r="O29" s="3">
-        <v>20.25</v>
+        <v>20.75</v>
       </c>
       <c r="P29" s="3">
-        <v>20.389070442992011</v>
+        <v>20.976851851851851</v>
       </c>
       <c r="Q29" s="3">
-        <v>20.510530137981117</v>
+        <v>21.074074074074073</v>
       </c>
     </row>
     <row r="30" spans="8:17">
@@ -1554,28 +1603,28 @@
         <v>17.75</v>
       </c>
       <c r="J30" s="3">
-        <v>18.413333333333334</v>
+        <v>18.373333333333335</v>
       </c>
       <c r="K30" s="3">
-        <v>19.071675294117643</v>
+        <v>19.053679999999996</v>
       </c>
       <c r="L30" s="3">
-        <v>19.727397647058822</v>
+        <v>19.788160000000001</v>
       </c>
       <c r="M30" s="3">
-        <v>19.90270117647059</v>
+        <v>20.08672</v>
       </c>
       <c r="N30" s="3">
-        <v>20.056282352941174</v>
+        <v>20.3888</v>
       </c>
       <c r="O30" s="3">
-        <v>20.2</v>
+        <v>20.68</v>
       </c>
       <c r="P30" s="3">
-        <v>20.333507625272333</v>
+        <v>20.89777777777778</v>
       </c>
       <c r="Q30" s="3">
-        <v>20.450108932461873</v>
+        <v>20.991111111111113</v>
       </c>
     </row>
     <row r="31" spans="8:17">
@@ -1587,28 +1636,28 @@
         <v>18.166666666666668</v>
       </c>
       <c r="J31" s="3">
-        <v>18.83653846153846</v>
+        <v>18.79807692307692</v>
       </c>
       <c r="K31" s="3">
-        <v>19.501610859728508</v>
+        <v>19.484307692307691</v>
       </c>
       <c r="L31" s="3">
-        <v>19.699420814479637</v>
+        <v>19.757846153846153</v>
       </c>
       <c r="M31" s="3">
-        <v>19.867981900452488</v>
+        <v>20.044923076923077</v>
       </c>
       <c r="N31" s="3">
-        <v>20.015656108597284</v>
+        <v>20.335384615384616</v>
       </c>
       <c r="O31" s="3">
-        <v>20.153846153846153</v>
+        <v>20.615384615384617</v>
       </c>
       <c r="P31" s="3">
-        <v>20.282218870454166</v>
+        <v>20.824786324786324</v>
       </c>
       <c r="Q31" s="3">
-        <v>20.394335511982572</v>
+        <v>20.914529914529915</v>
       </c>
     </row>
     <row r="32" spans="8:17">
@@ -1620,28 +1669,28 @@
         <v>18.583333333333332</v>
       </c>
       <c r="J32" s="3">
-        <v>19.25925925925926</v>
+        <v>19.222222222222221</v>
       </c>
       <c r="K32" s="3">
-        <v>19.483032679738564</v>
+        <v>19.46637037037037</v>
       </c>
       <c r="L32" s="3">
-        <v>19.673516339869281</v>
+        <v>19.729777777777777</v>
       </c>
       <c r="M32" s="3">
-        <v>19.83583442265795</v>
+        <v>20.006222222222224</v>
       </c>
       <c r="N32" s="3">
-        <v>19.978039215686273</v>
+        <v>20.285925925925927</v>
       </c>
       <c r="O32" s="3">
-        <v>20.111111111111111</v>
+        <v>20.555555555555557</v>
       </c>
       <c r="P32" s="3">
-        <v>20.234729282659568</v>
+        <v>20.757201646090536</v>
       </c>
       <c r="Q32" s="3">
-        <v>20.34269345598322</v>
+        <v>20.843621399176957</v>
       </c>
     </row>
     <row r="33" spans="8:17">
@@ -1653,28 +1702,28 @@
         <v>19</v>
       </c>
       <c r="J33" s="3">
-        <v>19.25</v>
+        <v>19.214285714285715</v>
       </c>
       <c r="K33" s="3">
-        <v>19.465781512605044</v>
+        <v>19.449714285714286</v>
       </c>
       <c r="L33" s="3">
-        <v>19.649462184873951</v>
+        <v>19.703714285714284</v>
       </c>
       <c r="M33" s="3">
-        <v>19.80598319327731</v>
+        <v>19.970285714285716</v>
       </c>
       <c r="N33" s="3">
-        <v>19.943109243697478</v>
+        <v>20.240000000000002</v>
       </c>
       <c r="O33" s="3">
-        <v>20.071428571428573</v>
+        <v>20.5</v>
       </c>
       <c r="P33" s="3">
-        <v>20.190631808278869</v>
+        <v>20.694444444444446</v>
       </c>
       <c r="Q33" s="3">
-        <v>20.294740118269534</v>
+        <v>20.777777777777779</v>
       </c>
     </row>
     <row r="34" spans="8:17">
@@ -1686,28 +1735,28 @@
         <v>19</v>
       </c>
       <c r="J34" s="3">
-        <v>19.241379310344829</v>
+        <v>19.206896551724139</v>
       </c>
       <c r="K34" s="3">
-        <v>19.449720081135904</v>
+        <v>19.434206896551725</v>
       </c>
       <c r="L34" s="3">
-        <v>19.627066937119675</v>
+        <v>19.679448275862068</v>
       </c>
       <c r="M34" s="3">
-        <v>19.778190669371195</v>
+        <v>19.936827586206896</v>
       </c>
       <c r="N34" s="3">
-        <v>19.910588235294117</v>
+        <v>20.197241379310345</v>
       </c>
       <c r="O34" s="3">
-        <v>20.03448275862069</v>
+        <v>20.448275862068964</v>
       </c>
       <c r="P34" s="3">
-        <v>20.149575539027872</v>
+        <v>20.636015325670499</v>
       </c>
       <c r="Q34" s="3">
-        <v>20.250093907294719</v>
+        <v>20.716475095785441</v>
       </c>
     </row>
     <row r="35" spans="8:17">
@@ -1719,28 +1768,28 @@
         <v>19</v>
       </c>
       <c r="J35" s="3">
-        <v>19.233333333333334</v>
+        <v>19.2</v>
       </c>
       <c r="K35" s="3">
-        <v>19.434729411764707</v>
+        <v>19.419733333333333</v>
       </c>
       <c r="L35" s="3">
-        <v>19.606164705882353</v>
+        <v>19.656799999999997</v>
       </c>
       <c r="M35" s="3">
-        <v>19.752250980392155</v>
+        <v>19.9056</v>
       </c>
       <c r="N35" s="3">
-        <v>19.880235294117647</v>
+        <v>20.157333333333334</v>
       </c>
       <c r="O35" s="3">
-        <v>20</v>
+        <v>20.399999999999999</v>
       </c>
       <c r="P35" s="3">
-        <v>20.11125635439361</v>
+        <v>20.581481481481482</v>
       </c>
       <c r="Q35" s="3">
-        <v>20.208424110384897</v>
+        <v>20.659259259259262</v>
       </c>
     </row>
     <row r="36" spans="8:17">
@@ -1752,28 +1801,28 @@
         <v>19</v>
       </c>
       <c r="J36" s="3">
-        <v>19.225806451612904</v>
+        <v>19.193548387096776</v>
       </c>
       <c r="K36" s="3">
-        <v>19.420705882352944</v>
+        <v>19.406193548387098</v>
       </c>
       <c r="L36" s="3">
-        <v>19.5866110056926</v>
+        <v>19.635612903225805</v>
       </c>
       <c r="M36" s="3">
-        <v>19.727984819734345</v>
+        <v>19.876387096774195</v>
       </c>
       <c r="N36" s="3">
-        <v>19.851840607210626</v>
+        <v>20.12</v>
       </c>
       <c r="O36" s="3">
-        <v>19.967741935483872</v>
+        <v>20.35483870967742</v>
       </c>
       <c r="P36" s="3">
-        <v>20.075409375219621</v>
+        <v>20.53046594982079</v>
       </c>
       <c r="Q36" s="3">
-        <v>20.169442687469253</v>
+        <v>20.605734767025091</v>
       </c>
     </row>
     <row r="37" spans="8:17">
@@ -1785,28 +1834,28 @@
         <v>19</v>
       </c>
       <c r="J37" s="3">
-        <v>19.21875</v>
+        <v>19.1875</v>
       </c>
       <c r="K37" s="3">
-        <v>19.407558823529413</v>
+        <v>19.3935</v>
       </c>
       <c r="L37" s="3">
-        <v>19.568279411764706</v>
+        <v>19.615749999999998</v>
       </c>
       <c r="M37" s="3">
-        <v>19.705235294117646</v>
+        <v>19.849</v>
       </c>
       <c r="N37" s="3">
-        <v>19.825220588235293</v>
+        <v>20.085000000000001</v>
       </c>
       <c r="O37" s="3">
-        <v>19.9375</v>
+        <v>20.3125</v>
       </c>
       <c r="P37" s="3">
-        <v>20.041802832244009</v>
+        <v>20.482638888888889</v>
       </c>
       <c r="Q37" s="3">
-        <v>20.132897603485841</v>
+        <v>20.555555555555557</v>
       </c>
     </row>
     <row r="38" spans="8:17">
@@ -1818,28 +1867,28 @@
         <v>19</v>
       </c>
       <c r="J38" s="3">
-        <v>19.212121212121211</v>
+        <v>19.181818181818183</v>
       </c>
       <c r="K38" s="3">
-        <v>19.395208556149733</v>
+        <v>19.381575757575757</v>
       </c>
       <c r="L38" s="3">
-        <v>19.551058823529413</v>
+        <v>19.597090909090909</v>
       </c>
       <c r="M38" s="3">
-        <v>19.683864527629233</v>
+        <v>19.823272727272727</v>
       </c>
       <c r="N38" s="3">
-        <v>19.800213903743316</v>
+        <v>20.052121212121214</v>
       </c>
       <c r="O38" s="3">
-        <v>19.90909090909091</v>
+        <v>20.272727272727273</v>
       </c>
       <c r="P38" s="3">
-        <v>20.010233049448736</v>
+        <v>20.437710437710439</v>
       </c>
       <c r="Q38" s="3">
-        <v>20.098567373077177</v>
+        <v>20.508417508417509</v>
       </c>
     </row>
     <row r="39" spans="8:17">
@@ -1851,28 +1900,28 @@
         <v>19</v>
       </c>
       <c r="J39" s="3">
-        <v>19.205882352941178</v>
+        <v>19.176470588235293</v>
       </c>
       <c r="K39" s="3">
-        <v>19.383584775086508</v>
+        <v>19.370352941176471</v>
       </c>
       <c r="L39" s="3">
-        <v>19.534851211072663</v>
+        <v>19.579529411764703</v>
       </c>
       <c r="M39" s="3">
-        <v>19.663750865051902</v>
+        <v>19.79905882352941</v>
       </c>
       <c r="N39" s="3">
-        <v>19.776678200692039</v>
+        <v>20.021176470588237</v>
       </c>
       <c r="O39" s="3">
-        <v>19.882352941176471</v>
+        <v>20.235294117647058</v>
       </c>
       <c r="P39" s="3">
-        <v>19.980520312700243</v>
+        <v>20.395424836601308</v>
       </c>
       <c r="Q39" s="3">
-        <v>20.066256567986674</v>
+        <v>20.464052287581701</v>
       </c>
     </row>
     <row r="40" spans="8:17">
@@ -1884,28 +1933,28 @@
         <v>19</v>
       </c>
       <c r="J40" s="3">
-        <v>19.2</v>
+        <v>19.171428571428571</v>
       </c>
       <c r="K40" s="3">
-        <v>19.372625210084035</v>
+        <v>19.359771428571428</v>
       </c>
       <c r="L40" s="3">
-        <v>19.519569747899158</v>
+        <v>19.562971428571426</v>
       </c>
       <c r="M40" s="3">
-        <v>19.644786554621849</v>
+        <v>19.776228571428572</v>
       </c>
       <c r="N40" s="3">
-        <v>19.754487394957984</v>
+        <v>19.992000000000001</v>
       </c>
       <c r="O40" s="3">
-        <v>19.857142857142858</v>
+        <v>20.2</v>
       </c>
       <c r="P40" s="3">
-        <v>19.952505446623093</v>
+        <v>20.355555555555554</v>
       </c>
       <c r="Q40" s="3">
-        <v>20.035792094615626</v>
+        <v>20.422222222222224</v>
       </c>
     </row>
     <row r="41" spans="8:17">
@@ -1917,28 +1966,28 @@
         <v>19</v>
       </c>
       <c r="J41" s="3">
-        <v>19.194444444444443</v>
+        <v>19.166666666666668</v>
       </c>
       <c r="K41" s="3">
-        <v>19.362274509803925</v>
+        <v>19.349777777777778</v>
       </c>
       <c r="L41" s="3">
-        <v>19.50513725490196</v>
+        <v>19.547333333333331</v>
       </c>
       <c r="M41" s="3">
-        <v>19.626875816993461</v>
+        <v>19.754666666666665</v>
       </c>
       <c r="N41" s="3">
-        <v>19.733529411764707</v>
+        <v>19.964444444444446</v>
       </c>
       <c r="O41" s="3">
-        <v>19.833333333333332</v>
+        <v>20.166666666666668</v>
       </c>
       <c r="P41" s="3">
-        <v>19.926046961994675</v>
+        <v>20.317901234567902</v>
       </c>
       <c r="Q41" s="3">
-        <v>20.007020091987414</v>
+        <v>20.382716049382719</v>
       </c>
     </row>
     <row r="42" spans="8:17">
@@ -1950,28 +1999,28 @@
         <v>19</v>
       </c>
       <c r="J42" s="3">
-        <v>19.189189189189189</v>
+        <v>19.162162162162161</v>
       </c>
       <c r="K42" s="3">
-        <v>19.352483306836248</v>
+        <v>19.340324324324325</v>
       </c>
       <c r="L42" s="3">
-        <v>19.491484896661369</v>
+        <v>19.532540540540538</v>
       </c>
       <c r="M42" s="3">
-        <v>19.609933227344992</v>
+        <v>19.734270270270269</v>
       </c>
       <c r="N42" s="3">
-        <v>19.713704292527822</v>
+        <v>19.938378378378378</v>
       </c>
       <c r="O42" s="3">
-        <v>19.810810810810811</v>
+        <v>20.135135135135137</v>
       </c>
       <c r="P42" s="3">
-        <v>19.90101866572455</v>
+        <v>20.282282282282281</v>
       </c>
       <c r="Q42" s="3">
-        <v>19.97980333274451</v>
+        <v>20.345345345345347</v>
       </c>
     </row>
     <row r="43" spans="8:17">
@@ -1983,28 +2032,28 @@
         <v>19</v>
       </c>
       <c r="J43" s="3">
-        <v>19.184210526315791</v>
+        <v>19.157894736842106</v>
       </c>
       <c r="K43" s="3">
-        <v>19.343207430340559</v>
+        <v>19.33136842105263</v>
       </c>
       <c r="L43" s="3">
-        <v>19.478551083591331</v>
+        <v>19.518526315789472</v>
       </c>
       <c r="M43" s="3">
-        <v>19.593882352941176</v>
+        <v>19.714947368421054</v>
       </c>
       <c r="N43" s="3">
-        <v>19.694922600619194</v>
+        <v>19.913684210526316</v>
       </c>
       <c r="O43" s="3">
-        <v>19.789473684210527</v>
+        <v>20.105263157894736</v>
       </c>
       <c r="P43" s="3">
-        <v>19.87730764820548</v>
+        <v>20.248538011695906</v>
       </c>
       <c r="Q43" s="3">
-        <v>19.954019034514392</v>
+        <v>20.309941520467838</v>
       </c>
     </row>
     <row r="44" spans="8:17">
@@ -2016,28 +2065,28 @@
         <v>19</v>
       </c>
       <c r="J44" s="3">
-        <v>19.179487179487179</v>
+        <v>19.153846153846153</v>
       </c>
       <c r="K44" s="3">
-        <v>19.334407239819004</v>
+        <v>19.322871794871794</v>
       </c>
       <c r="L44" s="3">
-        <v>19.466280542986425</v>
+        <v>19.505230769230767</v>
       </c>
       <c r="M44" s="3">
-        <v>19.578654600301657</v>
+        <v>19.696615384615384</v>
       </c>
       <c r="N44" s="3">
-        <v>19.67710407239819</v>
+        <v>19.890256410256409</v>
       </c>
       <c r="O44" s="3">
-        <v>19.76923076923077</v>
+        <v>20.076923076923077</v>
       </c>
       <c r="P44" s="3">
-        <v>19.854812580302777</v>
+        <v>20.216524216524217</v>
       </c>
       <c r="Q44" s="3">
-        <v>19.929557007988382</v>
+        <v>20.276353276353277</v>
       </c>
     </row>
   </sheetData>
@@ -2048,4 +2097,1488 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="C4:U44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="35.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:21">
+      <c r="C4" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="24"/>
+      <c r="F4" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="26"/>
+      <c r="H4" s="27"/>
+      <c r="K4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" s="1"/>
+      <c r="M4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+    </row>
+    <row r="5" spans="3:21" ht="15.75" thickBot="1">
+      <c r="C5" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="L5" s="2"/>
+      <c r="M5" s="6">
+        <v>0</v>
+      </c>
+      <c r="N5" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="O5" s="6">
+        <f>N5+0.25</f>
+        <v>0.5</v>
+      </c>
+      <c r="P5" s="6">
+        <f t="shared" ref="P5:U5" si="0">O5+0.25</f>
+        <v>0.75</v>
+      </c>
+      <c r="Q5" s="6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R5" s="6">
+        <f t="shared" si="0"/>
+        <v>1.25</v>
+      </c>
+      <c r="S5" s="6">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="T5" s="6">
+        <f t="shared" si="0"/>
+        <v>1.75</v>
+      </c>
+      <c r="U5" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="3:21">
+      <c r="C6" s="10">
+        <v>0.25</v>
+      </c>
+      <c r="D6" s="11">
+        <v>12</v>
+      </c>
+      <c r="F6" s="18">
+        <v>0.75</v>
+      </c>
+      <c r="G6" s="19">
+        <v>1.75</v>
+      </c>
+      <c r="H6" s="11">
+        <v>12.5</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="L6" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="M6" s="3">
+        <f t="array" ref="M6:U44">FS("Kalahari.splineSurfaceWithForwardPointsAdded", C6:C14,D6:D14,F6:H15,D18,M5:U5,L6:L44)</f>
+        <v>12</v>
+      </c>
+      <c r="N6" s="3">
+        <v>12</v>
+      </c>
+      <c r="O6" s="3">
+        <v>12</v>
+      </c>
+      <c r="P6" s="3">
+        <v>12</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>12</v>
+      </c>
+      <c r="R6" s="3">
+        <v>12</v>
+      </c>
+      <c r="S6" s="3">
+        <v>13.999999999999943</v>
+      </c>
+      <c r="T6" s="3">
+        <v>16.46084729064043</v>
+      </c>
+      <c r="U6" s="3">
+        <v>19.135448275862018</v>
+      </c>
+    </row>
+    <row r="7" spans="3:21">
+      <c r="C7" s="10">
+        <v>1</v>
+      </c>
+      <c r="D7" s="11"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="11"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="7">
+        <f>L6+0.25</f>
+        <v>0.5</v>
+      </c>
+      <c r="M7" s="3">
+        <v>12</v>
+      </c>
+      <c r="N7" s="3">
+        <v>12</v>
+      </c>
+      <c r="O7" s="3">
+        <v>12</v>
+      </c>
+      <c r="P7" s="3">
+        <v>12</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>12</v>
+      </c>
+      <c r="R7" s="3">
+        <v>12.999999999999972</v>
+      </c>
+      <c r="S7" s="3">
+        <v>15.230423645320187</v>
+      </c>
+      <c r="T7" s="3">
+        <v>17.798147783251224</v>
+      </c>
+      <c r="U7" s="3">
+        <v>19.890955665024634</v>
+      </c>
+    </row>
+    <row r="8" spans="3:21">
+      <c r="C8" s="10">
+        <v>1.5</v>
+      </c>
+      <c r="D8" s="11">
+        <v>12</v>
+      </c>
+      <c r="F8" s="18"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="11"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="7">
+        <f t="shared" ref="L8:L43" si="1">L7+0.25</f>
+        <v>0.75</v>
+      </c>
+      <c r="M8" s="3">
+        <v>12</v>
+      </c>
+      <c r="N8" s="3">
+        <v>12</v>
+      </c>
+      <c r="O8" s="3">
+        <v>12</v>
+      </c>
+      <c r="P8" s="3">
+        <v>12</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>12.666666666666648</v>
+      </c>
+      <c r="R8" s="3">
+        <v>14.153615763546791</v>
+      </c>
+      <c r="S8" s="3">
+        <v>16.532098522167463</v>
+      </c>
+      <c r="T8" s="3">
+        <v>18.747586206896568</v>
+      </c>
+      <c r="U8" s="3">
+        <v>20.030975369458105</v>
+      </c>
+    </row>
+    <row r="9" spans="3:21">
+      <c r="C9" s="10">
+        <v>2</v>
+      </c>
+      <c r="D9" s="11"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="11"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M9" s="3">
+        <v>12</v>
+      </c>
+      <c r="N9" s="3">
+        <v>12</v>
+      </c>
+      <c r="O9" s="3">
+        <v>12</v>
+      </c>
+      <c r="P9" s="3">
+        <v>12.499999999999986</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>13.615211822660093</v>
+      </c>
+      <c r="R9" s="3">
+        <v>15.399073891625598</v>
+      </c>
+      <c r="S9" s="3">
+        <v>17.560689655172411</v>
+      </c>
+      <c r="T9" s="3">
+        <v>19.138443349753686</v>
+      </c>
+      <c r="U9" s="3">
+        <v>19.384788177339928</v>
+      </c>
+    </row>
+    <row r="10" spans="3:21">
+      <c r="C10" s="10">
+        <v>3</v>
+      </c>
+      <c r="D10" s="16">
+        <v>15</v>
+      </c>
+      <c r="F10" s="18"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="11"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="7">
+        <f t="shared" si="1"/>
+        <v>1.25</v>
+      </c>
+      <c r="M10" s="3">
+        <v>12</v>
+      </c>
+      <c r="N10" s="3">
+        <v>12</v>
+      </c>
+      <c r="O10" s="3">
+        <v>12.399999999999988</v>
+      </c>
+      <c r="P10" s="3">
+        <v>13.292169458128075</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>14.719259113300478</v>
+      </c>
+      <c r="R10" s="3">
+        <v>16.448551724137928</v>
+      </c>
+      <c r="S10" s="3">
+        <v>18.110754679802938</v>
+      </c>
+      <c r="T10" s="3">
+        <v>18.800000000000029</v>
+      </c>
+      <c r="U10" s="3">
+        <v>18.101580541871925</v>
+      </c>
+    </row>
+    <row r="11" spans="3:21">
+      <c r="C11" s="10">
+        <v>4</v>
+      </c>
+      <c r="D11" s="11">
+        <v>14</v>
+      </c>
+      <c r="F11" s="18"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="11"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="7">
+        <f t="shared" si="1"/>
+        <v>1.5</v>
+      </c>
+      <c r="M11" s="3">
+        <v>12</v>
+      </c>
+      <c r="N11" s="3">
+        <v>12.333333333333323</v>
+      </c>
+      <c r="O11" s="3">
+        <v>13.076807881773396</v>
+      </c>
+      <c r="P11" s="3">
+        <v>14.266049261083731</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>15.707126436781607</v>
+      </c>
+      <c r="R11" s="3">
+        <v>17.092295566502447</v>
+      </c>
+      <c r="S11" s="3">
+        <v>18.000000000000014</v>
+      </c>
+      <c r="T11" s="3">
+        <v>17.828125000000011</v>
+      </c>
+      <c r="U11" s="3">
+        <v>16.756525451559938</v>
+      </c>
+    </row>
+    <row r="12" spans="3:21">
+      <c r="C12" s="10">
+        <v>5</v>
+      </c>
+      <c r="D12" s="11"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="11"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="7">
+        <f t="shared" si="1"/>
+        <v>1.75</v>
+      </c>
+      <c r="M12" s="3">
+        <v>12.285714285714278</v>
+      </c>
+      <c r="N12" s="3">
+        <v>12.922978184377197</v>
+      </c>
+      <c r="O12" s="3">
+        <v>13.94232793807177</v>
+      </c>
+      <c r="P12" s="3">
+        <v>15.177536945812806</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>16.364824771287811</v>
+      </c>
+      <c r="R12" s="3">
+        <v>17.142857142857157</v>
+      </c>
+      <c r="S12" s="3">
+        <v>17.28125</v>
+      </c>
+      <c r="T12" s="3">
+        <v>16.714285714285722</v>
+      </c>
+      <c r="U12" s="3">
+        <v>15.697557529908519</v>
+      </c>
+    </row>
+    <row r="13" spans="3:21">
+      <c r="C13" s="10">
+        <v>7</v>
+      </c>
+      <c r="D13" s="11">
+        <v>19</v>
+      </c>
+      <c r="F13" s="18"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="11"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="7">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="M13" s="3">
+        <v>12.807605911330047</v>
+      </c>
+      <c r="N13" s="3">
+        <v>13.699536945812799</v>
+      </c>
+      <c r="O13" s="3">
+        <v>14.780344827586205</v>
+      </c>
+      <c r="P13" s="3">
+        <v>15.819221674876836</v>
+      </c>
+      <c r="Q13" s="3">
+        <v>16.500000000000011</v>
+      </c>
+      <c r="R13" s="3">
+        <v>16.62109375</v>
+      </c>
+      <c r="S13" s="3">
+        <v>16.375</v>
+      </c>
+      <c r="T13" s="3">
+        <v>15.792968750000007</v>
+      </c>
+      <c r="U13" s="3">
+        <v>15.192394088669953</v>
+      </c>
+    </row>
+    <row r="14" spans="3:21">
+      <c r="C14" s="12">
+        <v>10</v>
+      </c>
+      <c r="D14" s="13"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="11"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="7">
+        <f t="shared" si="1"/>
+        <v>2.25</v>
+      </c>
+      <c r="M14" s="3">
+        <v>13.510699507389155</v>
+      </c>
+      <c r="N14" s="3">
+        <v>14.471417624521072</v>
+      </c>
+      <c r="O14" s="3">
+        <v>15.394863711001632</v>
+      </c>
+      <c r="P14" s="3">
+        <v>16.000000000000011</v>
+      </c>
+      <c r="Q14" s="3">
+        <v>16.107638888888889</v>
+      </c>
+      <c r="R14" s="3">
+        <v>15.888888888888889</v>
+      </c>
+      <c r="S14" s="3">
+        <v>15.59375</v>
+      </c>
+      <c r="T14" s="3">
+        <v>15.333333333333339</v>
+      </c>
+      <c r="U14" s="3">
+        <v>15.846942893632551</v>
+      </c>
+    </row>
+    <row r="15" spans="3:21">
+      <c r="F15" s="20"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="13"/>
+      <c r="L15" s="7">
+        <f t="shared" si="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="M15" s="3">
+        <v>14.224275862068964</v>
+      </c>
+      <c r="N15" s="3">
+        <v>15.055377339901469</v>
+      </c>
+      <c r="O15" s="3">
+        <v>15.600000000000009</v>
+      </c>
+      <c r="P15" s="3">
+        <v>15.696875</v>
+      </c>
+      <c r="Q15" s="3">
+        <v>15.5</v>
+      </c>
+      <c r="R15" s="3">
+        <v>15.234375</v>
+      </c>
+      <c r="S15" s="3">
+        <v>15.2</v>
+      </c>
+      <c r="T15" s="3">
+        <v>15.90833333333334</v>
+      </c>
+      <c r="U15" s="3">
+        <v>16.453915270935962</v>
+      </c>
+    </row>
+    <row r="16" spans="3:21">
+      <c r="L16" s="7">
+        <f t="shared" si="1"/>
+        <v>2.75</v>
+      </c>
+      <c r="M16" s="3">
+        <v>14.777615763546789</v>
+      </c>
+      <c r="N16" s="3">
+        <v>15.27272727272728</v>
+      </c>
+      <c r="O16" s="3">
+        <v>15.360795454545455</v>
+      </c>
+      <c r="P16" s="3">
+        <v>15.181818181818182</v>
+      </c>
+      <c r="Q16" s="3">
+        <v>14.940340909090908</v>
+      </c>
+      <c r="R16" s="3">
+        <v>14.909090909090908</v>
+      </c>
+      <c r="S16" s="3">
+        <v>15.734848484848486</v>
+      </c>
+      <c r="T16" s="3">
+        <v>16.45454545454546</v>
+      </c>
+      <c r="U16" s="3">
+        <v>17.026286609941785</v>
+      </c>
+    </row>
+    <row r="17" spans="3:21">
+      <c r="L17" s="7">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="M17" s="3">
+        <v>15.000000000000007</v>
+      </c>
+      <c r="N17" s="3">
+        <v>15.080729166666666</v>
+      </c>
+      <c r="O17" s="3">
+        <v>14.916666666666666</v>
+      </c>
+      <c r="P17" s="3">
+        <v>14.6953125</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>14.666666666666666</v>
+      </c>
+      <c r="R17" s="3">
+        <v>15.423611111111112</v>
+      </c>
+      <c r="S17" s="3">
+        <v>16.25</v>
+      </c>
+      <c r="T17" s="3">
+        <v>16.979166666666671</v>
+      </c>
+      <c r="U17" s="3">
+        <v>17.572707170224415</v>
+      </c>
+    </row>
+    <row r="18" spans="3:21">
+      <c r="C18" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="L18" s="7">
+        <f t="shared" si="1"/>
+        <v>3.25</v>
+      </c>
+      <c r="M18" s="3">
+        <v>14.84375</v>
+      </c>
+      <c r="N18" s="3">
+        <v>14.692307692307692</v>
+      </c>
+      <c r="O18" s="3">
+        <v>14.48798076923077</v>
+      </c>
+      <c r="P18" s="3">
+        <v>14.461538461538462</v>
+      </c>
+      <c r="Q18" s="3">
+        <v>15.160256410256411</v>
+      </c>
+      <c r="R18" s="3">
+        <v>15.923076923076923</v>
+      </c>
+      <c r="S18" s="3">
+        <v>16.75</v>
+      </c>
+      <c r="T18" s="3">
+        <v>17.487179487179496</v>
+      </c>
+      <c r="U18" s="3">
+        <v>18.099165593027664</v>
+      </c>
+    </row>
+    <row r="19" spans="3:21">
+      <c r="L19" s="7">
+        <f t="shared" si="1"/>
+        <v>3.5</v>
+      </c>
+      <c r="M19" s="3">
+        <v>14.5</v>
+      </c>
+      <c r="N19" s="3">
+        <v>14.310267857142858</v>
+      </c>
+      <c r="O19" s="3">
+        <v>14.285714285714286</v>
+      </c>
+      <c r="P19" s="3">
+        <v>14.93452380952381</v>
+      </c>
+      <c r="Q19" s="3">
+        <v>15.642857142857142</v>
+      </c>
+      <c r="R19" s="3">
+        <v>16.410714285714285</v>
+      </c>
+      <c r="S19" s="3">
+        <v>17.238095238095241</v>
+      </c>
+      <c r="T19" s="3">
+        <v>17.982142857142861</v>
+      </c>
+      <c r="U19" s="3">
+        <v>18.609939479239976</v>
+      </c>
+    </row>
+    <row r="20" spans="3:21">
+      <c r="L20" s="7">
+        <f t="shared" si="1"/>
+        <v>3.75</v>
+      </c>
+      <c r="M20" s="3">
+        <v>14.15625</v>
+      </c>
+      <c r="N20" s="3">
+        <v>14.133333333333333</v>
+      </c>
+      <c r="O20" s="3">
+        <v>14.738888888888889</v>
+      </c>
+      <c r="P20" s="3">
+        <v>15.4</v>
+      </c>
+      <c r="Q20" s="3">
+        <v>16.116666666666667</v>
+      </c>
+      <c r="R20" s="3">
+        <v>16.888888888888893</v>
+      </c>
+      <c r="S20" s="3">
+        <v>17.716666666666665</v>
+      </c>
+      <c r="T20" s="3">
+        <v>18.466666666666672</v>
+      </c>
+      <c r="U20" s="3">
+        <v>19.108165736179537</v>
+      </c>
+    </row>
+    <row r="21" spans="3:21">
+      <c r="L21" s="7">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="M21" s="3">
+        <v>14</v>
+      </c>
+      <c r="N21" s="3">
+        <v>14.567708333333334</v>
+      </c>
+      <c r="O21" s="3">
+        <v>15.1875</v>
+      </c>
+      <c r="P21" s="3">
+        <v>15.859375</v>
+      </c>
+      <c r="Q21" s="3">
+        <v>16.583333333333336</v>
+      </c>
+      <c r="R21" s="3">
+        <v>17.359375</v>
+      </c>
+      <c r="S21" s="3">
+        <v>18.1875</v>
+      </c>
+      <c r="T21" s="3">
+        <v>18.942708333333339</v>
+      </c>
+      <c r="U21" s="3">
+        <v>19.596197044334978</v>
+      </c>
+    </row>
+    <row r="22" spans="3:21">
+      <c r="L22" s="7">
+        <f t="shared" si="1"/>
+        <v>4.25</v>
+      </c>
+      <c r="M22" s="3">
+        <v>14.416666666666668</v>
+      </c>
+      <c r="N22" s="3">
+        <v>15</v>
+      </c>
+      <c r="O22" s="3">
+        <v>15.632352941176471</v>
+      </c>
+      <c r="P22" s="3">
+        <v>16.313725490196081</v>
+      </c>
+      <c r="Q22" s="3">
+        <v>17.044117647058822</v>
+      </c>
+      <c r="R22" s="3">
+        <v>17.823529411764707</v>
+      </c>
+      <c r="S22" s="3">
+        <v>18.651960784313729</v>
+      </c>
+      <c r="T22" s="3">
+        <v>19.411764705882355</v>
+      </c>
+      <c r="U22" s="3">
+        <v>20.075832512315273</v>
+      </c>
+    </row>
+    <row r="23" spans="3:21">
+      <c r="L23" s="7">
+        <f t="shared" si="1"/>
+        <v>4.5</v>
+      </c>
+      <c r="M23" s="3">
+        <v>14.833333333333334</v>
+      </c>
+      <c r="N23" s="3">
+        <v>15.430555555555555</v>
+      </c>
+      <c r="O23" s="3">
+        <v>16.074074074074076</v>
+      </c>
+      <c r="P23" s="3">
+        <v>16.763888888888889</v>
+      </c>
+      <c r="Q23" s="3">
+        <v>17.5</v>
+      </c>
+      <c r="R23" s="3">
+        <v>18.282407407407408</v>
+      </c>
+      <c r="S23" s="3">
+        <v>19.111111111111111</v>
+      </c>
+      <c r="T23" s="3">
+        <v>19.875000000000004</v>
+      </c>
+      <c r="U23" s="3">
+        <v>20.548471446816279</v>
+      </c>
+    </row>
+    <row r="24" spans="3:21">
+      <c r="L24" s="7">
+        <f t="shared" si="1"/>
+        <v>4.75</v>
+      </c>
+      <c r="M24" s="3">
+        <v>15.25</v>
+      </c>
+      <c r="N24" s="3">
+        <v>15.859649122807019</v>
+      </c>
+      <c r="O24" s="3">
+        <v>16.513157894736842</v>
+      </c>
+      <c r="P24" s="3">
+        <v>17.210526315789473</v>
+      </c>
+      <c r="Q24" s="3">
+        <v>17.951754385964914</v>
+      </c>
+      <c r="R24" s="3">
+        <v>18.736842105263158</v>
+      </c>
+      <c r="S24" s="3">
+        <v>19.565789473684209</v>
+      </c>
+      <c r="T24" s="3">
+        <v>20.333333333333339</v>
+      </c>
+      <c r="U24" s="3">
+        <v>21.015218563650503</v>
+      </c>
+    </row>
+    <row r="25" spans="3:21">
+      <c r="L25" s="7">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="M25" s="3">
+        <v>15.666666666666668</v>
+      </c>
+      <c r="N25" s="3">
+        <v>16.287500000000001</v>
+      </c>
+      <c r="O25" s="3">
+        <v>16.95</v>
+      </c>
+      <c r="P25" s="3">
+        <v>17.654166666666669</v>
+      </c>
+      <c r="Q25" s="3">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="R25" s="3">
+        <v>19.1875</v>
+      </c>
+      <c r="S25" s="3">
+        <v>20.016666666666669</v>
+      </c>
+      <c r="T25" s="3">
+        <v>20.787500000000001</v>
+      </c>
+      <c r="U25" s="3">
+        <v>21.476957635467983</v>
+      </c>
+    </row>
+    <row r="26" spans="3:21">
+      <c r="L26" s="7">
+        <f t="shared" si="1"/>
+        <v>5.25</v>
+      </c>
+      <c r="M26" s="3">
+        <v>16.083333333333332</v>
+      </c>
+      <c r="N26" s="3">
+        <v>16.714285714285715</v>
+      </c>
+      <c r="O26" s="3">
+        <v>17.384920634920636</v>
+      </c>
+      <c r="P26" s="3">
+        <v>18.095238095238095</v>
+      </c>
+      <c r="Q26" s="3">
+        <v>18.845238095238095</v>
+      </c>
+      <c r="R26" s="3">
+        <v>19.634920634920636</v>
+      </c>
+      <c r="S26" s="3">
+        <v>20.464285714285712</v>
+      </c>
+      <c r="T26" s="3">
+        <v>21.238095238095241</v>
+      </c>
+      <c r="U26" s="3">
+        <v>21.359007271874269</v>
+      </c>
+    </row>
+    <row r="27" spans="3:21">
+      <c r="L27" s="7">
+        <f t="shared" si="1"/>
+        <v>5.5</v>
+      </c>
+      <c r="M27" s="3">
+        <v>16.5</v>
+      </c>
+      <c r="N27" s="3">
+        <v>17.140151515151516</v>
+      </c>
+      <c r="O27" s="3">
+        <v>17.818181818181817</v>
+      </c>
+      <c r="P27" s="3">
+        <v>18.53409090909091</v>
+      </c>
+      <c r="Q27" s="3">
+        <v>19.287878787878789</v>
+      </c>
+      <c r="R27" s="3">
+        <v>20.079545454545453</v>
+      </c>
+      <c r="S27" s="3">
+        <v>20.90909090909091</v>
+      </c>
+      <c r="T27" s="3">
+        <v>21.13636363636364</v>
+      </c>
+      <c r="U27" s="3">
+        <v>21.251779668607256</v>
+      </c>
+    </row>
+    <row r="28" spans="3:21">
+      <c r="L28" s="7">
+        <f t="shared" si="1"/>
+        <v>5.75</v>
+      </c>
+      <c r="M28" s="3">
+        <v>16.916666666666668</v>
+      </c>
+      <c r="N28" s="3">
+        <v>17.565217391304348</v>
+      </c>
+      <c r="O28" s="3">
+        <v>18.25</v>
+      </c>
+      <c r="P28" s="3">
+        <v>18.971014492753625</v>
+      </c>
+      <c r="Q28" s="3">
+        <v>19.728260869565215</v>
+      </c>
+      <c r="R28" s="3">
+        <v>20.521739130434781</v>
+      </c>
+      <c r="S28" s="3">
+        <v>20.826086956521738</v>
+      </c>
+      <c r="T28" s="3">
+        <v>21.043478260869566</v>
+      </c>
+      <c r="U28" s="3">
+        <v>21.153876204754766</v>
+      </c>
+    </row>
+    <row r="29" spans="3:21">
+      <c r="L29" s="7">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="M29" s="3">
+        <v>17.333333333333332</v>
+      </c>
+      <c r="N29" s="3">
+        <v>17.989583333333332</v>
+      </c>
+      <c r="O29" s="3">
+        <v>18.680555555555557</v>
+      </c>
+      <c r="P29" s="3">
+        <v>19.406249999999996</v>
+      </c>
+      <c r="Q29" s="3">
+        <v>20.166666666666668</v>
+      </c>
+      <c r="R29" s="3">
+        <v>20.458333333333332</v>
+      </c>
+      <c r="S29" s="3">
+        <v>20.75</v>
+      </c>
+      <c r="T29" s="3">
+        <v>20.958333333333336</v>
+      </c>
+      <c r="U29" s="3">
+        <v>21.064131362889984</v>
+      </c>
+    </row>
+    <row r="30" spans="3:21">
+      <c r="L30" s="7">
+        <f t="shared" si="1"/>
+        <v>6.25</v>
+      </c>
+      <c r="M30" s="3">
+        <v>17.75</v>
+      </c>
+      <c r="N30" s="3">
+        <v>18.413333333333334</v>
+      </c>
+      <c r="O30" s="3">
+        <v>19.11</v>
+      </c>
+      <c r="P30" s="3">
+        <v>19.84</v>
+      </c>
+      <c r="Q30" s="3">
+        <v>20.12</v>
+      </c>
+      <c r="R30" s="3">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="S30" s="3">
+        <v>20.68</v>
+      </c>
+      <c r="T30" s="3">
+        <v>20.88</v>
+      </c>
+      <c r="U30" s="3">
+        <v>20.981566108374388</v>
+      </c>
+    </row>
+    <row r="31" spans="3:21">
+      <c r="L31" s="7">
+        <f t="shared" si="1"/>
+        <v>6.5</v>
+      </c>
+      <c r="M31" s="3">
+        <v>18.166666666666668</v>
+      </c>
+      <c r="N31" s="3">
+        <v>18.83653846153846</v>
+      </c>
+      <c r="O31" s="3">
+        <v>19.53846153846154</v>
+      </c>
+      <c r="P31" s="3">
+        <v>19.807692307692307</v>
+      </c>
+      <c r="Q31" s="3">
+        <v>20.076923076923077</v>
+      </c>
+      <c r="R31" s="3">
+        <v>20.346153846153847</v>
+      </c>
+      <c r="S31" s="3">
+        <v>20.615384615384617</v>
+      </c>
+      <c r="T31" s="3">
+        <v>20.807692307692307</v>
+      </c>
+      <c r="U31" s="3">
+        <v>20.905352027283065</v>
+      </c>
+    </row>
+    <row r="32" spans="3:21">
+      <c r="L32" s="7">
+        <f t="shared" si="1"/>
+        <v>6.75</v>
+      </c>
+      <c r="M32" s="3">
+        <v>18.583333333333332</v>
+      </c>
+      <c r="N32" s="3">
+        <v>19.25925925925926</v>
+      </c>
+      <c r="O32" s="3">
+        <v>19.518518518518519</v>
+      </c>
+      <c r="P32" s="3">
+        <v>19.777777777777779</v>
+      </c>
+      <c r="Q32" s="3">
+        <v>20.037037037037038</v>
+      </c>
+      <c r="R32" s="3">
+        <v>20.296296296296298</v>
+      </c>
+      <c r="S32" s="3">
+        <v>20.555555555555557</v>
+      </c>
+      <c r="T32" s="3">
+        <v>20.74074074074074</v>
+      </c>
+      <c r="U32" s="3">
+        <v>20.834783433679988</v>
+      </c>
+    </row>
+    <row r="33" spans="12:21">
+      <c r="L33" s="7">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="M33" s="3">
+        <v>19</v>
+      </c>
+      <c r="N33" s="3">
+        <v>19.25</v>
+      </c>
+      <c r="O33" s="3">
+        <v>19.5</v>
+      </c>
+      <c r="P33" s="3">
+        <v>19.75</v>
+      </c>
+      <c r="Q33" s="3">
+        <v>20</v>
+      </c>
+      <c r="R33" s="3">
+        <v>20.25</v>
+      </c>
+      <c r="S33" s="3">
+        <v>20.5</v>
+      </c>
+      <c r="T33" s="3">
+        <v>20.678571428571427</v>
+      </c>
+      <c r="U33" s="3">
+        <v>20.769255453905703</v>
+      </c>
+    </row>
+    <row r="34" spans="12:21">
+      <c r="L34" s="7">
+        <f t="shared" si="1"/>
+        <v>7.25</v>
+      </c>
+      <c r="M34" s="3">
+        <v>19</v>
+      </c>
+      <c r="N34" s="3">
+        <v>19.241379310344829</v>
+      </c>
+      <c r="O34" s="3">
+        <v>19.482758620689655</v>
+      </c>
+      <c r="P34" s="3">
+        <v>19.724137931034484</v>
+      </c>
+      <c r="Q34" s="3">
+        <v>19.96551724137931</v>
+      </c>
+      <c r="R34" s="3">
+        <v>20.206896551724139</v>
+      </c>
+      <c r="S34" s="3">
+        <v>20.448275862068964</v>
+      </c>
+      <c r="T34" s="3">
+        <v>20.620689655172413</v>
+      </c>
+      <c r="U34" s="3">
+        <v>20.708246645150332</v>
+      </c>
+    </row>
+    <row r="35" spans="12:21">
+      <c r="L35" s="7">
+        <f t="shared" si="1"/>
+        <v>7.5</v>
+      </c>
+      <c r="M35" s="3">
+        <v>19</v>
+      </c>
+      <c r="N35" s="3">
+        <v>19.233333333333334</v>
+      </c>
+      <c r="O35" s="3">
+        <v>19.466666666666665</v>
+      </c>
+      <c r="P35" s="3">
+        <v>19.7</v>
+      </c>
+      <c r="Q35" s="3">
+        <v>19.933333333333334</v>
+      </c>
+      <c r="R35" s="3">
+        <v>20.166666666666668</v>
+      </c>
+      <c r="S35" s="3">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="T35" s="3">
+        <v>20.566666666666666</v>
+      </c>
+      <c r="U35" s="3">
+        <v>20.65130509031199</v>
+      </c>
+    </row>
+    <row r="36" spans="12:21">
+      <c r="L36" s="7">
+        <f t="shared" si="1"/>
+        <v>7.75</v>
+      </c>
+      <c r="M36" s="3">
+        <v>19</v>
+      </c>
+      <c r="N36" s="3">
+        <v>19.225806451612904</v>
+      </c>
+      <c r="O36" s="3">
+        <v>19.451612903225808</v>
+      </c>
+      <c r="P36" s="3">
+        <v>19.677419354838708</v>
+      </c>
+      <c r="Q36" s="3">
+        <v>19.903225806451612</v>
+      </c>
+      <c r="R36" s="3">
+        <v>20.129032258064516</v>
+      </c>
+      <c r="S36" s="3">
+        <v>20.35483870967742</v>
+      </c>
+      <c r="T36" s="3">
+        <v>20.516129032258064</v>
+      </c>
+      <c r="U36" s="3">
+        <v>20.598037184172892</v>
+      </c>
+    </row>
+    <row r="37" spans="12:21">
+      <c r="L37" s="7">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="M37" s="3">
+        <v>19</v>
+      </c>
+      <c r="N37" s="3">
+        <v>19.21875</v>
+      </c>
+      <c r="O37" s="3">
+        <v>19.4375</v>
+      </c>
+      <c r="P37" s="3">
+        <v>19.65625</v>
+      </c>
+      <c r="Q37" s="3">
+        <v>19.875</v>
+      </c>
+      <c r="R37" s="3">
+        <v>20.09375</v>
+      </c>
+      <c r="S37" s="3">
+        <v>20.3125</v>
+      </c>
+      <c r="T37" s="3">
+        <v>20.46875</v>
+      </c>
+      <c r="U37" s="3">
+        <v>20.548098522167489</v>
+      </c>
+    </row>
+    <row r="38" spans="12:21">
+      <c r="L38" s="7">
+        <f t="shared" si="1"/>
+        <v>8.25</v>
+      </c>
+      <c r="M38" s="3">
+        <v>19</v>
+      </c>
+      <c r="N38" s="3">
+        <v>19.212121212121211</v>
+      </c>
+      <c r="O38" s="3">
+        <v>19.424242424242426</v>
+      </c>
+      <c r="P38" s="3">
+        <v>19.636363636363637</v>
+      </c>
+      <c r="Q38" s="3">
+        <v>19.848484848484848</v>
+      </c>
+      <c r="R38" s="3">
+        <v>20.060606060606062</v>
+      </c>
+      <c r="S38" s="3">
+        <v>20.272727272727273</v>
+      </c>
+      <c r="T38" s="3">
+        <v>20.424242424242426</v>
+      </c>
+      <c r="U38" s="3">
+        <v>20.501186445738171</v>
+      </c>
+    </row>
+    <row r="39" spans="12:21">
+      <c r="L39" s="7">
+        <f t="shared" si="1"/>
+        <v>8.5</v>
+      </c>
+      <c r="M39" s="3">
+        <v>19</v>
+      </c>
+      <c r="N39" s="3">
+        <v>19.205882352941178</v>
+      </c>
+      <c r="O39" s="3">
+        <v>19.411764705882351</v>
+      </c>
+      <c r="P39" s="3">
+        <v>19.617647058823529</v>
+      </c>
+      <c r="Q39" s="3">
+        <v>19.823529411764707</v>
+      </c>
+      <c r="R39" s="3">
+        <v>20.029411764705884</v>
+      </c>
+      <c r="S39" s="3">
+        <v>20.235294117647058</v>
+      </c>
+      <c r="T39" s="3">
+        <v>20.382352941176471</v>
+      </c>
+      <c r="U39" s="3">
+        <v>20.457033903216459</v>
+      </c>
+    </row>
+    <row r="40" spans="12:21">
+      <c r="L40" s="7">
+        <f t="shared" si="1"/>
+        <v>8.75</v>
+      </c>
+      <c r="M40" s="3">
+        <v>19</v>
+      </c>
+      <c r="N40" s="3">
+        <v>19.2</v>
+      </c>
+      <c r="O40" s="3">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="P40" s="3">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="Q40" s="3">
+        <v>19.8</v>
+      </c>
+      <c r="R40" s="3">
+        <v>20</v>
+      </c>
+      <c r="S40" s="3">
+        <v>20.2</v>
+      </c>
+      <c r="T40" s="3">
+        <v>20.342857142857142</v>
+      </c>
+      <c r="U40" s="3">
+        <v>20.415404363124562</v>
+      </c>
+    </row>
+    <row r="41" spans="12:21">
+      <c r="L41" s="7">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="M41" s="3">
+        <v>19</v>
+      </c>
+      <c r="N41" s="3">
+        <v>19.194444444444443</v>
+      </c>
+      <c r="O41" s="3">
+        <v>19.388888888888889</v>
+      </c>
+      <c r="P41" s="3">
+        <v>19.583333333333332</v>
+      </c>
+      <c r="Q41" s="3">
+        <v>19.777777777777779</v>
+      </c>
+      <c r="R41" s="3">
+        <v>19.972222222222221</v>
+      </c>
+      <c r="S41" s="3">
+        <v>20.166666666666668</v>
+      </c>
+      <c r="T41" s="3">
+        <v>20.305555555555557</v>
+      </c>
+      <c r="U41" s="3">
+        <v>20.376087575259991</v>
+      </c>
+    </row>
+    <row r="42" spans="12:21">
+      <c r="L42" s="7">
+        <f t="shared" si="1"/>
+        <v>9.25</v>
+      </c>
+      <c r="M42" s="3">
+        <v>19</v>
+      </c>
+      <c r="N42" s="3">
+        <v>19.189189189189189</v>
+      </c>
+      <c r="O42" s="3">
+        <v>19.378378378378379</v>
+      </c>
+      <c r="P42" s="3">
+        <v>19.567567567567568</v>
+      </c>
+      <c r="Q42" s="3">
+        <v>19.756756756756758</v>
+      </c>
+      <c r="R42" s="3">
+        <v>19.945945945945947</v>
+      </c>
+      <c r="S42" s="3">
+        <v>20.135135135135137</v>
+      </c>
+      <c r="T42" s="3">
+        <v>20.27027027027027</v>
+      </c>
+      <c r="U42" s="3">
+        <v>20.338896019171884</v>
+      </c>
+    </row>
+    <row r="43" spans="12:21">
+      <c r="L43" s="7">
+        <f t="shared" si="1"/>
+        <v>9.5</v>
+      </c>
+      <c r="M43" s="3">
+        <v>19</v>
+      </c>
+      <c r="N43" s="3">
+        <v>19.184210526315791</v>
+      </c>
+      <c r="O43" s="3">
+        <v>19.368421052631579</v>
+      </c>
+      <c r="P43" s="3">
+        <v>19.55263157894737</v>
+      </c>
+      <c r="Q43" s="3">
+        <v>19.736842105263158</v>
+      </c>
+      <c r="R43" s="3">
+        <v>19.921052631578949</v>
+      </c>
+      <c r="S43" s="3">
+        <v>20.105263157894736</v>
+      </c>
+      <c r="T43" s="3">
+        <v>20.236842105263158</v>
+      </c>
+      <c r="U43" s="3">
+        <v>20.303661913404202</v>
+      </c>
+    </row>
+    <row r="44" spans="12:21">
+      <c r="L44" s="7">
+        <f>L43+0.25</f>
+        <v>9.75</v>
+      </c>
+      <c r="M44" s="3">
+        <v>19</v>
+      </c>
+      <c r="N44" s="3">
+        <v>19.179487179487179</v>
+      </c>
+      <c r="O44" s="3">
+        <v>19.358974358974358</v>
+      </c>
+      <c r="P44" s="3">
+        <v>19.53846153846154</v>
+      </c>
+      <c r="Q44" s="3">
+        <v>19.717948717948719</v>
+      </c>
+      <c r="R44" s="3">
+        <v>19.897435897435898</v>
+      </c>
+      <c r="S44" s="3">
+        <v>20.076923076923077</v>
+      </c>
+      <c r="T44" s="3">
+        <v>20.205128205128204</v>
+      </c>
+      <c r="U44" s="3">
+        <v>20.270234684855374</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="F4:H4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Changed excel fwds to use length
</commit_message>
<xml_diff>
--- a/InterpolationExamples.xlsx
+++ b/InterpolationExamples.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
   <si>
     <t>Length (Years)</t>
   </si>
@@ -42,9 +42,6 @@
   </si>
   <si>
     <t>Start</t>
-  </si>
-  <si>
-    <t>End</t>
   </si>
   <si>
     <t>Alpha</t>
@@ -2104,7 +2101,7 @@
   <dimension ref="C4:U44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2146,7 +2143,7 @@
         <v>8</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H5" s="17" t="s">
         <v>3</v>
@@ -2192,16 +2189,16 @@
         <v>0.25</v>
       </c>
       <c r="D6" s="11">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6" s="18">
         <v>0.75</v>
       </c>
       <c r="G6" s="19">
-        <v>1.75</v>
+        <v>1</v>
       </c>
       <c r="H6" s="11">
-        <v>12.5</v>
+        <v>13</v>
       </c>
       <c r="K6" s="4" t="s">
         <v>0</v>
@@ -2211,31 +2208,31 @@
       </c>
       <c r="M6" s="3">
         <f t="array" ref="M6:U44">FS("Kalahari.splineSurfaceWithForwardPointsAdded", C6:C14,D6:D14,F6:H15,D18,M5:U5,L6:L44)</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="N6" s="3">
-        <v>12</v>
+        <v>11.419055276957838</v>
       </c>
       <c r="O6" s="3">
-        <v>12</v>
+        <v>11.805517638530336</v>
       </c>
       <c r="P6" s="3">
-        <v>12</v>
+        <v>12.103032475607165</v>
       </c>
       <c r="Q6" s="3">
-        <v>12</v>
+        <v>12.483789404025366</v>
       </c>
       <c r="R6" s="3">
-        <v>12</v>
+        <v>13.188605204879323</v>
       </c>
       <c r="S6" s="3">
-        <v>13.999999999999943</v>
+        <v>14.224572915488153</v>
       </c>
       <c r="T6" s="3">
-        <v>16.46084729064043</v>
+        <v>16.592971485111818</v>
       </c>
       <c r="U6" s="3">
-        <v>19.135448275862018</v>
+        <v>19.126250767669092</v>
       </c>
     </row>
     <row r="7" spans="3:21">
@@ -2243,40 +2240,46 @@
         <v>1</v>
       </c>
       <c r="D7" s="11"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="11"/>
+      <c r="F7" s="18">
+        <v>1.25</v>
+      </c>
+      <c r="G7" s="19">
+        <v>4.75</v>
+      </c>
+      <c r="H7" s="11">
+        <v>19</v>
+      </c>
       <c r="K7" s="4"/>
       <c r="L7" s="7">
         <f>L6+0.25</f>
         <v>0.5</v>
       </c>
       <c r="M7" s="3">
-        <v>12</v>
+        <v>11.209527638478919</v>
       </c>
       <c r="N7" s="3">
-        <v>12</v>
+        <v>11.612286457744087</v>
       </c>
       <c r="O7" s="3">
-        <v>12</v>
+        <v>11.954275057068751</v>
       </c>
       <c r="P7" s="3">
-        <v>12</v>
+        <v>12.293410939816265</v>
       </c>
       <c r="Q7" s="3">
-        <v>12</v>
+        <v>12.836197304452345</v>
       </c>
       <c r="R7" s="3">
-        <v>12.999999999999972</v>
+        <v>13.706589060183738</v>
       </c>
       <c r="S7" s="3">
-        <v>15.230423645320187</v>
+        <v>15.408772200299985</v>
       </c>
       <c r="T7" s="3">
-        <v>17.798147783251224</v>
+        <v>17.859611126390455</v>
       </c>
       <c r="U7" s="3">
-        <v>19.890955665024634</v>
+        <v>19.828477928226768</v>
       </c>
     </row>
     <row r="8" spans="3:21">
@@ -2295,31 +2298,31 @@
         <v>0.75</v>
       </c>
       <c r="M8" s="3">
-        <v>12</v>
+        <v>11.408190971829391</v>
       </c>
       <c r="N8" s="3">
-        <v>12</v>
+        <v>11.775868463698446</v>
       </c>
       <c r="O8" s="3">
-        <v>12</v>
+        <v>12.130779839387623</v>
       </c>
       <c r="P8" s="3">
-        <v>12</v>
+        <v>12.591809028170617</v>
       </c>
       <c r="Q8" s="3">
-        <v>12.666666666666648</v>
+        <v>13.298989174797613</v>
       </c>
       <c r="R8" s="3">
-        <v>14.153615763546791</v>
+        <v>14.668716535159765</v>
       </c>
       <c r="S8" s="3">
-        <v>16.532098522167463</v>
+        <v>16.647931722756354</v>
       </c>
       <c r="T8" s="3">
-        <v>18.747586206896568</v>
+        <v>18.749975780521783</v>
       </c>
       <c r="U8" s="3">
-        <v>20.030975369458105</v>
+        <v>19.938831864823666</v>
       </c>
     </row>
     <row r="9" spans="3:21">
@@ -2336,31 +2339,31 @@
         <v>1</v>
       </c>
       <c r="M9" s="3">
-        <v>12</v>
+        <v>11.581901347773835</v>
       </c>
       <c r="N9" s="3">
-        <v>12</v>
+        <v>11.952848698780176</v>
       </c>
       <c r="O9" s="3">
-        <v>12</v>
+        <v>12.395236180760548</v>
       </c>
       <c r="P9" s="3">
-        <v>12.499999999999986</v>
+        <v>13.000000000000002</v>
       </c>
       <c r="Q9" s="3">
-        <v>13.615211822660093</v>
+        <v>14.122484752376165</v>
       </c>
       <c r="R9" s="3">
-        <v>15.399073891625598</v>
+        <v>15.783100093287096</v>
       </c>
       <c r="S9" s="3">
-        <v>17.560689655172411</v>
+        <v>17.618625064263377</v>
       </c>
       <c r="T9" s="3">
-        <v>19.138443349753686</v>
+        <v>19.102366769895703</v>
       </c>
       <c r="U9" s="3">
-        <v>19.384788177339928</v>
+        <v>19.295613899849958</v>
       </c>
     </row>
     <row r="10" spans="3:21">
@@ -2379,31 +2382,31 @@
         <v>1.25</v>
       </c>
       <c r="M10" s="3">
-        <v>12</v>
+        <v>11.76227895902414</v>
       </c>
       <c r="N10" s="3">
-        <v>12</v>
+        <v>12.200000000000006</v>
       </c>
       <c r="O10" s="3">
-        <v>12.399999999999988</v>
+        <v>12.761103527706069</v>
       </c>
       <c r="P10" s="3">
-        <v>13.292169458128075</v>
+        <v>13.718594297022367</v>
       </c>
       <c r="Q10" s="3">
-        <v>14.719259113300478</v>
+        <v>15.123237955434751</v>
       </c>
       <c r="R10" s="3">
-        <v>16.448551724137928</v>
+        <v>16.732621092386566</v>
       </c>
       <c r="S10" s="3">
-        <v>18.110754679802938</v>
+        <v>18.126807999014193</v>
       </c>
       <c r="T10" s="3">
-        <v>18.800000000000029</v>
+        <v>18.755085416902329</v>
       </c>
       <c r="U10" s="3">
-        <v>18.101580541871925</v>
+        <v>18.030241119879999</v>
       </c>
     </row>
     <row r="11" spans="3:21">
@@ -2422,31 +2425,31 @@
         <v>1.5</v>
       </c>
       <c r="M11" s="3">
-        <v>12</v>
+        <v>12.000000000000005</v>
       </c>
       <c r="N11" s="3">
-        <v>12.333333333333323</v>
+        <v>12.53742881924803</v>
       </c>
       <c r="O11" s="3">
-        <v>13.076807881773396</v>
+        <v>13.399748187273694</v>
       </c>
       <c r="P11" s="3">
-        <v>14.266049261083731</v>
+        <v>14.619870375463487</v>
       </c>
       <c r="Q11" s="3">
-        <v>15.707126436781607</v>
+        <v>16.024482477659699</v>
       </c>
       <c r="R11" s="3">
-        <v>17.092295566502447</v>
+        <v>17.303774199991715</v>
       </c>
       <c r="S11" s="3">
-        <v>18.000000000000014</v>
+        <v>17.999999999999968</v>
       </c>
       <c r="T11" s="3">
-        <v>17.828125000000011</v>
+        <v>17.790696180751969</v>
       </c>
       <c r="U11" s="3">
-        <v>16.756525451559938</v>
+        <v>16.697075933233332</v>
       </c>
     </row>
     <row r="12" spans="3:21">
@@ -2463,31 +2466,31 @@
         <v>1.75</v>
       </c>
       <c r="M12" s="3">
-        <v>12.285714285714278</v>
+        <v>12.317796130784027</v>
       </c>
       <c r="N12" s="3">
-        <v>12.922978184377197</v>
+        <v>13.116792057228571</v>
       </c>
       <c r="O12" s="3">
-        <v>13.94232793807177</v>
+        <v>14.217819984473037</v>
       </c>
       <c r="P12" s="3">
-        <v>15.177536945812806</v>
+        <v>15.464275334509336</v>
       </c>
       <c r="Q12" s="3">
-        <v>16.364824771287811</v>
+        <v>16.615204943425091</v>
       </c>
       <c r="R12" s="3">
-        <v>17.142857142857157</v>
+        <v>17.312657886411305</v>
       </c>
       <c r="S12" s="3">
-        <v>17.28125</v>
+        <v>17.281249999999996</v>
       </c>
       <c r="T12" s="3">
-        <v>16.714285714285722</v>
+        <v>16.682203869215975</v>
       </c>
       <c r="U12" s="3">
-        <v>15.697557529908519</v>
+        <v>15.646600799914285</v>
       </c>
     </row>
     <row r="13" spans="3:21">
@@ -2506,31 +2509,31 @@
         <v>2</v>
       </c>
       <c r="M13" s="3">
-        <v>12.807605911330047</v>
+        <v>12.852193050075</v>
       </c>
       <c r="N13" s="3">
-        <v>13.699536945812799</v>
+        <v>13.867974396033636</v>
       </c>
       <c r="O13" s="3">
-        <v>14.780344827586205</v>
+        <v>15.006930622511963</v>
       </c>
       <c r="P13" s="3">
-        <v>15.819221674876836</v>
+        <v>16.051183384947851</v>
       </c>
       <c r="Q13" s="3">
-        <v>16.500000000000011</v>
+        <v>16.70904932611306</v>
       </c>
       <c r="R13" s="3">
-        <v>16.62109375</v>
+        <v>16.769669400609914</v>
       </c>
       <c r="S13" s="3">
-        <v>16.375</v>
+        <v>16.374999999999996</v>
       </c>
       <c r="T13" s="3">
-        <v>15.792968750000007</v>
+        <v>15.764897135563977</v>
       </c>
       <c r="U13" s="3">
-        <v>15.192394088669953</v>
+        <v>15.147806949925</v>
       </c>
     </row>
     <row r="14" spans="3:21">
@@ -2547,31 +2550,31 @@
         <v>2.25</v>
       </c>
       <c r="M14" s="3">
-        <v>13.510699507389155</v>
+        <v>13.549310574252122</v>
       </c>
       <c r="N14" s="3">
-        <v>14.471417624521072</v>
+        <v>14.608277806339281</v>
       </c>
       <c r="O14" s="3">
-        <v>15.394863711001632</v>
+        <v>15.579442746457017</v>
       </c>
       <c r="P14" s="3">
-        <v>16.000000000000011</v>
+        <v>16.197269676056848</v>
       </c>
       <c r="Q14" s="3">
-        <v>16.107638888888889</v>
+        <v>16.293460512100516</v>
       </c>
       <c r="R14" s="3">
-        <v>15.888888888888889</v>
+        <v>16.02095613387548</v>
       </c>
       <c r="S14" s="3">
-        <v>15.59375</v>
+        <v>15.593749999999996</v>
       </c>
       <c r="T14" s="3">
-        <v>15.333333333333339</v>
+        <v>15.30838078716798</v>
       </c>
       <c r="U14" s="3">
-        <v>15.846942893632551</v>
+        <v>15.303706199895171</v>
       </c>
     </row>
     <row r="15" spans="3:21">
@@ -2583,31 +2586,31 @@
         <v>2.5</v>
       </c>
       <c r="M15" s="3">
-        <v>14.224275862068964</v>
+        <v>14.247450025705353</v>
       </c>
       <c r="N15" s="3">
-        <v>15.055377339901469</v>
+        <v>15.1634039995071</v>
       </c>
       <c r="O15" s="3">
-        <v>15.600000000000009</v>
+        <v>15.758094472304199</v>
       </c>
       <c r="P15" s="3">
-        <v>15.696875</v>
+        <v>15.874417708451181</v>
       </c>
       <c r="Q15" s="3">
-        <v>15.5</v>
+        <v>15.667239460890466</v>
       </c>
       <c r="R15" s="3">
-        <v>15.234375</v>
+        <v>15.353235520487932</v>
       </c>
       <c r="S15" s="3">
-        <v>15.2</v>
+        <v>15.199999999999998</v>
       </c>
       <c r="T15" s="3">
-        <v>15.90833333333334</v>
+        <v>15.432632728416838</v>
       </c>
       <c r="U15" s="3">
-        <v>16.453915270935962</v>
+        <v>15.900410342695267</v>
       </c>
     </row>
     <row r="16" spans="3:21">
@@ -2616,31 +2619,31 @@
         <v>2.75</v>
       </c>
       <c r="M16" s="3">
-        <v>14.777615763546789</v>
+        <v>14.784912726824636</v>
       </c>
       <c r="N16" s="3">
-        <v>15.27272727272728</v>
+        <v>15.363636363636347</v>
       </c>
       <c r="O16" s="3">
-        <v>15.360795454545455</v>
+        <v>15.504517702094743</v>
       </c>
       <c r="P16" s="3">
-        <v>15.181818181818182</v>
+        <v>15.343220644046529</v>
       </c>
       <c r="Q16" s="3">
-        <v>14.940340909090908</v>
+        <v>15.092376782627696</v>
       </c>
       <c r="R16" s="3">
-        <v>14.909090909090908</v>
+        <v>15.017145927716301</v>
       </c>
       <c r="S16" s="3">
-        <v>15.734848484848486</v>
+        <v>15.322809109059683</v>
       </c>
       <c r="T16" s="3">
-        <v>16.45454545454546</v>
+        <v>15.963370446551318</v>
       </c>
       <c r="U16" s="3">
-        <v>17.026286609941785</v>
+        <v>16.743293439163139</v>
       </c>
     </row>
     <row r="17" spans="3:21">
@@ -2649,36 +2652,36 @@
         <v>3</v>
       </c>
       <c r="M17" s="3">
-        <v>15.000000000000007</v>
+        <v>14.999999999999986</v>
       </c>
       <c r="N17" s="3">
-        <v>15.080729166666666</v>
+        <v>15.1640625</v>
       </c>
       <c r="O17" s="3">
-        <v>14.916666666666666</v>
+        <v>15.048412060253513</v>
       </c>
       <c r="P17" s="3">
-        <v>14.6953125</v>
+        <v>14.843264757042652</v>
       </c>
       <c r="Q17" s="3">
-        <v>14.666666666666666</v>
+        <v>14.806032884075387</v>
       </c>
       <c r="R17" s="3">
-        <v>15.423611111111112</v>
+        <v>15.144958783711322</v>
       </c>
       <c r="S17" s="3">
-        <v>16.25</v>
+        <v>15.818470652296055</v>
       </c>
       <c r="T17" s="3">
-        <v>16.979166666666671</v>
+        <v>16.730766609658861</v>
       </c>
       <c r="U17" s="3">
-        <v>17.572707170224415</v>
+        <v>17.675322508113908</v>
       </c>
     </row>
     <row r="18" spans="3:21">
       <c r="C18" s="17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D18" s="22">
         <v>0.5</v>
@@ -2691,28 +2694,28 @@
         <v>14.84375</v>
       </c>
       <c r="N18" s="3">
-        <v>14.692307692307692</v>
+        <v>14.76923076923077</v>
       </c>
       <c r="O18" s="3">
-        <v>14.48798076923077</v>
+        <v>14.609591901772474</v>
       </c>
       <c r="P18" s="3">
-        <v>14.461538461538462</v>
+        <v>14.598109775731679</v>
       </c>
       <c r="Q18" s="3">
-        <v>15.160256410256411</v>
+        <v>14.940253446812401</v>
       </c>
       <c r="R18" s="3">
-        <v>15.923076923076923</v>
+        <v>15.616173310187076</v>
       </c>
       <c r="S18" s="3">
-        <v>16.75</v>
+        <v>16.537982479338037</v>
       </c>
       <c r="T18" s="3">
-        <v>17.487179487179496</v>
+        <v>17.592064737113748</v>
       </c>
       <c r="U18" s="3">
-        <v>18.099165593027664</v>
+        <v>18.56259869634885</v>
       </c>
     </row>
     <row r="19" spans="3:21">
@@ -2724,28 +2727,28 @@
         <v>14.5</v>
       </c>
       <c r="N19" s="3">
-        <v>14.310267857142858</v>
+        <v>14.381696428571429</v>
       </c>
       <c r="O19" s="3">
-        <v>14.285714285714286</v>
+        <v>14.398638908788726</v>
       </c>
       <c r="P19" s="3">
-        <v>14.93452380952381</v>
+        <v>14.737594806012027</v>
       </c>
       <c r="Q19" s="3">
-        <v>15.642857142857142</v>
+        <v>15.392431602604095</v>
       </c>
       <c r="R19" s="3">
-        <v>16.410714285714285</v>
+        <v>16.298741245448131</v>
       </c>
       <c r="S19" s="3">
-        <v>17.238095238095241</v>
+        <v>17.351529606997634</v>
       </c>
       <c r="T19" s="3">
-        <v>17.982142857142861</v>
+        <v>18.421911038403348</v>
       </c>
       <c r="U19" s="3">
-        <v>18.609939479239976</v>
+        <v>19.286095090089361</v>
       </c>
     </row>
     <row r="20" spans="3:21">
@@ -2757,28 +2760,28 @@
         <v>14.15625</v>
       </c>
       <c r="N20" s="3">
-        <v>14.133333333333333</v>
+        <v>14.2</v>
       </c>
       <c r="O20" s="3">
-        <v>14.738888888888889</v>
+        <v>14.542122994846581</v>
       </c>
       <c r="P20" s="3">
-        <v>15.4</v>
+        <v>15.173138327470967</v>
       </c>
       <c r="Q20" s="3">
-        <v>16.116666666666667</v>
+        <v>16.044411122686611</v>
       </c>
       <c r="R20" s="3">
-        <v>16.888888888888893</v>
+        <v>17.07400131352308</v>
       </c>
       <c r="S20" s="3">
-        <v>17.716666666666665</v>
+        <v>18.142088496875665</v>
       </c>
       <c r="T20" s="3">
-        <v>18.466666666666672</v>
+        <v>19.106553516424192</v>
       </c>
       <c r="U20" s="3">
-        <v>19.108165736179537</v>
+        <v>19.736699401836166</v>
       </c>
     </row>
     <row r="21" spans="3:21">
@@ -2790,28 +2793,28 @@
         <v>14</v>
       </c>
       <c r="N21" s="3">
-        <v>14.567708333333334</v>
+        <v>14.346931262478535</v>
       </c>
       <c r="O21" s="3">
-        <v>15.1875</v>
+        <v>14.962662034412178</v>
       </c>
       <c r="P21" s="3">
-        <v>15.859375</v>
+        <v>15.798074957244147</v>
       </c>
       <c r="Q21" s="3">
-        <v>16.583333333333336</v>
+        <v>16.787113069179473</v>
       </c>
       <c r="R21" s="3">
-        <v>17.359375</v>
+        <v>17.832495791125897</v>
       </c>
       <c r="S21" s="3">
-        <v>18.1875</v>
+        <v>18.801429728865692</v>
       </c>
       <c r="T21" s="3">
-        <v>18.942708333333339</v>
+        <v>19.540216407040894</v>
       </c>
       <c r="U21" s="3">
-        <v>19.596197044334978</v>
+        <v>19.812115649657493</v>
       </c>
     </row>
     <row r="22" spans="3:21">
@@ -2820,31 +2823,31 @@
         <v>4.25</v>
       </c>
       <c r="M22" s="3">
-        <v>14.416666666666668</v>
+        <v>14.150052952920973</v>
       </c>
       <c r="N22" s="3">
-        <v>15</v>
+        <v>14.754214578091334</v>
       </c>
       <c r="O22" s="3">
-        <v>15.632352941176471</v>
+        <v>15.563218644378628</v>
       </c>
       <c r="P22" s="3">
-        <v>16.313725490196081</v>
+        <v>16.511578916616397</v>
       </c>
       <c r="Q22" s="3">
-        <v>17.044117647058822</v>
+        <v>17.517866003649395</v>
       </c>
       <c r="R22" s="3">
-        <v>17.823529411764707</v>
+        <v>18.471263580395906</v>
       </c>
       <c r="S22" s="3">
-        <v>18.651960784313729</v>
+        <v>19.227531495773086</v>
       </c>
       <c r="T22" s="3">
-        <v>19.411764705882355</v>
+        <v>19.62275422821363</v>
       </c>
       <c r="U22" s="3">
-        <v>20.075832512315273</v>
+        <v>20.230006340181649</v>
       </c>
     </row>
     <row r="23" spans="3:21">
@@ -2853,31 +2856,31 @@
         <v>4.5</v>
       </c>
       <c r="M23" s="3">
-        <v>14.833333333333334</v>
+        <v>14.545647101530705</v>
       </c>
       <c r="N23" s="3">
-        <v>15.430555555555555</v>
+        <v>15.332987346188585</v>
       </c>
       <c r="O23" s="3">
-        <v>16.074074074074076</v>
+        <v>16.250131067833834</v>
       </c>
       <c r="P23" s="3">
-        <v>16.763888888888889</v>
+        <v>17.217041918758159</v>
       </c>
       <c r="Q23" s="3">
-        <v>17.5</v>
+        <v>18.138626126153095</v>
       </c>
       <c r="R23" s="3">
-        <v>18.282407407407408</v>
+        <v>18.892035590723435</v>
       </c>
       <c r="S23" s="3">
-        <v>19.111111111111111</v>
+        <v>19.32285526639555</v>
       </c>
       <c r="T23" s="3">
-        <v>19.875000000000004</v>
+        <v>20.027948848233326</v>
       </c>
       <c r="U23" s="3">
-        <v>20.548471446816279</v>
+        <v>20.643349691486499</v>
       </c>
     </row>
     <row r="24" spans="3:21">
@@ -2886,31 +2889,31 @@
         <v>4.75</v>
       </c>
       <c r="M24" s="3">
-        <v>15.25</v>
+        <v>15.104935380599713</v>
       </c>
       <c r="N24" s="3">
-        <v>15.859649122807019</v>
+        <v>15.995863920945627</v>
       </c>
       <c r="O24" s="3">
-        <v>16.513157894736842</v>
+        <v>16.932224851377747</v>
       </c>
       <c r="P24" s="3">
-        <v>17.210526315789473</v>
+        <v>17.820963302440152</v>
       </c>
       <c r="Q24" s="3">
-        <v>17.951754385964914</v>
+        <v>18.554759475634061</v>
       </c>
       <c r="R24" s="3">
-        <v>18.736842105263158</v>
+        <v>18.999999999999957</v>
       </c>
       <c r="S24" s="3">
-        <v>19.565789473684209</v>
+        <v>19.722508009667791</v>
       </c>
       <c r="T24" s="3">
-        <v>20.333333333333339</v>
+        <v>20.430171891150991</v>
       </c>
       <c r="U24" s="3">
-        <v>21.015218563650503</v>
+        <v>21.052863704501455</v>
       </c>
     </row>
     <row r="25" spans="3:21">
@@ -2919,31 +2922,31 @@
         <v>5</v>
       </c>
       <c r="M25" s="3">
-        <v>15.666666666666668</v>
+        <v>15.746070724898345</v>
       </c>
       <c r="N25" s="3">
-        <v>16.287500000000001</v>
+        <v>16.656566372656751</v>
       </c>
       <c r="O25" s="3">
-        <v>16.95</v>
+        <v>17.52019101924466</v>
       </c>
       <c r="P25" s="3">
-        <v>17.654166666666669</v>
+        <v>18.232173125632716</v>
       </c>
       <c r="Q25" s="3">
-        <v>18.399999999999999</v>
+        <v>18.674189470201227</v>
       </c>
       <c r="R25" s="3">
-        <v>19.1875</v>
+        <v>19.395812869428369</v>
       </c>
       <c r="S25" s="3">
-        <v>20.016666666666669</v>
+        <v>20.11989194236785</v>
       </c>
       <c r="T25" s="3">
-        <v>20.787500000000001</v>
+        <v>20.829869093531975</v>
       </c>
       <c r="U25" s="3">
-        <v>21.476957635467983</v>
+        <v>21.459122779969999</v>
       </c>
     </row>
     <row r="26" spans="3:21">
@@ -2952,31 +2955,31 @@
         <v>5.25</v>
       </c>
       <c r="M26" s="3">
-        <v>16.083333333333332</v>
+        <v>16.387206069196907</v>
       </c>
       <c r="N26" s="3">
-        <v>16.714285714285715</v>
+        <v>17.22966074580243</v>
       </c>
       <c r="O26" s="3">
-        <v>17.384920634920636</v>
+        <v>17.926141911961174</v>
       </c>
       <c r="P26" s="3">
-        <v>18.095238095238095</v>
+        <v>18.361277232363413</v>
       </c>
       <c r="Q26" s="3">
-        <v>18.845238095238095</v>
+        <v>19.066668894885368</v>
       </c>
       <c r="R26" s="3">
-        <v>19.634920634920636</v>
+        <v>19.78983066915411</v>
       </c>
       <c r="S26" s="3">
-        <v>20.464285714285712</v>
+        <v>20.515331180291792</v>
       </c>
       <c r="T26" s="3">
-        <v>21.238095238095241</v>
+        <v>21.227401289738658</v>
       </c>
       <c r="U26" s="3">
-        <v>21.359007271874269</v>
+        <v>21.342021695209525</v>
       </c>
     </row>
     <row r="27" spans="3:21">
@@ -2985,31 +2988,31 @@
         <v>5.5</v>
       </c>
       <c r="M27" s="3">
-        <v>16.5</v>
+        <v>16.946494348265958</v>
       </c>
       <c r="N27" s="3">
-        <v>17.140151515151516</v>
+        <v>17.630365246733749</v>
       </c>
       <c r="O27" s="3">
-        <v>17.818181818181817</v>
+        <v>18.063288159916457</v>
       </c>
       <c r="P27" s="3">
-        <v>18.53409090909091</v>
+        <v>18.750139966736359</v>
       </c>
       <c r="Q27" s="3">
-        <v>19.287878787878789</v>
+        <v>19.457737884375529</v>
       </c>
       <c r="R27" s="3">
-        <v>20.079545454545453</v>
+        <v>20.182298181409408</v>
       </c>
       <c r="S27" s="3">
         <v>20.90909090909091</v>
       </c>
       <c r="T27" s="3">
-        <v>21.13636363636364</v>
+        <v>21.126155776568719</v>
       </c>
       <c r="U27" s="3">
-        <v>21.251779668607256</v>
+        <v>21.235566163609089</v>
       </c>
     </row>
     <row r="28" spans="3:21">
@@ -3018,31 +3021,31 @@
         <v>5.75</v>
       </c>
       <c r="M28" s="3">
-        <v>16.916666666666668</v>
+        <v>17.34208849687576</v>
       </c>
       <c r="N28" s="3">
-        <v>17.565217391304348</v>
+        <v>17.774408469353038</v>
       </c>
       <c r="O28" s="3">
-        <v>18.25</v>
+        <v>18.448199865510009</v>
       </c>
       <c r="P28" s="3">
-        <v>18.971014492753625</v>
+        <v>19.137968083994295</v>
       </c>
       <c r="Q28" s="3">
-        <v>19.728260869565215</v>
+        <v>19.847580408479665</v>
       </c>
       <c r="R28" s="3">
-        <v>20.521739130434781</v>
+        <v>20.573417617603447</v>
       </c>
       <c r="S28" s="3">
         <v>20.826086956521738</v>
       </c>
       <c r="T28" s="3">
-        <v>21.043478260869566</v>
+        <v>21.033714221065733</v>
       </c>
       <c r="U28" s="3">
-        <v>21.153876204754766</v>
+        <v>21.13836763475652</v>
       </c>
     </row>
     <row r="29" spans="3:21">
@@ -3051,31 +3054,31 @@
         <v>6</v>
       </c>
       <c r="M29" s="3">
-        <v>17.333333333333332</v>
+        <v>17.492141449796662</v>
       </c>
       <c r="N29" s="3">
-        <v>17.989583333333332</v>
+        <v>18.155318840987004</v>
       </c>
       <c r="O29" s="3">
-        <v>18.680555555555557</v>
+        <v>18.832449315433298</v>
       </c>
       <c r="P29" s="3">
-        <v>19.406249999999996</v>
+        <v>19.524890911276646</v>
       </c>
       <c r="Q29" s="3">
-        <v>20.166666666666668</v>
+        <v>20.236349775371028</v>
       </c>
       <c r="R29" s="3">
-        <v>20.458333333333332</v>
+        <v>20.507858550203306</v>
       </c>
       <c r="S29" s="3">
         <v>20.75</v>
       </c>
       <c r="T29" s="3">
-        <v>20.958333333333336</v>
+        <v>20.948976128521327</v>
       </c>
       <c r="U29" s="3">
-        <v>21.064131362889984</v>
+        <v>21.049268983308334</v>
       </c>
     </row>
     <row r="30" spans="3:21">
@@ -3084,31 +3087,31 @@
         <v>6.25</v>
       </c>
       <c r="M30" s="3">
-        <v>17.75</v>
+        <v>17.869106087347522</v>
       </c>
       <c r="N30" s="3">
-        <v>18.413333333333334</v>
+        <v>18.535913553894279</v>
       </c>
       <c r="O30" s="3">
-        <v>19.11</v>
+        <v>19.216115980366791</v>
       </c>
       <c r="P30" s="3">
-        <v>19.84</v>
+        <v>19.911017083380472</v>
       </c>
       <c r="Q30" s="3">
-        <v>20.12</v>
+        <v>20.186895784356185</v>
       </c>
       <c r="R30" s="3">
-        <v>20.399999999999999</v>
+        <v>20.447544208195172</v>
       </c>
       <c r="S30" s="3">
         <v>20.68</v>
       </c>
       <c r="T30" s="3">
-        <v>20.88</v>
+        <v>20.871017083380476</v>
       </c>
       <c r="U30" s="3">
-        <v>20.981566108374388</v>
+        <v>20.967298223975998</v>
       </c>
     </row>
     <row r="31" spans="3:21">
@@ -3117,31 +3120,31 @@
         <v>6.5</v>
       </c>
       <c r="M31" s="3">
-        <v>18.166666666666668</v>
+        <v>18.246070724898345</v>
       </c>
       <c r="N31" s="3">
-        <v>18.83653846153846</v>
+        <v>18.91622903023568</v>
       </c>
       <c r="O31" s="3">
-        <v>19.53846153846154</v>
+        <v>19.599267104732391</v>
       </c>
       <c r="P31" s="3">
-        <v>19.807692307692307</v>
+        <v>19.87597796478892</v>
       </c>
       <c r="Q31" s="3">
-        <v>20.076923076923077</v>
+        <v>20.141245946496333</v>
       </c>
       <c r="R31" s="3">
-        <v>20.346153846153847</v>
+        <v>20.391869430956895</v>
       </c>
       <c r="S31" s="3">
         <v>20.615384615384617</v>
       </c>
       <c r="T31" s="3">
-        <v>20.807692307692307</v>
+        <v>20.799054887865843</v>
       </c>
       <c r="U31" s="3">
-        <v>20.905352027283065</v>
+        <v>20.89163290766923</v>
       </c>
     </row>
     <row r="32" spans="3:21">
@@ -3150,31 +3153,31 @@
         <v>6.75</v>
       </c>
       <c r="M32" s="3">
-        <v>18.583333333333332</v>
+        <v>18.623035362449173</v>
       </c>
       <c r="N32" s="3">
-        <v>19.25925925925926</v>
+        <v>19.296296296296298</v>
       </c>
       <c r="O32" s="3">
-        <v>19.518518518518519</v>
+        <v>19.577072026779341</v>
       </c>
       <c r="P32" s="3">
-        <v>19.777777777777779</v>
+        <v>19.843534336463403</v>
       </c>
       <c r="Q32" s="3">
-        <v>20.037037037037038</v>
+        <v>20.098977578107583</v>
       </c>
       <c r="R32" s="3">
-        <v>20.296296296296298</v>
+        <v>20.340318711291825</v>
       </c>
       <c r="S32" s="3">
         <v>20.555555555555557</v>
       </c>
       <c r="T32" s="3">
-        <v>20.74074074074074</v>
+        <v>20.732423225352292</v>
       </c>
       <c r="U32" s="3">
-        <v>20.834783433679988</v>
+        <v>20.821572429607407</v>
       </c>
     </row>
     <row r="33" spans="12:21">
@@ -3186,28 +3189,28 @@
         <v>19</v>
       </c>
       <c r="N33" s="3">
-        <v>19.25</v>
+        <v>19.285714285714285</v>
       </c>
       <c r="O33" s="3">
-        <v>19.5</v>
+        <v>19.556462311537221</v>
       </c>
       <c r="P33" s="3">
-        <v>19.75</v>
+        <v>19.813408110161138</v>
       </c>
       <c r="Q33" s="3">
-        <v>20</v>
+        <v>20.059728378889453</v>
       </c>
       <c r="R33" s="3">
-        <v>20.25</v>
+        <v>20.292450185888548</v>
       </c>
       <c r="S33" s="3">
         <v>20.5</v>
       </c>
       <c r="T33" s="3">
-        <v>20.678571428571427</v>
+        <v>20.670550967303996</v>
       </c>
       <c r="U33" s="3">
-        <v>20.769255453905703</v>
+        <v>20.756516271407143</v>
       </c>
     </row>
     <row r="34" spans="12:21">
@@ -3219,28 +3222,28 @@
         <v>19</v>
       </c>
       <c r="N34" s="3">
-        <v>19.241379310344829</v>
+        <v>19.275862068965516</v>
       </c>
       <c r="O34" s="3">
-        <v>19.482758620689655</v>
+        <v>19.537273955966974</v>
       </c>
       <c r="P34" s="3">
-        <v>19.724137931034484</v>
+        <v>19.78535955463834</v>
       </c>
       <c r="Q34" s="3">
-        <v>19.96551724137931</v>
+        <v>20.023186020996715</v>
       </c>
       <c r="R34" s="3">
-        <v>20.206896551724139</v>
+        <v>20.247882938099288</v>
       </c>
       <c r="S34" s="3">
         <v>20.448275862068964</v>
       </c>
       <c r="T34" s="3">
-        <v>20.620689655172413</v>
+        <v>20.612945761534892</v>
       </c>
       <c r="U34" s="3">
-        <v>20.708246645150332</v>
+        <v>20.695946744806896</v>
       </c>
     </row>
     <row r="35" spans="12:21">
@@ -3252,28 +3255,28 @@
         <v>19</v>
       </c>
       <c r="N35" s="3">
-        <v>19.233333333333334</v>
+        <v>19.266666666666666</v>
       </c>
       <c r="O35" s="3">
-        <v>19.466666666666665</v>
+        <v>19.519364824101405</v>
       </c>
       <c r="P35" s="3">
-        <v>19.7</v>
+        <v>19.759180902817061</v>
       </c>
       <c r="Q35" s="3">
-        <v>19.933333333333334</v>
+        <v>19.989079820296823</v>
       </c>
       <c r="R35" s="3">
-        <v>20.166666666666668</v>
+        <v>20.206286840162644</v>
       </c>
       <c r="S35" s="3">
         <v>20.399999999999999</v>
       </c>
       <c r="T35" s="3">
-        <v>20.566666666666666</v>
+        <v>20.559180902817062</v>
       </c>
       <c r="U35" s="3">
-        <v>20.65130509031199</v>
+        <v>20.639415186646666</v>
       </c>
     </row>
     <row r="36" spans="12:21">
@@ -3285,28 +3288,28 @@
         <v>19</v>
       </c>
       <c r="N36" s="3">
-        <v>19.225806451612904</v>
+        <v>19.258064516129032</v>
       </c>
       <c r="O36" s="3">
-        <v>19.451612903225808</v>
+        <v>19.502611120098134</v>
       </c>
       <c r="P36" s="3">
-        <v>19.677419354838708</v>
+        <v>19.734691196274575</v>
       </c>
       <c r="Q36" s="3">
-        <v>19.903225806451612</v>
+        <v>19.957174019642089</v>
       </c>
       <c r="R36" s="3">
-        <v>20.129032258064516</v>
+        <v>20.16737436144772</v>
       </c>
       <c r="S36" s="3">
         <v>20.35483870967742</v>
       </c>
       <c r="T36" s="3">
-        <v>20.516129032258064</v>
+        <v>20.508884744661675</v>
       </c>
       <c r="U36" s="3">
-        <v>20.598037184172892</v>
+        <v>20.586530825787097</v>
       </c>
     </row>
     <row r="37" spans="12:21">
@@ -3318,28 +3321,28 @@
         <v>19</v>
       </c>
       <c r="N37" s="3">
-        <v>19.21875</v>
+        <v>19.25</v>
       </c>
       <c r="O37" s="3">
-        <v>19.4375</v>
+        <v>19.486904522595069</v>
       </c>
       <c r="P37" s="3">
-        <v>19.65625</v>
+        <v>19.711732096390996</v>
       </c>
       <c r="Q37" s="3">
-        <v>19.875</v>
+        <v>19.927262331528272</v>
       </c>
       <c r="R37" s="3">
-        <v>20.09375</v>
+        <v>20.130893912652478</v>
       </c>
       <c r="S37" s="3">
         <v>20.3125</v>
       </c>
       <c r="T37" s="3">
-        <v>20.46875</v>
+        <v>20.461732096390996</v>
       </c>
       <c r="U37" s="3">
-        <v>20.548098522167489</v>
+        <v>20.53695173748125</v>
       </c>
     </row>
     <row r="38" spans="12:21">
@@ -3351,28 +3354,28 @@
         <v>19</v>
       </c>
       <c r="N38" s="3">
-        <v>19.212121212121211</v>
+        <v>19.242424242424242</v>
       </c>
       <c r="O38" s="3">
-        <v>19.424242424242426</v>
+        <v>19.472149840092186</v>
       </c>
       <c r="P38" s="3">
-        <v>19.636363636363637</v>
+        <v>19.69016445710642</v>
       </c>
       <c r="Q38" s="3">
-        <v>19.848484848484848</v>
+        <v>19.899163472997113</v>
       </c>
       <c r="R38" s="3">
-        <v>20.060606060606062</v>
+        <v>20.096624400147856</v>
       </c>
       <c r="S38" s="3">
         <v>20.272727272727273</v>
       </c>
       <c r="T38" s="3">
-        <v>20.424242424242426</v>
+        <v>20.417437184379146</v>
       </c>
       <c r="U38" s="3">
-        <v>20.501186445738171</v>
+        <v>20.490377442406061</v>
       </c>
     </row>
     <row r="39" spans="12:21">
@@ -3384,28 +3387,28 @@
         <v>19</v>
       </c>
       <c r="N39" s="3">
-        <v>19.205882352941178</v>
+        <v>19.235294117647058</v>
       </c>
       <c r="O39" s="3">
-        <v>19.411764705882351</v>
+        <v>19.458263080089477</v>
       </c>
       <c r="P39" s="3">
-        <v>19.617647058823529</v>
+        <v>19.669865502485642</v>
       </c>
       <c r="Q39" s="3">
-        <v>19.823529411764707</v>
+        <v>19.872717488497198</v>
       </c>
       <c r="R39" s="3">
-        <v>20.029411764705884</v>
+        <v>20.06437074131998</v>
       </c>
       <c r="S39" s="3">
         <v>20.235294117647058</v>
       </c>
       <c r="T39" s="3">
-        <v>20.382352941176471</v>
+        <v>20.37574785542682</v>
       </c>
       <c r="U39" s="3">
-        <v>20.457033903216459</v>
+        <v>20.446542811747058</v>
       </c>
     </row>
     <row r="40" spans="12:21">
@@ -3417,28 +3420,28 @@
         <v>19</v>
       </c>
       <c r="N40" s="3">
-        <v>19.2</v>
+        <v>19.228571428571428</v>
       </c>
       <c r="O40" s="3">
-        <v>19.399999999999999</v>
+        <v>19.445169849229778</v>
       </c>
       <c r="P40" s="3">
-        <v>19.600000000000001</v>
+        <v>19.65072648812891</v>
       </c>
       <c r="Q40" s="3">
-        <v>19.8</v>
+        <v>19.847782703111562</v>
       </c>
       <c r="R40" s="3">
-        <v>20</v>
+        <v>20.033960148710836</v>
       </c>
       <c r="S40" s="3">
         <v>20.2</v>
       </c>
       <c r="T40" s="3">
-        <v>20.342857142857142</v>
+        <v>20.336440773843197</v>
       </c>
       <c r="U40" s="3">
-        <v>20.415404363124562</v>
+        <v>20.405213017125714</v>
       </c>
     </row>
     <row r="41" spans="12:21">
@@ -3450,28 +3453,28 @@
         <v>19</v>
       </c>
       <c r="N41" s="3">
-        <v>19.194444444444443</v>
+        <v>19.222222222222221</v>
       </c>
       <c r="O41" s="3">
-        <v>19.388888888888889</v>
+        <v>19.432804020084504</v>
       </c>
       <c r="P41" s="3">
-        <v>19.583333333333332</v>
+        <v>19.632650752347551</v>
       </c>
       <c r="Q41" s="3">
-        <v>19.777777777777779</v>
+        <v>19.824233183580688</v>
       </c>
       <c r="R41" s="3">
-        <v>19.972222222222221</v>
+        <v>20.005239033468868</v>
       </c>
       <c r="S41" s="3">
         <v>20.166666666666668</v>
       </c>
       <c r="T41" s="3">
-        <v>20.305555555555557</v>
+        <v>20.299317419014219</v>
       </c>
       <c r="U41" s="3">
-        <v>20.376087575259991</v>
+        <v>20.366179322205554</v>
       </c>
     </row>
     <row r="42" spans="12:21">
@@ -3483,28 +3486,28 @@
         <v>19</v>
       </c>
       <c r="N42" s="3">
-        <v>19.189189189189189</v>
+        <v>19.216216216216218</v>
       </c>
       <c r="O42" s="3">
-        <v>19.378378378378379</v>
+        <v>19.421106614136274</v>
       </c>
       <c r="P42" s="3">
-        <v>19.567567567567568</v>
+        <v>19.615552083365184</v>
       </c>
       <c r="Q42" s="3">
-        <v>19.756756756756758</v>
+        <v>19.80195661105148</v>
       </c>
       <c r="R42" s="3">
-        <v>19.945945945945947</v>
+        <v>19.978070410942685</v>
       </c>
       <c r="S42" s="3">
         <v>20.135135135135137</v>
       </c>
       <c r="T42" s="3">
-        <v>20.27027027027027</v>
+        <v>20.264200732013833</v>
       </c>
       <c r="U42" s="3">
-        <v>20.338896019171884</v>
+        <v>20.329255556740542</v>
       </c>
     </row>
     <row r="43" spans="12:21">
@@ -3516,28 +3519,28 @@
         <v>19</v>
       </c>
       <c r="N43" s="3">
-        <v>19.184210526315791</v>
+        <v>19.210526315789473</v>
       </c>
       <c r="O43" s="3">
-        <v>19.368421052631579</v>
+        <v>19.41002486113269</v>
       </c>
       <c r="P43" s="3">
-        <v>19.55263157894737</v>
+        <v>19.599353344329259</v>
       </c>
       <c r="Q43" s="3">
-        <v>19.736842105263158</v>
+        <v>19.780852489708018</v>
       </c>
       <c r="R43" s="3">
-        <v>19.921052631578949</v>
+        <v>19.952331715917875</v>
       </c>
       <c r="S43" s="3">
         <v>20.105263157894736</v>
       </c>
       <c r="T43" s="3">
-        <v>20.236842105263158</v>
+        <v>20.23093229169768</v>
       </c>
       <c r="U43" s="3">
-        <v>20.303661913404202</v>
+        <v>20.294275147352632</v>
       </c>
     </row>
     <row r="44" spans="12:21">
@@ -3549,28 +3552,28 @@
         <v>19</v>
       </c>
       <c r="N44" s="3">
-        <v>19.179487179487179</v>
+        <v>19.205128205128204</v>
       </c>
       <c r="O44" s="3">
-        <v>19.358974358974358</v>
+        <v>19.399511403154929</v>
       </c>
       <c r="P44" s="3">
-        <v>19.53846153846154</v>
+        <v>19.58398530985928</v>
       </c>
       <c r="Q44" s="3">
-        <v>19.717948717948719</v>
+        <v>19.760830630997557</v>
       </c>
       <c r="R44" s="3">
-        <v>19.897435897435898</v>
+        <v>19.927912953971266</v>
       </c>
       <c r="S44" s="3">
         <v>20.076923076923077</v>
       </c>
       <c r="T44" s="3">
-        <v>20.205128205128204</v>
+        <v>20.199369925243893</v>
       </c>
       <c r="U44" s="3">
-        <v>20.270234684855374</v>
+        <v>20.261088605112821</v>
       </c>
     </row>
   </sheetData>

</xml_diff>